<commit_message>
finished CB addr decoding, now to sim config and RSA
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3807AC16-B404-4E6C-A422-1D538F660265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09578229-C099-4BE6-9C52-3BEE52712D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="7" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3111" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="852">
   <si>
     <t>预测</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3451,7 +3451,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4101,6 +4101,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4499,11 +4502,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W1" s="217" t="s">
+      <c r="W1" s="218" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="217"/>
-      <c r="Y1" s="217"/>
+      <c r="X1" s="218"/>
+      <c r="Y1" s="218"/>
       <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
@@ -4518,11 +4521,11 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W3" s="217" t="s">
+      <c r="W3" s="218" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="217"/>
-      <c r="Y3" s="217"/>
+      <c r="X3" s="218"/>
+      <c r="Y3" s="218"/>
       <c r="Z3" s="24" t="s">
         <v>57</v>
       </c>
@@ -5299,30 +5302,30 @@
   <sheetData>
     <row r="1" spans="2:23" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="221" t="s">
+      <c r="C1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="224" t="s">
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="224"/>
+      <c r="G1" s="225" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="222"/>
-      <c r="K1" s="221" t="s">
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="223"/>
+      <c r="K1" s="222" t="s">
         <v>454</v>
       </c>
-      <c r="L1" s="222"/>
-      <c r="M1" s="222"/>
-      <c r="N1" s="223"/>
-      <c r="O1" s="221" t="s">
+      <c r="L1" s="223"/>
+      <c r="M1" s="223"/>
+      <c r="N1" s="224"/>
+      <c r="O1" s="222" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="222"/>
-      <c r="R1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="223"/>
+      <c r="R1" s="224"/>
     </row>
     <row r="2" spans="2:23" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -5379,27 +5382,27 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="225" t="s">
+      <c r="C3" s="226" t="s">
         <v>271</v>
       </c>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="227"/>
-      <c r="G3" s="225"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="227"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227"/>
+      <c r="I3" s="227"/>
+      <c r="J3" s="228"/>
       <c r="K3" s="40"/>
       <c r="O3" s="40"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="225" t="s">
+      <c r="S3" s="226" t="s">
         <v>414</v>
       </c>
-      <c r="T3" s="226"/>
-      <c r="U3" s="226"/>
-      <c r="V3" s="227"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="227"/>
+      <c r="V3" s="228"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -5452,12 +5455,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="218" t="s">
+      <c r="S5" s="219" t="s">
         <v>514</v>
       </c>
-      <c r="T5" s="219"/>
-      <c r="U5" s="219"/>
-      <c r="V5" s="220"/>
+      <c r="T5" s="220"/>
+      <c r="U5" s="220"/>
+      <c r="V5" s="221"/>
       <c r="W5" s="89" t="s">
         <v>516</v>
       </c>
@@ -5483,12 +5486,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="218" t="s">
+      <c r="S6" s="219" t="s">
         <v>431</v>
       </c>
-      <c r="T6" s="219"/>
-      <c r="U6" s="219"/>
-      <c r="V6" s="220"/>
+      <c r="T6" s="220"/>
+      <c r="U6" s="220"/>
+      <c r="V6" s="221"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B7" s="39" t="s">
@@ -6567,30 +6570,30 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="72"/>
-      <c r="C1" s="221" t="s">
+      <c r="C1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="221" t="s">
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="224"/>
+      <c r="G1" s="222" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="223"/>
-      <c r="K1" s="221" t="s">
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="224"/>
+      <c r="K1" s="222" t="s">
         <v>454</v>
       </c>
-      <c r="L1" s="222"/>
-      <c r="M1" s="222"/>
-      <c r="N1" s="223"/>
-      <c r="O1" s="221" t="s">
+      <c r="L1" s="223"/>
+      <c r="M1" s="223"/>
+      <c r="N1" s="224"/>
+      <c r="O1" s="222" t="s">
         <v>189</v>
       </c>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="222"/>
-      <c r="R1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="223"/>
+      <c r="R1" s="224"/>
       <c r="S1" s="48"/>
       <c r="T1" s="48"/>
       <c r="U1" s="48"/>
@@ -6688,12 +6691,12 @@
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="225" t="s">
+      <c r="S3" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="226"/>
-      <c r="U3" s="226"/>
-      <c r="V3" s="227"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="227"/>
+      <c r="V3" s="228"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="72" t="s">
@@ -6758,12 +6761,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="218" t="s">
+      <c r="S5" s="219" t="s">
         <v>288</v>
       </c>
-      <c r="T5" s="219"/>
-      <c r="U5" s="219"/>
-      <c r="V5" s="220"/>
+      <c r="T5" s="220"/>
+      <c r="U5" s="220"/>
+      <c r="V5" s="221"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="72" t="s">
@@ -6793,12 +6796,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="218" t="s">
+      <c r="S6" s="219" t="s">
         <v>289</v>
       </c>
-      <c r="T6" s="219"/>
-      <c r="U6" s="219"/>
-      <c r="V6" s="220"/>
+      <c r="T6" s="220"/>
+      <c r="U6" s="220"/>
+      <c r="V6" s="221"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="72" t="s">
@@ -6865,12 +6868,12 @@
         <v>290</v>
       </c>
       <c r="R8" s="41"/>
-      <c r="S8" s="239" t="s">
+      <c r="S8" s="240" t="s">
         <v>390</v>
       </c>
-      <c r="T8" s="240"/>
-      <c r="U8" s="240"/>
-      <c r="V8" s="240"/>
+      <c r="T8" s="241"/>
+      <c r="U8" s="241"/>
+      <c r="V8" s="241"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="72" t="s">
@@ -9352,30 +9355,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="221" t="s">
+      <c r="B1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="224" t="s">
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="225" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="221" t="s">
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="222" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="222"/>
-      <c r="L1" s="222"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="221" t="s">
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+      <c r="M1" s="224"/>
+      <c r="N1" s="222" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="222"/>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="223"/>
+      <c r="O1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="224"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="35" t="s">
@@ -9461,12 +9464,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="225" t="s">
+      <c r="R3" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="226"/>
-      <c r="T3" s="226"/>
-      <c r="U3" s="227"/>
+      <c r="S3" s="227"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="228"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="71" t="s">
@@ -9528,12 +9531,12 @@
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="41"/>
-      <c r="R5" s="218" t="s">
+      <c r="R5" s="219" t="s">
         <v>288</v>
       </c>
-      <c r="S5" s="219"/>
-      <c r="T5" s="219"/>
-      <c r="U5" s="220"/>
+      <c r="S5" s="220"/>
+      <c r="T5" s="220"/>
+      <c r="U5" s="221"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="71" t="s">
@@ -9562,12 +9565,12 @@
       <c r="O6" s="38"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="41"/>
-      <c r="R6" s="218" t="s">
+      <c r="R6" s="219" t="s">
         <v>289</v>
       </c>
-      <c r="S6" s="219"/>
-      <c r="T6" s="219"/>
-      <c r="U6" s="220"/>
+      <c r="S6" s="220"/>
+      <c r="T6" s="220"/>
+      <c r="U6" s="221"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="71" t="s">
@@ -11104,30 +11107,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="221" t="s">
+      <c r="B1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="224" t="s">
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="225" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="221" t="s">
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="222" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="222"/>
-      <c r="L1" s="222"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="221" t="s">
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+      <c r="M1" s="224"/>
+      <c r="N1" s="222" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="222"/>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="223"/>
+      <c r="O1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="224"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="35" t="s">
@@ -11213,12 +11216,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="225" t="s">
+      <c r="R3" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="226"/>
-      <c r="T3" s="226"/>
-      <c r="U3" s="227"/>
+      <c r="S3" s="227"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="228"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="71" t="s">
@@ -11280,12 +11283,12 @@
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
       <c r="Q5" s="41"/>
-      <c r="R5" s="218" t="s">
+      <c r="R5" s="219" t="s">
         <v>288</v>
       </c>
-      <c r="S5" s="219"/>
-      <c r="T5" s="219"/>
-      <c r="U5" s="220"/>
+      <c r="S5" s="220"/>
+      <c r="T5" s="220"/>
+      <c r="U5" s="221"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="71" t="s">
@@ -11314,12 +11317,12 @@
       <c r="O6" s="38"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="41"/>
-      <c r="R6" s="218" t="s">
+      <c r="R6" s="219" t="s">
         <v>289</v>
       </c>
-      <c r="S6" s="219"/>
-      <c r="T6" s="219"/>
-      <c r="U6" s="220"/>
+      <c r="S6" s="220"/>
+      <c r="T6" s="220"/>
+      <c r="U6" s="221"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="71" t="s">
@@ -12816,30 +12819,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="21"/>
-      <c r="B1" s="221" t="s">
+      <c r="B1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="224" t="s">
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="225" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="221" t="s">
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="222" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="222"/>
-      <c r="L1" s="222"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="221" t="s">
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+      <c r="M1" s="224"/>
+      <c r="N1" s="222" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="222"/>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="223"/>
+      <c r="O1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="224"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
@@ -12926,12 +12929,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="225" t="s">
+      <c r="R3" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="226"/>
-      <c r="T3" s="226"/>
-      <c r="U3" s="227"/>
+      <c r="S3" s="227"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="228"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="39" t="s">
@@ -12984,12 +12987,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="218" t="s">
+      <c r="R5" s="219" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="219"/>
-      <c r="T5" s="219"/>
-      <c r="U5" s="220"/>
+      <c r="S5" s="220"/>
+      <c r="T5" s="220"/>
+      <c r="U5" s="221"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
@@ -13011,12 +13014,12 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="34"/>
-      <c r="R6" s="218" t="s">
+      <c r="R6" s="219" t="s">
         <v>268</v>
       </c>
-      <c r="S6" s="219"/>
-      <c r="T6" s="219"/>
-      <c r="U6" s="220"/>
+      <c r="S6" s="220"/>
+      <c r="T6" s="220"/>
+      <c r="U6" s="221"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="39" t="s">
@@ -14500,7 +14503,7 @@
   <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B58" sqref="B43:B58"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -15310,6 +15313,18 @@
       <c r="E24" s="24" t="s">
         <v>6</v>
       </c>
+      <c r="H24" s="217" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="217" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="217" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" s="217" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A25" s="24">
@@ -15324,6 +15339,9 @@
       </c>
       <c r="E25" s="101" t="s">
         <v>554</v>
+      </c>
+      <c r="H25" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.4">
@@ -16346,67 +16364,67 @@
       </c>
     </row>
     <row r="6" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="228" t="s">
+      <c r="B6" s="229" t="s">
         <v>526</v>
       </c>
-      <c r="C6" s="229"/>
-      <c r="D6" s="230"/>
-      <c r="E6" s="228" t="s">
+      <c r="C6" s="230"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="229" t="s">
         <v>527</v>
       </c>
-      <c r="F6" s="229"/>
-      <c r="G6" s="230"/>
+      <c r="F6" s="230"/>
+      <c r="G6" s="231"/>
     </row>
     <row r="7" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="228" t="s">
+      <c r="B7" s="229" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="229"/>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
-      <c r="G7" s="229"/>
-      <c r="H7" s="229"/>
-      <c r="I7" s="229"/>
-      <c r="J7" s="229"/>
-      <c r="K7" s="229"/>
-      <c r="L7" s="229"/>
-      <c r="M7" s="229"/>
-      <c r="N7" s="229"/>
-      <c r="O7" s="229"/>
-      <c r="P7" s="230"/>
-      <c r="Q7" s="228" t="s">
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
+      <c r="G7" s="230"/>
+      <c r="H7" s="230"/>
+      <c r="I7" s="230"/>
+      <c r="J7" s="230"/>
+      <c r="K7" s="230"/>
+      <c r="L7" s="230"/>
+      <c r="M7" s="230"/>
+      <c r="N7" s="230"/>
+      <c r="O7" s="230"/>
+      <c r="P7" s="231"/>
+      <c r="Q7" s="229" t="s">
         <v>221</v>
       </c>
-      <c r="R7" s="229"/>
-      <c r="S7" s="229"/>
-      <c r="T7" s="229"/>
-      <c r="U7" s="229"/>
-      <c r="V7" s="229"/>
-      <c r="W7" s="229"/>
-      <c r="X7" s="229"/>
-      <c r="Y7" s="229"/>
-      <c r="Z7" s="229"/>
-      <c r="AA7" s="230"/>
-      <c r="AB7" s="228" t="s">
+      <c r="R7" s="230"/>
+      <c r="S7" s="230"/>
+      <c r="T7" s="230"/>
+      <c r="U7" s="230"/>
+      <c r="V7" s="230"/>
+      <c r="W7" s="230"/>
+      <c r="X7" s="230"/>
+      <c r="Y7" s="230"/>
+      <c r="Z7" s="230"/>
+      <c r="AA7" s="231"/>
+      <c r="AB7" s="229" t="s">
         <v>222</v>
       </c>
-      <c r="AC7" s="229"/>
-      <c r="AD7" s="229"/>
-      <c r="AE7" s="229"/>
-      <c r="AF7" s="229"/>
-      <c r="AG7" s="229"/>
-      <c r="AH7" s="229"/>
-      <c r="AI7" s="229"/>
-      <c r="AJ7" s="229"/>
-      <c r="AK7" s="229"/>
-      <c r="AL7" s="229"/>
-      <c r="AM7" s="229"/>
-      <c r="AN7" s="229"/>
-      <c r="AO7" s="229"/>
-      <c r="AP7" s="229"/>
-      <c r="AQ7" s="229"/>
-      <c r="AR7" s="230"/>
+      <c r="AC7" s="230"/>
+      <c r="AD7" s="230"/>
+      <c r="AE7" s="230"/>
+      <c r="AF7" s="230"/>
+      <c r="AG7" s="230"/>
+      <c r="AH7" s="230"/>
+      <c r="AI7" s="230"/>
+      <c r="AJ7" s="230"/>
+      <c r="AK7" s="230"/>
+      <c r="AL7" s="230"/>
+      <c r="AM7" s="230"/>
+      <c r="AN7" s="230"/>
+      <c r="AO7" s="230"/>
+      <c r="AP7" s="230"/>
+      <c r="AQ7" s="230"/>
+      <c r="AR7" s="231"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.4">
       <c r="E9" s="48"/>
@@ -16450,7 +16468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431E16EB-4173-4BB0-A744-4BFFE60D57DA}">
   <dimension ref="A1:AZ82"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A32" sqref="A32"/>
     </sheetView>
@@ -16497,11 +16515,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.4">
-      <c r="C1" s="225" t="s">
+      <c r="C1" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
       <c r="F1" s="67"/>
       <c r="G1" s="63"/>
       <c r="H1" s="97"/>
@@ -16559,12 +16577,12 @@
     </row>
     <row r="5" spans="1:48" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:48" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="221" t="s">
+      <c r="C6" s="222" t="s">
         <v>664</v>
       </c>
-      <c r="D6" s="222"/>
-      <c r="E6" s="222"/>
-      <c r="F6" s="223"/>
+      <c r="D6" s="223"/>
+      <c r="E6" s="223"/>
+      <c r="F6" s="224"/>
       <c r="G6" s="136"/>
       <c r="H6" s="99"/>
       <c r="I6" s="99"/>
@@ -16573,27 +16591,27 @@
       <c r="L6" s="99"/>
       <c r="M6" s="99"/>
       <c r="N6" s="99"/>
-      <c r="O6" s="221" t="s">
+      <c r="O6" s="222" t="s">
         <v>665</v>
       </c>
-      <c r="P6" s="222"/>
-      <c r="Q6" s="222"/>
-      <c r="R6" s="223"/>
-      <c r="AE6" s="221" t="s">
+      <c r="P6" s="223"/>
+      <c r="Q6" s="223"/>
+      <c r="R6" s="224"/>
+      <c r="AE6" s="222" t="s">
         <v>1</v>
       </c>
-      <c r="AF6" s="222"/>
-      <c r="AG6" s="222"/>
-      <c r="AH6" s="223"/>
+      <c r="AF6" s="223"/>
+      <c r="AG6" s="223"/>
+      <c r="AH6" s="224"/>
       <c r="AI6" s="167"/>
-      <c r="AJ6" s="221" t="s">
+      <c r="AJ6" s="222" t="s">
         <v>663</v>
       </c>
-      <c r="AK6" s="222"/>
-      <c r="AL6" s="222"/>
-      <c r="AM6" s="222"/>
-      <c r="AN6" s="222"/>
-      <c r="AO6" s="223"/>
+      <c r="AK6" s="223"/>
+      <c r="AL6" s="223"/>
+      <c r="AM6" s="223"/>
+      <c r="AN6" s="223"/>
+      <c r="AO6" s="224"/>
     </row>
     <row r="7" spans="1:48" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C7" s="35" t="s">
@@ -16671,11 +16689,11 @@
       <c r="I8" s="99"/>
       <c r="J8" s="99"/>
       <c r="K8" s="99"/>
-      <c r="L8" s="232" t="s">
+      <c r="L8" s="233" t="s">
         <v>548</v>
       </c>
-      <c r="M8" s="232"/>
-      <c r="N8" s="232"/>
+      <c r="M8" s="233"/>
+      <c r="N8" s="233"/>
       <c r="O8" s="132"/>
       <c r="P8" s="133"/>
       <c r="Q8" s="133"/>
@@ -16696,12 +16714,12 @@
       <c r="AK8" s="168"/>
       <c r="AL8" s="168"/>
       <c r="AM8" s="168"/>
-      <c r="AP8" s="218" t="s">
+      <c r="AP8" s="219" t="s">
         <v>21</v>
       </c>
-      <c r="AQ8" s="219"/>
-      <c r="AR8" s="219"/>
-      <c r="AS8" s="220"/>
+      <c r="AQ8" s="220"/>
+      <c r="AR8" s="220"/>
+      <c r="AS8" s="221"/>
     </row>
     <row r="9" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C9" s="40"/>
@@ -16713,11 +16731,11 @@
       <c r="I9" s="135"/>
       <c r="J9" s="135"/>
       <c r="K9" s="135"/>
-      <c r="L9" s="234" t="s">
+      <c r="L9" s="235" t="s">
         <v>549</v>
       </c>
-      <c r="M9" s="234"/>
-      <c r="N9" s="233"/>
+      <c r="M9" s="235"/>
+      <c r="N9" s="234"/>
       <c r="O9" s="132"/>
       <c r="P9" s="133"/>
       <c r="Q9" s="133"/>
@@ -16759,9 +16777,9 @@
       <c r="I10" s="135"/>
       <c r="J10" s="135"/>
       <c r="K10" s="135"/>
-      <c r="L10" s="231"/>
-      <c r="M10" s="231"/>
-      <c r="N10" s="231"/>
+      <c r="L10" s="232"/>
+      <c r="M10" s="232"/>
+      <c r="N10" s="232"/>
       <c r="O10" s="132"/>
       <c r="P10" s="133"/>
       <c r="Q10" s="133"/>
@@ -16786,12 +16804,12 @@
       <c r="AK10" s="168"/>
       <c r="AL10" s="168"/>
       <c r="AM10" s="168"/>
-      <c r="AP10" s="218" t="s">
+      <c r="AP10" s="219" t="s">
         <v>56</v>
       </c>
-      <c r="AQ10" s="219"/>
-      <c r="AR10" s="219"/>
-      <c r="AS10" s="220"/>
+      <c r="AQ10" s="220"/>
+      <c r="AR10" s="220"/>
+      <c r="AS10" s="221"/>
     </row>
     <row r="11" spans="1:48" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C11" s="40"/>
@@ -16827,12 +16845,12 @@
       <c r="AK11" s="168"/>
       <c r="AL11" s="168"/>
       <c r="AM11" s="168"/>
-      <c r="AP11" s="218" t="s">
+      <c r="AP11" s="219" t="s">
         <v>662</v>
       </c>
-      <c r="AQ11" s="219"/>
-      <c r="AR11" s="219"/>
-      <c r="AS11" s="220"/>
+      <c r="AQ11" s="220"/>
+      <c r="AR11" s="220"/>
+      <c r="AS11" s="221"/>
       <c r="AT11" s="26" t="s">
         <v>269</v>
       </c>
@@ -16857,11 +16875,11 @@
       <c r="I12" s="99"/>
       <c r="J12" s="99"/>
       <c r="K12" s="99"/>
-      <c r="L12" s="235" t="s">
+      <c r="L12" s="236" t="s">
         <v>547</v>
       </c>
-      <c r="M12" s="235"/>
-      <c r="N12" s="235"/>
+      <c r="M12" s="236"/>
+      <c r="N12" s="236"/>
       <c r="O12" s="132"/>
       <c r="P12" s="133"/>
       <c r="Q12" s="133"/>
@@ -16875,12 +16893,12 @@
       <c r="AK12" s="168"/>
       <c r="AL12" s="168"/>
       <c r="AM12" s="168"/>
-      <c r="AP12" s="218" t="s">
+      <c r="AP12" s="219" t="s">
         <v>546</v>
       </c>
-      <c r="AQ12" s="219"/>
-      <c r="AR12" s="219"/>
-      <c r="AS12" s="220"/>
+      <c r="AQ12" s="220"/>
+      <c r="AR12" s="220"/>
+      <c r="AS12" s="221"/>
       <c r="AU12" s="21" t="s">
         <v>658</v>
       </c>
@@ -16895,12 +16913,12 @@
       <c r="B13" s="145" t="s">
         <v>541</v>
       </c>
-      <c r="C13" s="221" t="s">
+      <c r="C13" s="222" t="s">
         <v>550</v>
       </c>
-      <c r="D13" s="222"/>
-      <c r="E13" s="222"/>
-      <c r="F13" s="222"/>
+      <c r="D13" s="223"/>
+      <c r="E13" s="223"/>
+      <c r="F13" s="223"/>
       <c r="G13" s="181" t="s">
         <v>676</v>
       </c>
@@ -16923,11 +16941,11 @@
       <c r="N13" s="194" t="s">
         <v>680</v>
       </c>
-      <c r="O13" s="221" t="s">
+      <c r="O13" s="222" t="s">
         <v>551</v>
       </c>
-      <c r="P13" s="222"/>
-      <c r="Q13" s="222"/>
+      <c r="P13" s="223"/>
+      <c r="Q13" s="223"/>
       <c r="R13" s="170"/>
       <c r="S13" s="184" t="s">
         <v>717</v>
@@ -16963,18 +16981,18 @@
       <c r="AG13" s="63"/>
       <c r="AH13" s="46"/>
       <c r="AI13" s="167"/>
-      <c r="AJ13" s="218" t="s">
+      <c r="AJ13" s="219" t="s">
         <v>550</v>
       </c>
-      <c r="AK13" s="219"/>
-      <c r="AL13" s="219"/>
-      <c r="AM13" s="219"/>
-      <c r="AP13" s="218" t="s">
+      <c r="AK13" s="220"/>
+      <c r="AL13" s="220"/>
+      <c r="AM13" s="220"/>
+      <c r="AP13" s="219" t="s">
         <v>655</v>
       </c>
-      <c r="AQ13" s="217"/>
-      <c r="AR13" s="217"/>
-      <c r="AS13" s="217"/>
+      <c r="AQ13" s="218"/>
+      <c r="AR13" s="218"/>
+      <c r="AS13" s="218"/>
       <c r="AU13" s="21" t="s">
         <v>659</v>
       </c>
@@ -17651,8 +17669,8 @@
       </c>
       <c r="AN30" s="173"/>
       <c r="AO30" s="175"/>
-      <c r="AQ30" s="233"/>
-      <c r="AR30" s="233"/>
+      <c r="AQ30" s="234"/>
+      <c r="AR30" s="234"/>
     </row>
     <row r="31" spans="1:51" s="26" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="213" t="s">
@@ -18077,8 +18095,8 @@
         <v>90</v>
       </c>
       <c r="AN40" s="173"/>
-      <c r="AQ40" s="231"/>
-      <c r="AR40" s="231"/>
+      <c r="AQ40" s="232"/>
+      <c r="AR40" s="232"/>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A41" s="165" t="s">
@@ -18294,8 +18312,8 @@
         <v>678</v>
       </c>
       <c r="AO46" s="175"/>
-      <c r="AQ46" s="231"/>
-      <c r="AR46" s="231"/>
+      <c r="AQ46" s="232"/>
+      <c r="AR46" s="232"/>
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A47" s="165" t="s">
@@ -18369,12 +18387,12 @@
         <v>346</v>
       </c>
       <c r="B49" s="165"/>
-      <c r="C49" s="221" t="s">
+      <c r="C49" s="222" t="s">
         <v>550</v>
       </c>
-      <c r="D49" s="222"/>
-      <c r="E49" s="222"/>
-      <c r="F49" s="222"/>
+      <c r="D49" s="223"/>
+      <c r="E49" s="223"/>
+      <c r="F49" s="223"/>
       <c r="G49" s="181" t="s">
         <v>676</v>
       </c>
@@ -18397,11 +18415,11 @@
       <c r="N49" s="194" t="s">
         <v>680</v>
       </c>
-      <c r="O49" s="221" t="s">
+      <c r="O49" s="222" t="s">
         <v>551</v>
       </c>
-      <c r="P49" s="222"/>
-      <c r="Q49" s="222"/>
+      <c r="P49" s="223"/>
+      <c r="Q49" s="223"/>
       <c r="R49" s="203"/>
       <c r="S49" s="184" t="s">
         <v>717</v>
@@ -19626,12 +19644,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AQ40:AR40"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="AJ13:AM13"/>
-    <mergeCell ref="AP10:AS10"/>
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AP11:AS11"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="O49:Q49"/>
     <mergeCell ref="AQ46:AR46"/>
@@ -19648,6 +19660,12 @@
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="AP12:AS12"/>
+    <mergeCell ref="AQ40:AR40"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="AJ13:AM13"/>
+    <mergeCell ref="AP10:AS10"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AP11:AS11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19657,10 +19675,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34ECBBF-B660-41D9-BDE6-91AF01412A2C}">
-  <dimension ref="A1:AA46"/>
+  <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -19683,21 +19701,21 @@
     <col min="28" max="16384" width="9.06640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="B1" s="217" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="B1" s="218" t="s">
         <v>741</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
-      <c r="I1" s="217"/>
-      <c r="J1" s="217"/>
-      <c r="K1" s="217"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
@@ -19765,7 +19783,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
       <c r="K3" s="214" t="s">
         <v>543</v>
@@ -19777,7 +19795,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
       <c r="K4" s="214" t="s">
         <v>785</v>
@@ -19793,7 +19811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
       <c r="B5" s="190"/>
       <c r="C5" s="86"/>
@@ -19815,7 +19833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
       <c r="B6" s="190"/>
       <c r="C6" s="86"/>
@@ -19844,7 +19862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
       <c r="B7" s="190"/>
       <c r="C7" s="83" t="s">
@@ -19875,7 +19893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
       <c r="B8" s="83" t="s">
         <v>750</v>
@@ -19904,7 +19922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
       <c r="B9" s="83" t="s">
         <v>754</v>
@@ -19930,7 +19948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="83" t="s">
         <v>757</v>
@@ -19960,8 +19978,11 @@
       <c r="AA10" s="215">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB10" s="217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="190"/>
       <c r="C11" s="86"/>
@@ -19988,8 +20009,11 @@
       <c r="AA11" s="215">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB11" s="217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
       <c r="B12" s="190"/>
       <c r="C12" s="86"/>
@@ -20032,8 +20056,11 @@
       <c r="AA12" s="215">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB12" s="217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
       <c r="B13" s="190"/>
       <c r="C13" s="83" t="s">
@@ -20080,8 +20107,11 @@
       <c r="AA13" s="215">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB13" s="217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
       <c r="B14" s="83" t="s">
         <v>767</v>
@@ -20127,8 +20157,11 @@
       <c r="AA14" s="215">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB14" s="217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A15" s="21"/>
       <c r="B15" s="83" t="s">
         <v>770</v>
@@ -20173,8 +20206,11 @@
       <c r="AA15" s="215">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB15" s="217">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A16" s="21"/>
       <c r="B16" s="83" t="s">
         <v>772</v>
@@ -20216,8 +20252,11 @@
       <c r="AA16" s="215">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB16" s="217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
       <c r="B17" s="26"/>
       <c r="C17" s="86"/>
@@ -20257,8 +20296,11 @@
       <c r="AA17" s="215">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB17" s="217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
       <c r="B18" s="190"/>
       <c r="C18" s="86"/>
@@ -20297,8 +20339,11 @@
       <c r="AA18" s="215">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB18" s="217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
       <c r="B19" s="190"/>
       <c r="C19" s="83" t="s">
@@ -20342,8 +20387,11 @@
       <c r="AA19" s="215">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB19" s="217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A20" s="21"/>
       <c r="B20" s="83" t="s">
         <v>774</v>
@@ -20386,8 +20434,11 @@
       <c r="AA20" s="215">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB20" s="217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A21" s="21"/>
       <c r="B21" s="83" t="s">
         <v>776</v>
@@ -20430,8 +20481,11 @@
       <c r="AA21" s="215">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB21" s="217">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A22" s="21"/>
       <c r="B22" s="83" t="s">
         <v>778</v>
@@ -20469,8 +20523,11 @@
       <c r="AA22" s="215">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB22" s="217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A23" s="21"/>
       <c r="M23" s="212">
         <v>2</v>
@@ -20492,8 +20549,11 @@
       <c r="AA23" s="215">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB23" s="217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A24" s="21"/>
       <c r="M24" s="212">
         <v>3</v>
@@ -20510,8 +20570,11 @@
       <c r="AA24" s="215">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB24" s="217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A25" s="21"/>
       <c r="M25" s="212">
         <v>4</v>
@@ -20528,8 +20591,11 @@
       <c r="AA25" s="215">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB25" s="217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A26" s="21"/>
       <c r="M26" s="212">
         <v>5</v>
@@ -20546,8 +20612,11 @@
       <c r="AA26" s="215">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB26" s="217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A27" s="21"/>
       <c r="M27" s="212">
         <v>6</v>
@@ -20564,8 +20633,11 @@
       <c r="AA27" s="215">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="AB27" s="217">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A28" s="21"/>
       <c r="K28" s="212" t="s">
         <v>840</v>
@@ -20589,7 +20661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A29" s="21"/>
       <c r="M29" s="212">
         <v>2</v>
@@ -20607,7 +20679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A30" s="21"/>
       <c r="M30" s="212">
         <v>3</v>
@@ -20625,7 +20697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A31" s="21"/>
       <c r="M31" s="212">
         <v>4</v>
@@ -20643,7 +20715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A32" s="21"/>
       <c r="M32" s="212">
         <v>5</v>
@@ -20806,30 +20878,30 @@
   <sheetData>
     <row r="1" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="21"/>
-      <c r="B1" s="221" t="s">
+      <c r="B1" s="222" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="224" t="s">
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="225" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="221" t="s">
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="222" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="222"/>
-      <c r="L1" s="222"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="221" t="s">
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+      <c r="M1" s="224"/>
+      <c r="N1" s="222" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="222"/>
-      <c r="P1" s="222"/>
-      <c r="Q1" s="223"/>
+      <c r="O1" s="223"/>
+      <c r="P1" s="223"/>
+      <c r="Q1" s="224"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
@@ -20938,11 +21010,11 @@
       <c r="O3" s="43"/>
       <c r="P3" s="43"/>
       <c r="Q3" s="44"/>
-      <c r="R3" s="225" t="s">
+      <c r="R3" s="226" t="s">
         <v>264</v>
       </c>
-      <c r="S3" s="226"/>
-      <c r="T3" s="226"/>
+      <c r="S3" s="227"/>
+      <c r="T3" s="227"/>
       <c r="U3" s="45"/>
       <c r="W3" t="s">
         <v>676</v>
@@ -21116,12 +21188,12 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="34"/>
-      <c r="R6" s="236" t="s">
+      <c r="R6" s="237" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="237"/>
-      <c r="T6" s="237"/>
-      <c r="U6" s="238"/>
+      <c r="S6" s="238"/>
+      <c r="T6" s="238"/>
+      <c r="U6" s="239"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="39" t="s">
@@ -21147,12 +21219,12 @@
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="34"/>
-      <c r="R7" s="218" t="s">
+      <c r="R7" s="219" t="s">
         <v>617</v>
       </c>
-      <c r="S7" s="217"/>
-      <c r="T7" s="217"/>
-      <c r="U7" s="217"/>
+      <c r="S7" s="218"/>
+      <c r="T7" s="218"/>
+      <c r="U7" s="218"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A8" s="39" t="s">
@@ -21173,12 +21245,12 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="34"/>
-      <c r="R8" s="218" t="s">
+      <c r="R8" s="219" t="s">
         <v>616</v>
       </c>
-      <c r="S8" s="217"/>
-      <c r="T8" s="217"/>
-      <c r="U8" s="217"/>
+      <c r="S8" s="218"/>
+      <c r="T8" s="218"/>
+      <c r="U8" s="218"/>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A9" s="39" t="s">
@@ -21196,12 +21268,12 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
       <c r="Q9" s="34"/>
-      <c r="R9" s="218" t="s">
+      <c r="R9" s="219" t="s">
         <v>545</v>
       </c>
-      <c r="S9" s="219"/>
-      <c r="T9" s="219"/>
-      <c r="U9" s="220"/>
+      <c r="S9" s="220"/>
+      <c r="T9" s="220"/>
+      <c r="U9" s="221"/>
     </row>
     <row r="10" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="39" t="s">

</xml_diff>

<commit_message>
220424-v1 add some note to data stream
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CEAC6E-BBDB-4BCA-AA98-BB1B4F765605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54985C91-64A6-4784-8298-9792FC4B78A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="5" activeTab="12" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="5" activeTab="10" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD1,2" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4376" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4383" uniqueCount="960">
   <si>
     <t>预测</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3361,6 +3361,34 @@
   </si>
   <si>
     <t>输入到输出间隔=N+2+2=6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change C0 to TB_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHANGE C0 to TB3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cov_HT(7)还是在C0产生，只是映射存储到TB3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所以M的输入顺序不用变</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode&lt;=2'b00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode&lt;=2'b10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只改变PE_mode, 数据映射关系不变</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3792,7 +3820,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="297">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4588,6 +4616,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4666,22 +4712,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5008,11 +5045,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W1" s="265" t="s">
+      <c r="W1" s="271" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="265"/>
-      <c r="Y1" s="265"/>
+      <c r="X1" s="271"/>
+      <c r="Y1" s="271"/>
       <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
@@ -5027,11 +5064,11 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W3" s="265" t="s">
+      <c r="W3" s="271" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="265"/>
-      <c r="Y3" s="265"/>
+      <c r="X3" s="271"/>
+      <c r="Y3" s="271"/>
       <c r="Z3" s="24" t="s">
         <v>55</v>
       </c>
@@ -5809,57 +5846,57 @@
       <c r="A1" s="223" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="269" t="s">
+      <c r="B1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="272" t="s">
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="270"/>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="269" t="s">
+      <c r="G1" s="276"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="275" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="270"/>
-      <c r="L1" s="270"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="269" t="s">
+      <c r="K1" s="276"/>
+      <c r="L1" s="276"/>
+      <c r="M1" s="277"/>
+      <c r="N1" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="273" t="s">
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="277"/>
+      <c r="R1" s="279" t="s">
         <v>262</v>
       </c>
-      <c r="S1" s="274"/>
-      <c r="T1" s="274"/>
+      <c r="S1" s="280"/>
+      <c r="T1" s="280"/>
       <c r="U1" s="42"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="223"/>
-      <c r="B2" s="269" t="s">
+      <c r="B2" s="275" t="s">
         <v>623</v>
       </c>
-      <c r="C2" s="270"/>
-      <c r="D2" s="270"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="269" t="s">
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="277"/>
+      <c r="F2" s="275" t="s">
         <v>624</v>
       </c>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="269" t="s">
+      <c r="G2" s="276"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="277"/>
+      <c r="J2" s="275" t="s">
         <v>795</v>
       </c>
-      <c r="K2" s="270"/>
-      <c r="L2" s="270"/>
-      <c r="M2" s="271"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="277"/>
       <c r="N2" s="44"/>
       <c r="O2" s="227"/>
       <c r="P2" s="227"/>
@@ -5958,12 +5995,12 @@
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="34"/>
-      <c r="R4" s="284" t="s">
+      <c r="R4" s="290" t="s">
         <v>286</v>
       </c>
-      <c r="S4" s="285"/>
-      <c r="T4" s="285"/>
-      <c r="U4" s="286"/>
+      <c r="S4" s="291"/>
+      <c r="T4" s="291"/>
+      <c r="U4" s="292"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="223" t="s">
@@ -5986,12 +6023,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="266" t="s">
+      <c r="R5" s="272" t="s">
         <v>873</v>
       </c>
-      <c r="S5" s="267"/>
-      <c r="T5" s="267"/>
-      <c r="U5" s="268"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="274"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="223" t="s">
@@ -7661,11 +7698,11 @@
       <c r="K93" s="221"/>
       <c r="L93" s="231"/>
       <c r="M93" s="231"/>
-      <c r="R93" s="273" t="s">
+      <c r="R93" s="279" t="s">
         <v>262</v>
       </c>
-      <c r="S93" s="274"/>
-      <c r="T93" s="274"/>
+      <c r="S93" s="280"/>
+      <c r="T93" s="280"/>
       <c r="U93" s="42"/>
     </row>
     <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -7754,12 +7791,12 @@
       <c r="K96" s="82"/>
       <c r="L96" s="82"/>
       <c r="M96" s="83"/>
-      <c r="R96" s="284" t="s">
+      <c r="R96" s="290" t="s">
         <v>54</v>
       </c>
-      <c r="S96" s="287"/>
-      <c r="T96" s="287"/>
-      <c r="U96" s="288"/>
+      <c r="S96" s="293"/>
+      <c r="T96" s="293"/>
+      <c r="U96" s="294"/>
     </row>
     <row r="97" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="223" t="s">
@@ -7781,12 +7818,12 @@
       <c r="K97" s="82"/>
       <c r="L97" s="82"/>
       <c r="M97" s="83"/>
-      <c r="R97" s="273" t="s">
+      <c r="R97" s="279" t="s">
         <v>873</v>
       </c>
-      <c r="S97" s="274"/>
-      <c r="T97" s="274"/>
-      <c r="U97" s="275"/>
+      <c r="S97" s="280"/>
+      <c r="T97" s="280"/>
+      <c r="U97" s="281"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A98" s="223" t="s">
@@ -7838,11 +7875,11 @@
       <c r="K100" s="82"/>
       <c r="L100" s="82"/>
       <c r="M100" s="83"/>
-      <c r="R100" s="273" t="s">
+      <c r="R100" s="279" t="s">
         <v>874</v>
       </c>
-      <c r="S100" s="274"/>
-      <c r="T100" s="274"/>
+      <c r="S100" s="280"/>
+      <c r="T100" s="280"/>
       <c r="U100" s="42"/>
     </row>
     <row r="101" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -7938,12 +7975,12 @@
       <c r="M103" s="34" t="s">
         <v>476</v>
       </c>
-      <c r="R103" s="284" t="s">
+      <c r="R103" s="290" t="s">
         <v>286</v>
       </c>
-      <c r="S103" s="287"/>
-      <c r="T103" s="287"/>
-      <c r="U103" s="288"/>
+      <c r="S103" s="293"/>
+      <c r="T103" s="293"/>
+      <c r="U103" s="294"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A104" s="223" t="s">
@@ -7960,12 +7997,12 @@
       <c r="L104" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="R104" s="273" t="s">
+      <c r="R104" s="279" t="s">
         <v>873</v>
       </c>
-      <c r="S104" s="274"/>
-      <c r="T104" s="274"/>
-      <c r="U104" s="275"/>
+      <c r="S104" s="280"/>
+      <c r="T104" s="280"/>
+      <c r="U104" s="281"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A105" s="223" t="s">
@@ -8315,12 +8352,12 @@
       <c r="L124" s="34" t="s">
         <v>772</v>
       </c>
-      <c r="R124" s="273" t="s">
+      <c r="R124" s="279" t="s">
         <v>885</v>
       </c>
-      <c r="S124" s="274"/>
-      <c r="T124" s="274"/>
-      <c r="U124" s="275"/>
+      <c r="S124" s="280"/>
+      <c r="T124" s="280"/>
+      <c r="U124" s="281"/>
     </row>
     <row r="125" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="223" t="s">
@@ -8396,23 +8433,23 @@
       <c r="G127" s="76" t="s">
         <v>582</v>
       </c>
-      <c r="R127" s="284" t="s">
+      <c r="R127" s="290" t="s">
         <v>877</v>
       </c>
-      <c r="S127" s="287"/>
-      <c r="T127" s="287"/>
-      <c r="U127" s="288"/>
+      <c r="S127" s="293"/>
+      <c r="T127" s="293"/>
+      <c r="U127" s="294"/>
     </row>
     <row r="128" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="223" t="s">
         <v>886</v>
       </c>
-      <c r="R128" s="269" t="s">
+      <c r="R128" s="275" t="s">
         <v>873</v>
       </c>
-      <c r="S128" s="270"/>
-      <c r="T128" s="270"/>
-      <c r="U128" s="271"/>
+      <c r="S128" s="276"/>
+      <c r="T128" s="276"/>
+      <c r="U128" s="277"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A129" s="223" t="s">
@@ -8467,12 +8504,12 @@
       <c r="F135" s="81" t="s">
         <v>854</v>
       </c>
-      <c r="R135" s="273" t="s">
+      <c r="R135" s="279" t="s">
         <v>905</v>
       </c>
-      <c r="S135" s="274"/>
-      <c r="T135" s="274"/>
-      <c r="U135" s="275"/>
+      <c r="S135" s="280"/>
+      <c r="T135" s="280"/>
+      <c r="U135" s="281"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A136" s="223" t="s">
@@ -8524,23 +8561,23 @@
       <c r="A138" s="223" t="s">
         <v>862</v>
       </c>
-      <c r="R138" s="284" t="s">
+      <c r="R138" s="290" t="s">
         <v>877</v>
       </c>
-      <c r="S138" s="287"/>
-      <c r="T138" s="287"/>
-      <c r="U138" s="288"/>
+      <c r="S138" s="293"/>
+      <c r="T138" s="293"/>
+      <c r="U138" s="294"/>
     </row>
     <row r="139" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="223" t="s">
         <v>863</v>
       </c>
-      <c r="R139" s="269" t="s">
+      <c r="R139" s="275" t="s">
         <v>916</v>
       </c>
-      <c r="S139" s="270"/>
-      <c r="T139" s="270"/>
-      <c r="U139" s="271"/>
+      <c r="S139" s="276"/>
+      <c r="T139" s="276"/>
+      <c r="U139" s="277"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A140" s="223" t="s">
@@ -8589,12 +8626,12 @@
       <c r="F145" s="77" t="s">
         <v>847</v>
       </c>
-      <c r="R145" s="273" t="s">
+      <c r="R145" s="279" t="s">
         <v>915</v>
       </c>
-      <c r="S145" s="274"/>
-      <c r="T145" s="274"/>
-      <c r="U145" s="275"/>
+      <c r="S145" s="280"/>
+      <c r="T145" s="280"/>
+      <c r="U145" s="281"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A146" s="223" t="s">
@@ -8646,12 +8683,12 @@
       <c r="A148" s="223" t="s">
         <v>887</v>
       </c>
-      <c r="R148" s="284" t="s">
+      <c r="R148" s="290" t="s">
         <v>877</v>
       </c>
-      <c r="S148" s="287"/>
-      <c r="T148" s="287"/>
-      <c r="U148" s="288"/>
+      <c r="S148" s="293"/>
+      <c r="T148" s="293"/>
+      <c r="U148" s="294"/>
     </row>
     <row r="149" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="223" t="s">
@@ -8661,12 +8698,12 @@
       <c r="Q149" s="77" t="s">
         <v>878</v>
       </c>
-      <c r="R149" s="269" t="s">
+      <c r="R149" s="275" t="s">
         <v>916</v>
       </c>
-      <c r="S149" s="270"/>
-      <c r="T149" s="270"/>
-      <c r="U149" s="271"/>
+      <c r="S149" s="276"/>
+      <c r="T149" s="276"/>
+      <c r="U149" s="277"/>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A150" s="223" t="s">
@@ -8775,6 +8812,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R138:U138"/>
+    <mergeCell ref="R139:U139"/>
+    <mergeCell ref="R148:U148"/>
+    <mergeCell ref="R149:U149"/>
+    <mergeCell ref="R135:U135"/>
+    <mergeCell ref="R145:U145"/>
+    <mergeCell ref="R128:U128"/>
+    <mergeCell ref="R93:T93"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="R97:U97"/>
+    <mergeCell ref="R100:T100"/>
+    <mergeCell ref="R103:U103"/>
+    <mergeCell ref="R104:U104"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="R127:U127"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="B1:E1"/>
@@ -8785,21 +8837,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="R128:U128"/>
-    <mergeCell ref="R93:T93"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="R97:U97"/>
-    <mergeCell ref="R100:T100"/>
-    <mergeCell ref="R103:U103"/>
-    <mergeCell ref="R104:U104"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="R127:U127"/>
-    <mergeCell ref="R138:U138"/>
-    <mergeCell ref="R139:U139"/>
-    <mergeCell ref="R148:U148"/>
-    <mergeCell ref="R149:U149"/>
-    <mergeCell ref="R135:U135"/>
-    <mergeCell ref="R145:U145"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8810,9 +8847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6F30D8-4F74-43CF-B0A2-082294AF7E0E}">
   <dimension ref="A1:AC51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H46" sqref="H46"/>
+      <selection pane="topRight" activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -8836,36 +8873,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="269" t="s">
+      <c r="C1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="272" t="s">
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="270"/>
-      <c r="K1" s="269" t="s">
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="276"/>
+      <c r="K1" s="275" t="s">
         <v>446</v>
       </c>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="269" t="s">
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="271"/>
-      <c r="Z1" s="269" t="s">
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="277"/>
+      <c r="Z1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="270"/>
-      <c r="AB1" s="270"/>
-      <c r="AC1" s="271"/>
+      <c r="AA1" s="276"/>
+      <c r="AB1" s="276"/>
+      <c r="AC1" s="277"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -8934,33 +8971,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="273" t="s">
+      <c r="C3" s="279" t="s">
         <v>269</v>
       </c>
-      <c r="D3" s="274"/>
-      <c r="E3" s="274"/>
-      <c r="F3" s="275"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="274"/>
-      <c r="I3" s="274"/>
-      <c r="J3" s="275"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="281"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
+      <c r="I3" s="280"/>
+      <c r="J3" s="281"/>
       <c r="K3" s="40"/>
       <c r="O3" s="40"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="273" t="s">
+      <c r="S3" s="279" t="s">
         <v>406</v>
       </c>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="275"/>
-      <c r="Z3" s="273" t="s">
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="281"/>
+      <c r="Z3" s="279" t="s">
         <v>269</v>
       </c>
-      <c r="AA3" s="274"/>
-      <c r="AB3" s="274"/>
-      <c r="AC3" s="275"/>
+      <c r="AA3" s="280"/>
+      <c r="AB3" s="280"/>
+      <c r="AC3" s="281"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -9017,12 +9054,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="266" t="s">
+      <c r="S5" s="272" t="s">
         <v>506</v>
       </c>
-      <c r="T5" s="267"/>
-      <c r="U5" s="267"/>
-      <c r="V5" s="268"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="274"/>
       <c r="W5" s="85" t="s">
         <v>508</v>
       </c>
@@ -9052,12 +9089,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="266" t="s">
+      <c r="S6" s="272" t="s">
         <v>945</v>
       </c>
-      <c r="T6" s="267"/>
-      <c r="U6" s="267"/>
-      <c r="V6" s="268"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="273"/>
+      <c r="V6" s="274"/>
       <c r="Z6" s="224"/>
       <c r="AA6" s="225"/>
       <c r="AB6" s="225"/>
@@ -9538,6 +9575,13 @@
       </c>
       <c r="N22" s="82"/>
       <c r="O22" s="33"/>
+      <c r="S22" s="295" t="s">
+        <v>955</v>
+      </c>
+      <c r="T22" s="299"/>
+      <c r="U22" s="299"/>
+      <c r="V22" s="299"/>
+      <c r="W22" s="299"/>
       <c r="Z22" s="80" t="s">
         <v>247</v>
       </c>
@@ -9584,6 +9628,12 @@
       <c r="O23" s="77" t="s">
         <v>430</v>
       </c>
+      <c r="S23" s="295" t="s">
+        <v>956</v>
+      </c>
+      <c r="T23" s="296"/>
+      <c r="U23" s="296"/>
+      <c r="V23" s="296"/>
       <c r="Z23" s="80" t="s">
         <v>249</v>
       </c>
@@ -9648,6 +9698,10 @@
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="34"/>
       <c r="O25" s="33"/>
       <c r="P25" s="75" t="s">
         <v>427</v>
@@ -9687,6 +9741,12 @@
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
+      <c r="K26" s="272" t="s">
+        <v>954</v>
+      </c>
+      <c r="L26" s="273"/>
+      <c r="M26" s="273"/>
+      <c r="N26" s="274"/>
       <c r="Q26" s="77" t="s">
         <v>429</v>
       </c>
@@ -9723,7 +9783,7 @@
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="77" t="s">
+      <c r="N27" s="77" t="s">
         <v>390</v>
       </c>
       <c r="R27" s="75" t="s">
@@ -9760,11 +9820,11 @@
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
-      <c r="K28" s="77" t="s">
+      <c r="M28" s="77" t="s">
+        <v>388</v>
+      </c>
+      <c r="N28" s="77" t="s">
         <v>391</v>
-      </c>
-      <c r="L28" s="77" t="s">
-        <v>388</v>
       </c>
       <c r="Z28" s="80" t="s">
         <v>256</v>
@@ -9804,10 +9864,10 @@
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
       <c r="L29" s="77" t="s">
+        <v>386</v>
+      </c>
+      <c r="M29" s="77" t="s">
         <v>389</v>
-      </c>
-      <c r="M29" s="77" t="s">
-        <v>386</v>
       </c>
       <c r="Z29" s="80" t="s">
         <v>259</v>
@@ -9842,12 +9902,11 @@
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="77" t="s">
+      <c r="K30" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="L30" s="77" t="s">
         <v>387</v>
-      </c>
-      <c r="N30" s="77" t="s">
-        <v>384</v>
       </c>
       <c r="O30" s="77" t="s">
         <v>438</v>
@@ -9881,12 +9940,10 @@
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="26"/>
+      <c r="K31" s="77" t="s">
+        <v>385</v>
+      </c>
       <c r="M31" s="26"/>
-      <c r="N31" s="77" t="s">
-        <v>385</v>
-      </c>
       <c r="O31" s="77" t="s">
         <v>439</v>
       </c>
@@ -10408,7 +10465,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="S23:V23"/>
+    <mergeCell ref="S22:W22"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="S6:V6"/>
@@ -10431,7 +10491,7 @@
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="O15" sqref="O15:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -10454,30 +10514,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="69"/>
       <c r="B1"/>
-      <c r="C1" s="269" t="s">
+      <c r="C1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="269" t="s">
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="275" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="269" t="s">
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="275" t="s">
         <v>446</v>
       </c>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="269" t="s">
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="271"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="277"/>
     </row>
     <row r="2" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="69"/>
@@ -10568,12 +10628,12 @@
       <c r="P3" s="260"/>
       <c r="Q3" s="260"/>
       <c r="R3" s="162"/>
-      <c r="S3" s="273" t="s">
+      <c r="S3" s="279" t="s">
         <v>951</v>
       </c>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="275"/>
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="281"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="69" t="s">
@@ -10640,12 +10700,12 @@
       <c r="P5" s="260"/>
       <c r="Q5" s="260"/>
       <c r="R5" s="162"/>
-      <c r="S5" s="266" t="s">
+      <c r="S5" s="272" t="s">
         <v>877</v>
       </c>
-      <c r="T5" s="267"/>
-      <c r="U5" s="267"/>
-      <c r="V5" s="268"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="274"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="69" t="s">
@@ -10674,12 +10734,12 @@
       <c r="P6" s="260"/>
       <c r="Q6" s="260"/>
       <c r="R6" s="162"/>
-      <c r="S6" s="266" t="s">
+      <c r="S6" s="272" t="s">
         <v>952</v>
       </c>
-      <c r="T6" s="267"/>
-      <c r="U6" s="267"/>
-      <c r="V6" s="268"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="273"/>
+      <c r="V6" s="274"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="69" t="s">
@@ -10736,10 +10796,10 @@
       <c r="P8" s="260"/>
       <c r="Q8" s="162"/>
       <c r="R8" s="162"/>
-      <c r="S8" s="289"/>
-      <c r="T8" s="290"/>
-      <c r="U8" s="290"/>
-      <c r="V8" s="290"/>
+      <c r="S8" s="295"/>
+      <c r="T8" s="296"/>
+      <c r="U8" s="296"/>
+      <c r="V8" s="296"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="69" t="s">
@@ -10927,10 +10987,12 @@
       <c r="N15" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="O15" s="165"/>
-      <c r="P15" s="162"/>
-      <c r="Q15" s="162"/>
-      <c r="R15" s="162"/>
+      <c r="O15" s="297" t="s">
+        <v>953</v>
+      </c>
+      <c r="P15" s="285"/>
+      <c r="Q15" s="285"/>
+      <c r="R15" s="298"/>
     </row>
     <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="69" t="s">
@@ -11180,11 +11242,11 @@
       <c r="J25" s="259"/>
       <c r="K25" s="165"/>
       <c r="L25" s="162"/>
-      <c r="M25" s="295"/>
+      <c r="M25" s="269"/>
       <c r="N25" s="162"/>
       <c r="O25" s="165"/>
       <c r="P25" s="162"/>
-      <c r="Q25" s="295"/>
+      <c r="Q25" s="269"/>
       <c r="R25" s="162"/>
     </row>
     <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.4">
@@ -11202,8 +11264,8 @@
       <c r="M26" s="259"/>
       <c r="N26" s="100"/>
       <c r="O26" s="165"/>
-      <c r="P26" s="295"/>
-      <c r="Q26" s="295"/>
+      <c r="P26" s="269"/>
+      <c r="Q26" s="269"/>
       <c r="R26" s="162"/>
     </row>
     <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.4">
@@ -11219,8 +11281,8 @@
       <c r="I27" s="32"/>
       <c r="J27" s="67"/>
       <c r="N27" s="100"/>
-      <c r="O27" s="296"/>
-      <c r="P27" s="295"/>
+      <c r="O27" s="270"/>
+      <c r="P27" s="269"/>
       <c r="Q27" s="162"/>
       <c r="R27" s="162"/>
     </row>
@@ -11366,7 +11428,7 @@
       <c r="I34" s="32"/>
       <c r="J34" s="259"/>
       <c r="K34" s="165"/>
-      <c r="L34" s="295"/>
+      <c r="L34" s="269"/>
       <c r="M34" s="162"/>
       <c r="N34" s="111"/>
       <c r="O34" s="263"/>
@@ -11385,7 +11447,7 @@
       <c r="H35" s="258"/>
       <c r="I35" s="258"/>
       <c r="J35" s="259"/>
-      <c r="K35" s="296"/>
+      <c r="K35" s="270"/>
       <c r="L35" s="162"/>
       <c r="M35" s="12"/>
       <c r="N35" s="162"/>
@@ -12431,7 +12493,8 @@
       <c r="R89" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="O15:R15"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="S8:V8"/>
     <mergeCell ref="C1:F1"/>
@@ -12450,16 +12513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D08606B-AA92-41E2-AB37-358CADF18961}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="G38" sqref="G38:J42"/>
+      <selection pane="topRight" activeCell="S8" sqref="S8:V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.06640625" style="68"/>
-    <col min="2" max="2" width="9.06640625" style="66"/>
+    <col min="2" max="2" width="13.6640625" style="66" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.06640625" style="32"/>
     <col min="5" max="5" width="9.06640625" style="67"/>
     <col min="6" max="6" width="11.3984375" style="45" bestFit="1" customWidth="1"/>
@@ -12477,30 +12540,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="69"/>
       <c r="B1"/>
-      <c r="C1" s="269" t="s">
+      <c r="C1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="269" t="s">
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="275" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="269" t="s">
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="275" t="s">
         <v>446</v>
       </c>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="269" t="s">
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="271"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="277"/>
       <c r="S1" s="230"/>
       <c r="T1" s="230"/>
       <c r="U1" s="230"/>
@@ -12566,7 +12629,9 @@
       <c r="A3" s="69">
         <v>0</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="s">
+        <v>958</v>
+      </c>
       <c r="C3" s="224" t="s">
         <v>137</v>
       </c>
@@ -12597,12 +12662,12 @@
       <c r="P3" s="225"/>
       <c r="Q3" s="225"/>
       <c r="R3" s="226"/>
-      <c r="S3" s="273" t="s">
+      <c r="S3" s="279" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="275"/>
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="281"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="69" t="s">
@@ -12669,12 +12734,12 @@
       <c r="P5" s="225"/>
       <c r="Q5" s="225"/>
       <c r="R5" s="226"/>
-      <c r="S5" s="266" t="s">
+      <c r="S5" s="272" t="s">
         <v>286</v>
       </c>
-      <c r="T5" s="267"/>
-      <c r="U5" s="267"/>
-      <c r="V5" s="268"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="274"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="69" t="s">
@@ -12705,12 +12770,12 @@
       <c r="P6" s="225"/>
       <c r="Q6" s="225"/>
       <c r="R6" s="226"/>
-      <c r="S6" s="266" t="s">
+      <c r="S6" s="272" t="s">
         <v>287</v>
       </c>
-      <c r="T6" s="267"/>
-      <c r="U6" s="267"/>
-      <c r="V6" s="268"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="273"/>
+      <c r="V6" s="274"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="69" t="s">
@@ -12778,18 +12843,20 @@
         <v>288</v>
       </c>
       <c r="R8" s="226"/>
-      <c r="S8" s="289" t="s">
-        <v>382</v>
-      </c>
-      <c r="T8" s="290"/>
-      <c r="U8" s="290"/>
-      <c r="V8" s="290"/>
+      <c r="S8" s="295" t="s">
+        <v>959</v>
+      </c>
+      <c r="T8" s="296"/>
+      <c r="U8" s="296"/>
+      <c r="V8" s="296"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9"/>
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>957</v>
+      </c>
       <c r="C9" s="226" t="s">
         <v>295</v>
       </c>
@@ -13281,7 +13348,9 @@
       <c r="A22" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" t="s">
+        <v>958</v>
+      </c>
       <c r="C22" s="224"/>
       <c r="D22" s="225"/>
       <c r="E22" s="225"/>
@@ -15087,7 +15156,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -15111,30 +15180,30 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="69"/>
-      <c r="C1" s="269" t="s">
+      <c r="C1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="269" t="s">
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="275" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="269" t="s">
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="275" t="s">
         <v>446</v>
       </c>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="269" t="s">
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="271"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="277"/>
       <c r="S1" s="45"/>
       <c r="T1" s="45"/>
       <c r="U1" s="45"/>
@@ -15232,12 +15301,12 @@
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="273" t="s">
+      <c r="S3" s="279" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="275"/>
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="281"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="69" t="s">
@@ -15302,12 +15371,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="266" t="s">
+      <c r="S5" s="272" t="s">
         <v>286</v>
       </c>
-      <c r="T5" s="267"/>
-      <c r="U5" s="267"/>
-      <c r="V5" s="268"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="274"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="69" t="s">
@@ -15337,12 +15406,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="266" t="s">
+      <c r="S6" s="272" t="s">
         <v>287</v>
       </c>
-      <c r="T6" s="267"/>
-      <c r="U6" s="267"/>
-      <c r="V6" s="268"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="273"/>
+      <c r="V6" s="274"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="69" t="s">
@@ -15409,12 +15478,12 @@
         <v>288</v>
       </c>
       <c r="R8" s="41"/>
-      <c r="S8" s="289" t="s">
+      <c r="S8" s="295" t="s">
         <v>382</v>
       </c>
-      <c r="T8" s="290"/>
-      <c r="U8" s="290"/>
-      <c r="V8" s="290"/>
+      <c r="T8" s="296"/>
+      <c r="U8" s="296"/>
+      <c r="V8" s="296"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="69" t="s">
@@ -17898,36 +17967,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="269" t="s">
+      <c r="C1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="272" t="s">
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="270"/>
-      <c r="K1" s="269" t="s">
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="276"/>
+      <c r="K1" s="275" t="s">
         <v>446</v>
       </c>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
-      <c r="O1" s="269" t="s">
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="271"/>
-      <c r="Z1" s="269" t="s">
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="277"/>
+      <c r="Z1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="270"/>
-      <c r="AB1" s="270"/>
-      <c r="AC1" s="271"/>
+      <c r="AA1" s="276"/>
+      <c r="AB1" s="276"/>
+      <c r="AC1" s="277"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -17996,33 +18065,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="273" t="s">
+      <c r="C3" s="279" t="s">
         <v>269</v>
       </c>
-      <c r="D3" s="274"/>
-      <c r="E3" s="274"/>
-      <c r="F3" s="275"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="274"/>
-      <c r="I3" s="274"/>
-      <c r="J3" s="275"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="281"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
+      <c r="I3" s="280"/>
+      <c r="J3" s="281"/>
       <c r="K3" s="224"/>
       <c r="O3" s="224"/>
       <c r="P3" s="225"/>
       <c r="Q3" s="225"/>
       <c r="R3" s="226"/>
-      <c r="S3" s="273" t="s">
+      <c r="S3" s="279" t="s">
         <v>406</v>
       </c>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="275"/>
-      <c r="Z3" s="273" t="s">
+      <c r="T3" s="280"/>
+      <c r="U3" s="280"/>
+      <c r="V3" s="281"/>
+      <c r="Z3" s="279" t="s">
         <v>269</v>
       </c>
-      <c r="AA3" s="274"/>
-      <c r="AB3" s="274"/>
-      <c r="AC3" s="275"/>
+      <c r="AA3" s="280"/>
+      <c r="AB3" s="280"/>
+      <c r="AC3" s="281"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -18079,12 +18148,12 @@
       <c r="P5" s="225"/>
       <c r="Q5" s="225"/>
       <c r="R5" s="226"/>
-      <c r="S5" s="266" t="s">
+      <c r="S5" s="272" t="s">
         <v>506</v>
       </c>
-      <c r="T5" s="267"/>
-      <c r="U5" s="267"/>
-      <c r="V5" s="268"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="273"/>
+      <c r="V5" s="274"/>
       <c r="W5" s="85" t="s">
         <v>508</v>
       </c>
@@ -18114,12 +18183,12 @@
       <c r="P6" s="225"/>
       <c r="Q6" s="225"/>
       <c r="R6" s="226"/>
-      <c r="S6" s="266" t="s">
+      <c r="S6" s="272" t="s">
         <v>423</v>
       </c>
-      <c r="T6" s="267"/>
-      <c r="U6" s="267"/>
-      <c r="V6" s="268"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="273"/>
+      <c r="V6" s="274"/>
       <c r="Z6" s="224"/>
       <c r="AA6" s="225"/>
       <c r="AB6" s="225"/>
@@ -19478,17 +19547,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="S5:V5"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="Z3:AC3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19519,30 +19588,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="21"/>
-      <c r="B1" s="269" t="s">
+      <c r="B1" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="272" t="s">
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="270"/>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="269" t="s">
+      <c r="G1" s="276"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="275" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="270"/>
-      <c r="L1" s="270"/>
-      <c r="M1" s="271"/>
-      <c r="N1" s="269" t="s">
+      <c r="K1" s="276"/>
+      <c r="L1" s="276"/>
+      <c r="M1" s="277"/>
+      <c r="N1" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="271"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="277"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
@@ -19629,12 +19698,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="273" t="s">
+      <c r="R3" s="279" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="274"/>
-      <c r="T3" s="274"/>
-      <c r="U3" s="275"/>
+      <c r="S3" s="280"/>
+      <c r="T3" s="280"/>
+      <c r="U3" s="281"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="39" t="s">
@@ -19687,12 +19756,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="266" t="s">
+      <c r="R5" s="272" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="267"/>
-      <c r="T5" s="267"/>
-      <c r="U5" s="268"/>
+      <c r="S5" s="273"/>
+      <c r="T5" s="273"/>
+      <c r="U5" s="274"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
@@ -19714,12 +19783,12 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="34"/>
-      <c r="R6" s="266" t="s">
+      <c r="R6" s="272" t="s">
         <v>266</v>
       </c>
-      <c r="S6" s="267"/>
-      <c r="T6" s="267"/>
-      <c r="U6" s="268"/>
+      <c r="S6" s="273"/>
+      <c r="T6" s="273"/>
+      <c r="U6" s="274"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="39" t="s">
@@ -23194,67 +23263,67 @@
       </c>
     </row>
     <row r="6" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="276" t="s">
+      <c r="B6" s="282" t="s">
         <v>518</v>
       </c>
-      <c r="C6" s="277"/>
-      <c r="D6" s="278"/>
-      <c r="E6" s="276" t="s">
+      <c r="C6" s="283"/>
+      <c r="D6" s="284"/>
+      <c r="E6" s="282" t="s">
         <v>519</v>
       </c>
-      <c r="F6" s="277"/>
-      <c r="G6" s="278"/>
+      <c r="F6" s="283"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="276" t="s">
+      <c r="B7" s="282" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="277"/>
-      <c r="D7" s="277"/>
-      <c r="E7" s="277"/>
-      <c r="F7" s="277"/>
-      <c r="G7" s="277"/>
-      <c r="H7" s="277"/>
-      <c r="I7" s="277"/>
-      <c r="J7" s="277"/>
-      <c r="K7" s="277"/>
-      <c r="L7" s="277"/>
-      <c r="M7" s="277"/>
-      <c r="N7" s="277"/>
-      <c r="O7" s="277"/>
-      <c r="P7" s="278"/>
-      <c r="Q7" s="276" t="s">
+      <c r="C7" s="283"/>
+      <c r="D7" s="283"/>
+      <c r="E7" s="283"/>
+      <c r="F7" s="283"/>
+      <c r="G7" s="283"/>
+      <c r="H7" s="283"/>
+      <c r="I7" s="283"/>
+      <c r="J7" s="283"/>
+      <c r="K7" s="283"/>
+      <c r="L7" s="283"/>
+      <c r="M7" s="283"/>
+      <c r="N7" s="283"/>
+      <c r="O7" s="283"/>
+      <c r="P7" s="284"/>
+      <c r="Q7" s="282" t="s">
         <v>219</v>
       </c>
-      <c r="R7" s="277"/>
-      <c r="S7" s="277"/>
-      <c r="T7" s="277"/>
-      <c r="U7" s="277"/>
-      <c r="V7" s="277"/>
-      <c r="W7" s="277"/>
-      <c r="X7" s="277"/>
-      <c r="Y7" s="277"/>
-      <c r="Z7" s="277"/>
-      <c r="AA7" s="278"/>
-      <c r="AB7" s="276" t="s">
+      <c r="R7" s="283"/>
+      <c r="S7" s="283"/>
+      <c r="T7" s="283"/>
+      <c r="U7" s="283"/>
+      <c r="V7" s="283"/>
+      <c r="W7" s="283"/>
+      <c r="X7" s="283"/>
+      <c r="Y7" s="283"/>
+      <c r="Z7" s="283"/>
+      <c r="AA7" s="284"/>
+      <c r="AB7" s="282" t="s">
         <v>220</v>
       </c>
-      <c r="AC7" s="277"/>
-      <c r="AD7" s="277"/>
-      <c r="AE7" s="277"/>
-      <c r="AF7" s="277"/>
-      <c r="AG7" s="277"/>
-      <c r="AH7" s="277"/>
-      <c r="AI7" s="277"/>
-      <c r="AJ7" s="277"/>
-      <c r="AK7" s="277"/>
-      <c r="AL7" s="277"/>
-      <c r="AM7" s="277"/>
-      <c r="AN7" s="277"/>
-      <c r="AO7" s="277"/>
-      <c r="AP7" s="277"/>
-      <c r="AQ7" s="277"/>
-      <c r="AR7" s="278"/>
+      <c r="AC7" s="283"/>
+      <c r="AD7" s="283"/>
+      <c r="AE7" s="283"/>
+      <c r="AF7" s="283"/>
+      <c r="AG7" s="283"/>
+      <c r="AH7" s="283"/>
+      <c r="AI7" s="283"/>
+      <c r="AJ7" s="283"/>
+      <c r="AK7" s="283"/>
+      <c r="AL7" s="283"/>
+      <c r="AM7" s="283"/>
+      <c r="AN7" s="283"/>
+      <c r="AO7" s="283"/>
+      <c r="AP7" s="283"/>
+      <c r="AQ7" s="283"/>
+      <c r="AR7" s="284"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.4">
       <c r="E9" s="45"/>
@@ -23323,18 +23392,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B1" s="265" t="s">
+      <c r="B1" s="271" t="s">
         <v>684</v>
       </c>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="265"/>
-      <c r="F1" s="265"/>
-      <c r="G1" s="265"/>
-      <c r="H1" s="265"/>
-      <c r="I1" s="265"/>
-      <c r="J1" s="265"/>
-      <c r="K1" s="265"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
@@ -24505,11 +24574,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D1" s="273" t="s">
+      <c r="D1" s="279" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
+      <c r="E1" s="280"/>
+      <c r="F1" s="280"/>
       <c r="G1" s="64"/>
       <c r="H1" s="60"/>
       <c r="I1" s="93"/>
@@ -24567,12 +24636,12 @@
     </row>
     <row r="5" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="269" t="s">
+      <c r="D6" s="275" t="s">
         <v>623</v>
       </c>
-      <c r="E6" s="270"/>
-      <c r="F6" s="270"/>
-      <c r="G6" s="271"/>
+      <c r="E6" s="276"/>
+      <c r="F6" s="276"/>
+      <c r="G6" s="277"/>
       <c r="H6" s="123"/>
       <c r="I6" s="95"/>
       <c r="J6" s="95"/>
@@ -24581,27 +24650,27 @@
       <c r="M6" s="95"/>
       <c r="N6" s="95"/>
       <c r="O6" s="95"/>
-      <c r="P6" s="269" t="s">
+      <c r="P6" s="275" t="s">
         <v>624</v>
       </c>
-      <c r="Q6" s="270"/>
-      <c r="R6" s="270"/>
-      <c r="S6" s="271"/>
-      <c r="AF6" s="269" t="s">
+      <c r="Q6" s="276"/>
+      <c r="R6" s="276"/>
+      <c r="S6" s="277"/>
+      <c r="AF6" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="AG6" s="270"/>
-      <c r="AH6" s="270"/>
-      <c r="AI6" s="271"/>
+      <c r="AG6" s="276"/>
+      <c r="AH6" s="276"/>
+      <c r="AI6" s="277"/>
       <c r="AJ6" s="154"/>
-      <c r="AK6" s="269" t="s">
+      <c r="AK6" s="275" t="s">
         <v>622</v>
       </c>
-      <c r="AL6" s="270"/>
-      <c r="AM6" s="270"/>
-      <c r="AN6" s="270"/>
-      <c r="AO6" s="270"/>
-      <c r="AP6" s="271"/>
+      <c r="AL6" s="276"/>
+      <c r="AM6" s="276"/>
+      <c r="AN6" s="276"/>
+      <c r="AO6" s="276"/>
+      <c r="AP6" s="277"/>
     </row>
     <row r="7" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D7" s="35" t="s">
@@ -24679,11 +24748,11 @@
       <c r="J8" s="95"/>
       <c r="K8" s="95"/>
       <c r="L8" s="95"/>
-      <c r="M8" s="280" t="s">
+      <c r="M8" s="286" t="s">
         <v>530</v>
       </c>
-      <c r="N8" s="280"/>
-      <c r="O8" s="280"/>
+      <c r="N8" s="286"/>
+      <c r="O8" s="286"/>
       <c r="P8" s="119"/>
       <c r="Q8" s="120"/>
       <c r="R8" s="120"/>
@@ -24704,12 +24773,12 @@
       <c r="AL8" s="155"/>
       <c r="AM8" s="155"/>
       <c r="AN8" s="155"/>
-      <c r="AQ8" s="266" t="s">
+      <c r="AQ8" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="AR8" s="267"/>
-      <c r="AS8" s="267"/>
-      <c r="AT8" s="268"/>
+      <c r="AR8" s="273"/>
+      <c r="AS8" s="273"/>
+      <c r="AT8" s="274"/>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D9" s="40"/>
@@ -24721,11 +24790,11 @@
       <c r="J9" s="122"/>
       <c r="K9" s="122"/>
       <c r="L9" s="122"/>
-      <c r="M9" s="282" t="s">
+      <c r="M9" s="288" t="s">
         <v>531</v>
       </c>
-      <c r="N9" s="282"/>
-      <c r="O9" s="281"/>
+      <c r="N9" s="288"/>
+      <c r="O9" s="287"/>
       <c r="P9" s="119"/>
       <c r="Q9" s="120"/>
       <c r="R9" s="120"/>
@@ -24767,9 +24836,9 @@
       <c r="J10" s="122"/>
       <c r="K10" s="122"/>
       <c r="L10" s="122"/>
-      <c r="M10" s="279"/>
-      <c r="N10" s="279"/>
-      <c r="O10" s="279"/>
+      <c r="M10" s="285"/>
+      <c r="N10" s="285"/>
+      <c r="O10" s="285"/>
       <c r="P10" s="119"/>
       <c r="Q10" s="120"/>
       <c r="R10" s="120"/>
@@ -24794,12 +24863,12 @@
       <c r="AL10" s="155"/>
       <c r="AM10" s="155"/>
       <c r="AN10" s="155"/>
-      <c r="AQ10" s="266" t="s">
+      <c r="AQ10" s="272" t="s">
         <v>54</v>
       </c>
-      <c r="AR10" s="267"/>
-      <c r="AS10" s="267"/>
-      <c r="AT10" s="268"/>
+      <c r="AR10" s="273"/>
+      <c r="AS10" s="273"/>
+      <c r="AT10" s="274"/>
     </row>
     <row r="11" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="40"/>
@@ -24835,12 +24904,12 @@
       <c r="AL11" s="155"/>
       <c r="AM11" s="155"/>
       <c r="AN11" s="155"/>
-      <c r="AQ11" s="266" t="s">
+      <c r="AQ11" s="272" t="s">
         <v>621</v>
       </c>
-      <c r="AR11" s="267"/>
-      <c r="AS11" s="267"/>
-      <c r="AT11" s="268"/>
+      <c r="AR11" s="273"/>
+      <c r="AS11" s="273"/>
+      <c r="AT11" s="274"/>
       <c r="AU11" s="26" t="s">
         <v>267</v>
       </c>
@@ -24866,11 +24935,11 @@
       <c r="J12" s="95"/>
       <c r="K12" s="95"/>
       <c r="L12" s="95"/>
-      <c r="M12" s="283" t="s">
+      <c r="M12" s="289" t="s">
         <v>529</v>
       </c>
-      <c r="N12" s="283"/>
-      <c r="O12" s="283"/>
+      <c r="N12" s="289"/>
+      <c r="O12" s="289"/>
       <c r="P12" s="119"/>
       <c r="Q12" s="120"/>
       <c r="R12" s="120"/>
@@ -24884,12 +24953,12 @@
       <c r="AL12" s="155"/>
       <c r="AM12" s="155"/>
       <c r="AN12" s="155"/>
-      <c r="AQ12" s="266" t="s">
+      <c r="AQ12" s="272" t="s">
         <v>528</v>
       </c>
-      <c r="AR12" s="267"/>
-      <c r="AS12" s="267"/>
-      <c r="AT12" s="268"/>
+      <c r="AR12" s="273"/>
+      <c r="AS12" s="273"/>
+      <c r="AT12" s="274"/>
       <c r="AV12" s="21" t="s">
         <v>617</v>
       </c>
@@ -24905,12 +24974,12 @@
         <v>524</v>
       </c>
       <c r="C13" s="132"/>
-      <c r="D13" s="269" t="s">
+      <c r="D13" s="275" t="s">
         <v>532</v>
       </c>
-      <c r="E13" s="270"/>
-      <c r="F13" s="270"/>
-      <c r="G13" s="270"/>
+      <c r="E13" s="276"/>
+      <c r="F13" s="276"/>
+      <c r="G13" s="276"/>
       <c r="H13" s="168" t="s">
         <v>635</v>
       </c>
@@ -24933,11 +25002,11 @@
       <c r="O13" s="181" t="s">
         <v>639</v>
       </c>
-      <c r="P13" s="269" t="s">
+      <c r="P13" s="275" t="s">
         <v>533</v>
       </c>
-      <c r="Q13" s="270"/>
-      <c r="R13" s="270"/>
+      <c r="Q13" s="276"/>
+      <c r="R13" s="276"/>
       <c r="S13" s="157"/>
       <c r="T13" s="171" t="s">
         <v>660</v>
@@ -24973,18 +25042,18 @@
       <c r="AH13" s="60"/>
       <c r="AI13" s="43"/>
       <c r="AJ13" s="154"/>
-      <c r="AK13" s="266" t="s">
+      <c r="AK13" s="272" t="s">
         <v>532</v>
       </c>
-      <c r="AL13" s="267"/>
-      <c r="AM13" s="267"/>
-      <c r="AN13" s="267"/>
-      <c r="AQ13" s="266" t="s">
+      <c r="AL13" s="273"/>
+      <c r="AM13" s="273"/>
+      <c r="AN13" s="273"/>
+      <c r="AQ13" s="272" t="s">
         <v>614</v>
       </c>
-      <c r="AR13" s="265"/>
-      <c r="AS13" s="265"/>
-      <c r="AT13" s="265"/>
+      <c r="AR13" s="271"/>
+      <c r="AS13" s="271"/>
+      <c r="AT13" s="271"/>
       <c r="AV13" s="21" t="s">
         <v>618</v>
       </c>
@@ -25676,8 +25745,8 @@
       </c>
       <c r="AO30" s="160"/>
       <c r="AP30" s="162"/>
-      <c r="AR30" s="281"/>
-      <c r="AS30" s="281"/>
+      <c r="AR30" s="287"/>
+      <c r="AS30" s="287"/>
     </row>
     <row r="31" spans="1:52" s="26" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="200" t="s">
@@ -26130,8 +26199,8 @@
         <v>88</v>
       </c>
       <c r="AO40" s="160"/>
-      <c r="AR40" s="279"/>
-      <c r="AS40" s="279"/>
+      <c r="AR40" s="285"/>
+      <c r="AS40" s="285"/>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A41" s="152" t="s">
@@ -26365,8 +26434,8 @@
         <v>637</v>
       </c>
       <c r="AP46" s="162"/>
-      <c r="AR46" s="279"/>
-      <c r="AS46" s="279"/>
+      <c r="AR46" s="285"/>
+      <c r="AS46" s="285"/>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A47" s="152" t="s">
@@ -26451,12 +26520,12 @@
         <v>526</v>
       </c>
       <c r="C49" s="179"/>
-      <c r="D49" s="269" t="s">
+      <c r="D49" s="275" t="s">
         <v>532</v>
       </c>
-      <c r="E49" s="270"/>
-      <c r="F49" s="270"/>
-      <c r="G49" s="270"/>
+      <c r="E49" s="276"/>
+      <c r="F49" s="276"/>
+      <c r="G49" s="276"/>
       <c r="H49" s="168" t="s">
         <v>635</v>
       </c>
@@ -26479,11 +26548,11 @@
       <c r="O49" s="181" t="s">
         <v>639</v>
       </c>
-      <c r="P49" s="269" t="s">
+      <c r="P49" s="275" t="s">
         <v>533</v>
       </c>
-      <c r="Q49" s="270"/>
-      <c r="R49" s="270"/>
+      <c r="Q49" s="276"/>
+      <c r="R49" s="276"/>
       <c r="S49" s="190"/>
       <c r="T49" s="171" t="s">
         <v>660</v>
@@ -27813,12 +27882,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AR40:AS40"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="AK13:AN13"/>
-    <mergeCell ref="AQ10:AT10"/>
-    <mergeCell ref="AQ8:AT8"/>
-    <mergeCell ref="AQ11:AT11"/>
     <mergeCell ref="D49:G49"/>
     <mergeCell ref="P49:R49"/>
     <mergeCell ref="AR46:AS46"/>
@@ -27835,6 +27898,12 @@
     <mergeCell ref="M10:O10"/>
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="AQ12:AT12"/>
+    <mergeCell ref="AR40:AS40"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="AK13:AN13"/>
+    <mergeCell ref="AQ10:AT10"/>
+    <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="AQ11:AT11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27892,11 +27961,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.4">
-      <c r="B1" s="273" t="s">
+      <c r="B1" s="279" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="274"/>
-      <c r="D1" s="274"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.4">
@@ -27921,49 +27990,49 @@
       </c>
     </row>
     <row r="4" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="284" t="s">
+      <c r="B4" s="290" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285"/>
-      <c r="E4" s="286"/>
+      <c r="C4" s="291"/>
+      <c r="D4" s="291"/>
+      <c r="E4" s="292"/>
     </row>
     <row r="5" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="266" t="s">
+      <c r="B5" s="272" t="s">
         <v>527</v>
       </c>
-      <c r="C5" s="267"/>
-      <c r="D5" s="267"/>
-      <c r="E5" s="268"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="274"/>
     </row>
     <row r="6" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="269" t="s">
+      <c r="B6" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="270"/>
-      <c r="D6" s="270"/>
-      <c r="E6" s="271"/>
-      <c r="F6" s="272" t="s">
+      <c r="C6" s="276"/>
+      <c r="D6" s="276"/>
+      <c r="E6" s="277"/>
+      <c r="F6" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="270"/>
-      <c r="H6" s="270"/>
-      <c r="I6" s="270"/>
-      <c r="J6" s="269" t="s">
+      <c r="G6" s="276"/>
+      <c r="H6" s="276"/>
+      <c r="I6" s="276"/>
+      <c r="J6" s="275" t="s">
         <v>184</v>
       </c>
-      <c r="K6" s="270"/>
-      <c r="L6" s="270"/>
-      <c r="M6" s="271"/>
-      <c r="N6" s="269" t="s">
+      <c r="K6" s="276"/>
+      <c r="L6" s="276"/>
+      <c r="M6" s="277"/>
+      <c r="N6" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="O6" s="270"/>
-      <c r="P6" s="270"/>
-      <c r="Q6" s="271"/>
+      <c r="O6" s="276"/>
+      <c r="P6" s="276"/>
+      <c r="Q6" s="277"/>
       <c r="V6" s="56"/>
       <c r="W6" s="57"/>
       <c r="X6" s="57"/>
@@ -27992,24 +28061,24 @@
     </row>
     <row r="7" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="209"/>
-      <c r="B7" s="269" t="s">
+      <c r="B7" s="275" t="s">
         <v>623</v>
       </c>
-      <c r="C7" s="270"/>
-      <c r="D7" s="270"/>
-      <c r="E7" s="271"/>
-      <c r="F7" s="269" t="s">
+      <c r="C7" s="276"/>
+      <c r="D7" s="276"/>
+      <c r="E7" s="277"/>
+      <c r="F7" s="275" t="s">
         <v>624</v>
       </c>
-      <c r="G7" s="270"/>
-      <c r="H7" s="270"/>
-      <c r="I7" s="271"/>
-      <c r="J7" s="269" t="s">
+      <c r="G7" s="276"/>
+      <c r="H7" s="276"/>
+      <c r="I7" s="277"/>
+      <c r="J7" s="275" t="s">
         <v>795</v>
       </c>
-      <c r="K7" s="270"/>
-      <c r="L7" s="270"/>
-      <c r="M7" s="271"/>
+      <c r="K7" s="276"/>
+      <c r="L7" s="276"/>
+      <c r="M7" s="277"/>
       <c r="N7" s="206"/>
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
@@ -31815,16 +31884,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31871,12 +31940,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.4">
-      <c r="B1" s="291"/>
-      <c r="C1" s="273" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="279" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="274"/>
-      <c r="E1" s="274"/>
+      <c r="D1" s="280"/>
+      <c r="E1" s="280"/>
       <c r="F1" s="42"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
@@ -31909,63 +31978,63 @@
       </c>
     </row>
     <row r="4" spans="1:35" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="284" t="s">
+      <c r="C4" s="290" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="285"/>
-      <c r="E4" s="285"/>
-      <c r="F4" s="286"/>
+      <c r="D4" s="291"/>
+      <c r="E4" s="291"/>
+      <c r="F4" s="292"/>
     </row>
     <row r="5" spans="1:35" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="266" t="s">
+      <c r="C5" s="272" t="s">
         <v>527</v>
       </c>
-      <c r="D5" s="267"/>
-      <c r="E5" s="267"/>
-      <c r="F5" s="268"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="274"/>
     </row>
     <row r="6" spans="1:35" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="291"/>
-      <c r="C6" s="269" t="s">
+      <c r="B6" s="265"/>
+      <c r="C6" s="275" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="270"/>
-      <c r="E6" s="270"/>
-      <c r="F6" s="271"/>
+      <c r="D6" s="276"/>
+      <c r="E6" s="276"/>
+      <c r="F6" s="277"/>
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
       <c r="I6" s="57"/>
       <c r="J6" s="58"/>
-      <c r="K6" s="272" t="s">
+      <c r="K6" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="L6" s="270"/>
-      <c r="M6" s="270"/>
-      <c r="N6" s="270"/>
+      <c r="L6" s="276"/>
+      <c r="M6" s="276"/>
+      <c r="N6" s="276"/>
       <c r="O6" s="56"/>
       <c r="P6" s="57"/>
       <c r="Q6" s="57"/>
       <c r="R6" s="58"/>
-      <c r="S6" s="269" t="s">
+      <c r="S6" s="275" t="s">
         <v>184</v>
       </c>
-      <c r="T6" s="270"/>
-      <c r="U6" s="270"/>
-      <c r="V6" s="271"/>
+      <c r="T6" s="276"/>
+      <c r="U6" s="276"/>
+      <c r="V6" s="277"/>
       <c r="W6" s="57"/>
       <c r="X6" s="57"/>
       <c r="Y6" s="57"/>
       <c r="Z6" s="57"/>
       <c r="AA6" s="58"/>
-      <c r="AB6" s="269" t="s">
+      <c r="AB6" s="275" t="s">
         <v>187</v>
       </c>
-      <c r="AC6" s="270"/>
-      <c r="AD6" s="270"/>
-      <c r="AE6" s="271"/>
+      <c r="AC6" s="276"/>
+      <c r="AD6" s="276"/>
+      <c r="AE6" s="277"/>
       <c r="AF6" s="213"/>
       <c r="AG6" s="214"/>
       <c r="AH6" s="214"/>
@@ -31973,53 +32042,53 @@
     </row>
     <row r="7" spans="1:35" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="209"/>
-      <c r="B7" s="292" t="s">
+      <c r="B7" s="266" t="s">
         <v>934</v>
       </c>
-      <c r="C7" s="270" t="s">
+      <c r="C7" s="276" t="s">
         <v>623</v>
       </c>
-      <c r="D7" s="270"/>
-      <c r="E7" s="270"/>
-      <c r="F7" s="271"/>
-      <c r="G7" s="269" t="s">
+      <c r="D7" s="276"/>
+      <c r="E7" s="276"/>
+      <c r="F7" s="277"/>
+      <c r="G7" s="275" t="s">
         <v>839</v>
       </c>
-      <c r="H7" s="270"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="271"/>
-      <c r="K7" s="269" t="s">
+      <c r="H7" s="276"/>
+      <c r="I7" s="276"/>
+      <c r="J7" s="277"/>
+      <c r="K7" s="275" t="s">
         <v>624</v>
       </c>
-      <c r="L7" s="270"/>
-      <c r="M7" s="270"/>
-      <c r="N7" s="271"/>
-      <c r="O7" s="269"/>
-      <c r="P7" s="270"/>
-      <c r="Q7" s="270"/>
-      <c r="R7" s="271"/>
-      <c r="S7" s="269" t="s">
+      <c r="L7" s="276"/>
+      <c r="M7" s="276"/>
+      <c r="N7" s="277"/>
+      <c r="O7" s="275"/>
+      <c r="P7" s="276"/>
+      <c r="Q7" s="276"/>
+      <c r="R7" s="277"/>
+      <c r="S7" s="275" t="s">
         <v>795</v>
       </c>
-      <c r="T7" s="270"/>
-      <c r="U7" s="270"/>
-      <c r="V7" s="271"/>
+      <c r="T7" s="276"/>
+      <c r="U7" s="276"/>
+      <c r="V7" s="277"/>
       <c r="AB7" s="216"/>
       <c r="AC7" s="216"/>
       <c r="AD7" s="216"/>
       <c r="AE7" s="217"/>
-      <c r="AF7" s="269" t="s">
+      <c r="AF7" s="275" t="s">
         <v>840</v>
       </c>
-      <c r="AG7" s="270"/>
-      <c r="AH7" s="270"/>
-      <c r="AI7" s="271"/>
+      <c r="AG7" s="276"/>
+      <c r="AH7" s="276"/>
+      <c r="AI7" s="277"/>
     </row>
     <row r="8" spans="1:35" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="209">
         <v>0</v>
       </c>
-      <c r="B8" s="293" t="s">
+      <c r="B8" s="267" t="s">
         <v>935</v>
       </c>
       <c r="C8" s="261" t="s">
@@ -32246,7 +32315,7 @@
       <c r="A14" s="209" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="294" t="s">
+      <c r="B14" s="268" t="s">
         <v>936</v>
       </c>
       <c r="C14" s="82"/>
@@ -33283,6 +33352,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="K6:N6"/>
     <mergeCell ref="AF7:AI7"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="C7:F7"/>
@@ -33291,11 +33365,6 @@
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="O7:R7"/>
     <mergeCell ref="S6:V6"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="K6:N6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
220428-rev1 cplt MUX&deMUX revise
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7539ECD3-6A0F-435B-AD01-944ED56BAB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB45F72-8483-4480-9428-805128523E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="5" activeTab="8" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="5" activeTab="10" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD1,2" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4464" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4475" uniqueCount="968">
   <si>
     <t>预测</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3402,6 +3402,26 @@
   </si>
   <si>
     <t>NEW_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`5-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`3-11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4-00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`6-10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3842,7 +3862,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4680,6 +4700,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4767,14 +4796,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="58" fontId="2" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5100,11 +5126,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W1" s="279" t="s">
+      <c r="W1" s="282" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="279"/>
-      <c r="Y1" s="279"/>
+      <c r="X1" s="282"/>
+      <c r="Y1" s="282"/>
       <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
@@ -5119,11 +5145,11 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W3" s="279" t="s">
+      <c r="W3" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="279"/>
-      <c r="Y3" s="279"/>
+      <c r="X3" s="282"/>
+      <c r="Y3" s="282"/>
       <c r="Z3" s="24" t="s">
         <v>55</v>
       </c>
@@ -5901,57 +5927,57 @@
       <c r="A1" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="283" t="s">
+      <c r="B1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="286" t="s">
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="284"/>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="283" t="s">
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="286" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="284"/>
-      <c r="L1" s="284"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="283" t="s">
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="284"/>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="287" t="s">
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="290" t="s">
         <v>258</v>
       </c>
-      <c r="S1" s="288"/>
-      <c r="T1" s="288"/>
+      <c r="S1" s="291"/>
+      <c r="T1" s="291"/>
       <c r="U1" s="42"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="222"/>
-      <c r="B2" s="283" t="s">
+      <c r="B2" s="286" t="s">
         <v>619</v>
       </c>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="283" t="s">
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="286" t="s">
         <v>620</v>
       </c>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
-      <c r="J2" s="283" t="s">
+      <c r="G2" s="287"/>
+      <c r="H2" s="287"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="286" t="s">
         <v>791</v>
       </c>
-      <c r="K2" s="284"/>
-      <c r="L2" s="284"/>
-      <c r="M2" s="285"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="288"/>
       <c r="N2" s="44"/>
       <c r="O2" s="226"/>
       <c r="P2" s="226"/>
@@ -6050,12 +6076,12 @@
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="34"/>
-      <c r="R4" s="298" t="s">
+      <c r="R4" s="301" t="s">
         <v>282</v>
       </c>
-      <c r="S4" s="299"/>
-      <c r="T4" s="299"/>
-      <c r="U4" s="300"/>
+      <c r="S4" s="302"/>
+      <c r="T4" s="302"/>
+      <c r="U4" s="303"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="222" t="s">
@@ -6078,12 +6104,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="280" t="s">
+      <c r="R5" s="283" t="s">
         <v>869</v>
       </c>
-      <c r="S5" s="281"/>
-      <c r="T5" s="281"/>
-      <c r="U5" s="282"/>
+      <c r="S5" s="284"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="285"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="222" t="s">
@@ -7753,11 +7779,11 @@
       <c r="K93" s="220"/>
       <c r="L93" s="230"/>
       <c r="M93" s="230"/>
-      <c r="R93" s="287" t="s">
+      <c r="R93" s="290" t="s">
         <v>258</v>
       </c>
-      <c r="S93" s="288"/>
-      <c r="T93" s="288"/>
+      <c r="S93" s="291"/>
+      <c r="T93" s="291"/>
       <c r="U93" s="42"/>
     </row>
     <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -7846,12 +7872,12 @@
       <c r="K96" s="81"/>
       <c r="L96" s="81"/>
       <c r="M96" s="82"/>
-      <c r="R96" s="298" t="s">
+      <c r="R96" s="301" t="s">
         <v>54</v>
       </c>
-      <c r="S96" s="301"/>
-      <c r="T96" s="301"/>
-      <c r="U96" s="302"/>
+      <c r="S96" s="304"/>
+      <c r="T96" s="304"/>
+      <c r="U96" s="305"/>
     </row>
     <row r="97" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="222" t="s">
@@ -7873,12 +7899,12 @@
       <c r="K97" s="81"/>
       <c r="L97" s="81"/>
       <c r="M97" s="82"/>
-      <c r="R97" s="287" t="s">
+      <c r="R97" s="290" t="s">
         <v>869</v>
       </c>
-      <c r="S97" s="288"/>
-      <c r="T97" s="288"/>
-      <c r="U97" s="289"/>
+      <c r="S97" s="291"/>
+      <c r="T97" s="291"/>
+      <c r="U97" s="292"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A98" s="222" t="s">
@@ -7930,11 +7956,11 @@
       <c r="K100" s="81"/>
       <c r="L100" s="81"/>
       <c r="M100" s="82"/>
-      <c r="R100" s="287" t="s">
+      <c r="R100" s="290" t="s">
         <v>870</v>
       </c>
-      <c r="S100" s="288"/>
-      <c r="T100" s="288"/>
+      <c r="S100" s="291"/>
+      <c r="T100" s="291"/>
       <c r="U100" s="42"/>
     </row>
     <row r="101" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -8030,12 +8056,12 @@
       <c r="M103" s="34" t="s">
         <v>472</v>
       </c>
-      <c r="R103" s="298" t="s">
+      <c r="R103" s="301" t="s">
         <v>282</v>
       </c>
-      <c r="S103" s="301"/>
-      <c r="T103" s="301"/>
-      <c r="U103" s="302"/>
+      <c r="S103" s="304"/>
+      <c r="T103" s="304"/>
+      <c r="U103" s="305"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A104" s="222" t="s">
@@ -8052,12 +8078,12 @@
       <c r="L104" s="34" t="s">
         <v>469</v>
       </c>
-      <c r="R104" s="287" t="s">
+      <c r="R104" s="290" t="s">
         <v>869</v>
       </c>
-      <c r="S104" s="288"/>
-      <c r="T104" s="288"/>
-      <c r="U104" s="289"/>
+      <c r="S104" s="291"/>
+      <c r="T104" s="291"/>
+      <c r="U104" s="292"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A105" s="222" t="s">
@@ -8407,12 +8433,12 @@
       <c r="L124" s="34" t="s">
         <v>768</v>
       </c>
-      <c r="R124" s="287" t="s">
+      <c r="R124" s="290" t="s">
         <v>881</v>
       </c>
-      <c r="S124" s="288"/>
-      <c r="T124" s="288"/>
-      <c r="U124" s="289"/>
+      <c r="S124" s="291"/>
+      <c r="T124" s="291"/>
+      <c r="U124" s="292"/>
     </row>
     <row r="125" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="222" t="s">
@@ -8488,23 +8514,23 @@
       <c r="G127" s="75" t="s">
         <v>578</v>
       </c>
-      <c r="R127" s="298" t="s">
+      <c r="R127" s="301" t="s">
         <v>873</v>
       </c>
-      <c r="S127" s="301"/>
-      <c r="T127" s="301"/>
-      <c r="U127" s="302"/>
+      <c r="S127" s="304"/>
+      <c r="T127" s="304"/>
+      <c r="U127" s="305"/>
     </row>
     <row r="128" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="222" t="s">
         <v>882</v>
       </c>
-      <c r="R128" s="283" t="s">
+      <c r="R128" s="286" t="s">
         <v>869</v>
       </c>
-      <c r="S128" s="284"/>
-      <c r="T128" s="284"/>
-      <c r="U128" s="285"/>
+      <c r="S128" s="287"/>
+      <c r="T128" s="287"/>
+      <c r="U128" s="288"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A129" s="222" t="s">
@@ -8559,12 +8585,12 @@
       <c r="F135" s="80" t="s">
         <v>850</v>
       </c>
-      <c r="R135" s="287" t="s">
+      <c r="R135" s="290" t="s">
         <v>901</v>
       </c>
-      <c r="S135" s="288"/>
-      <c r="T135" s="288"/>
-      <c r="U135" s="289"/>
+      <c r="S135" s="291"/>
+      <c r="T135" s="291"/>
+      <c r="U135" s="292"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A136" s="222" t="s">
@@ -8616,23 +8642,23 @@
       <c r="A138" s="222" t="s">
         <v>858</v>
       </c>
-      <c r="R138" s="298" t="s">
+      <c r="R138" s="301" t="s">
         <v>873</v>
       </c>
-      <c r="S138" s="301"/>
-      <c r="T138" s="301"/>
-      <c r="U138" s="302"/>
+      <c r="S138" s="304"/>
+      <c r="T138" s="304"/>
+      <c r="U138" s="305"/>
     </row>
     <row r="139" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="222" t="s">
         <v>859</v>
       </c>
-      <c r="R139" s="283" t="s">
+      <c r="R139" s="286" t="s">
         <v>912</v>
       </c>
-      <c r="S139" s="284"/>
-      <c r="T139" s="284"/>
-      <c r="U139" s="285"/>
+      <c r="S139" s="287"/>
+      <c r="T139" s="287"/>
+      <c r="U139" s="288"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A140" s="222" t="s">
@@ -8681,12 +8707,12 @@
       <c r="F145" s="76" t="s">
         <v>843</v>
       </c>
-      <c r="R145" s="287" t="s">
+      <c r="R145" s="290" t="s">
         <v>911</v>
       </c>
-      <c r="S145" s="288"/>
-      <c r="T145" s="288"/>
-      <c r="U145" s="289"/>
+      <c r="S145" s="291"/>
+      <c r="T145" s="291"/>
+      <c r="U145" s="292"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A146" s="222" t="s">
@@ -8738,12 +8764,12 @@
       <c r="A148" s="222" t="s">
         <v>883</v>
       </c>
-      <c r="R148" s="298" t="s">
+      <c r="R148" s="301" t="s">
         <v>873</v>
       </c>
-      <c r="S148" s="301"/>
-      <c r="T148" s="301"/>
-      <c r="U148" s="302"/>
+      <c r="S148" s="304"/>
+      <c r="T148" s="304"/>
+      <c r="U148" s="305"/>
     </row>
     <row r="149" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="222" t="s">
@@ -8753,12 +8779,12 @@
       <c r="Q149" s="76" t="s">
         <v>874</v>
       </c>
-      <c r="R149" s="283" t="s">
+      <c r="R149" s="286" t="s">
         <v>912</v>
       </c>
-      <c r="S149" s="284"/>
-      <c r="T149" s="284"/>
-      <c r="U149" s="285"/>
+      <c r="S149" s="287"/>
+      <c r="T149" s="287"/>
+      <c r="U149" s="288"/>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A150" s="222" t="s">
@@ -8902,7 +8928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6F30D8-4F74-43CF-B0A2-082294AF7E0E}">
   <dimension ref="A1:AC51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="N28" sqref="N28"/>
     </sheetView>
@@ -8928,36 +8954,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="283" t="s">
+      <c r="C1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="286" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="284"/>
-      <c r="K1" s="283" t="s">
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="286" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="283" t="s">
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="286" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="285"/>
-      <c r="Z1" s="283" t="s">
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="288"/>
+      <c r="Z1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="284"/>
-      <c r="AB1" s="284"/>
-      <c r="AC1" s="285"/>
+      <c r="AA1" s="287"/>
+      <c r="AB1" s="287"/>
+      <c r="AC1" s="288"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -9026,33 +9052,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="287" t="s">
+      <c r="C3" s="290" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="287"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="289"/>
+      <c r="D3" s="291"/>
+      <c r="E3" s="291"/>
+      <c r="F3" s="292"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="291"/>
+      <c r="I3" s="291"/>
+      <c r="J3" s="292"/>
       <c r="K3" s="40"/>
       <c r="O3" s="40"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="287" t="s">
+      <c r="S3" s="290" t="s">
         <v>402</v>
       </c>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="289"/>
-      <c r="Z3" s="287" t="s">
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="292"/>
+      <c r="Z3" s="290" t="s">
         <v>265</v>
       </c>
-      <c r="AA3" s="288"/>
-      <c r="AB3" s="288"/>
-      <c r="AC3" s="289"/>
+      <c r="AA3" s="291"/>
+      <c r="AB3" s="291"/>
+      <c r="AC3" s="292"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -9109,12 +9135,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="280" t="s">
+      <c r="S5" s="283" t="s">
         <v>502</v>
       </c>
-      <c r="T5" s="281"/>
-      <c r="U5" s="281"/>
-      <c r="V5" s="282"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="284"/>
+      <c r="V5" s="285"/>
       <c r="W5" s="84" t="s">
         <v>504</v>
       </c>
@@ -9144,12 +9170,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="280" t="s">
+      <c r="S6" s="283" t="s">
         <v>941</v>
       </c>
-      <c r="T6" s="281"/>
-      <c r="U6" s="281"/>
-      <c r="V6" s="282"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="284"/>
+      <c r="V6" s="285"/>
       <c r="Z6" s="223"/>
       <c r="AA6" s="224"/>
       <c r="AB6" s="224"/>
@@ -9636,13 +9662,13 @@
       <c r="O22" s="76" t="s">
         <v>426</v>
       </c>
-      <c r="S22" s="303" t="s">
+      <c r="S22" s="306" t="s">
         <v>951</v>
       </c>
-      <c r="T22" s="305"/>
-      <c r="U22" s="305"/>
-      <c r="V22" s="305"/>
-      <c r="W22" s="305"/>
+      <c r="T22" s="308"/>
+      <c r="U22" s="308"/>
+      <c r="V22" s="308"/>
+      <c r="W22" s="308"/>
       <c r="Z22" s="79" t="s">
         <v>243</v>
       </c>
@@ -9692,12 +9718,12 @@
       <c r="P23" s="74" t="s">
         <v>422</v>
       </c>
-      <c r="S23" s="303" t="s">
+      <c r="S23" s="306" t="s">
         <v>952</v>
       </c>
-      <c r="T23" s="304"/>
-      <c r="U23" s="304"/>
-      <c r="V23" s="304"/>
+      <c r="T23" s="307"/>
+      <c r="U23" s="307"/>
+      <c r="V23" s="307"/>
       <c r="Z23" s="79" t="s">
         <v>245</v>
       </c>
@@ -9803,12 +9829,12 @@
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="280" t="s">
+      <c r="K26" s="283" t="s">
         <v>950</v>
       </c>
-      <c r="L26" s="281"/>
-      <c r="M26" s="281"/>
-      <c r="N26" s="282"/>
+      <c r="L26" s="284"/>
+      <c r="M26" s="284"/>
+      <c r="N26" s="285"/>
       <c r="R26" s="74" t="s">
         <v>421</v>
       </c>
@@ -10562,7 +10588,7 @@
     <col min="11" max="11" width="9.06640625" style="275"/>
     <col min="12" max="12" width="9.06640625" style="278"/>
     <col min="13" max="13" width="9.06640625" style="66"/>
-    <col min="14" max="14" width="9.06640625" style="310"/>
+    <col min="14" max="14" width="9.06640625" style="281"/>
     <col min="15" max="15" width="9.06640625" style="275"/>
     <col min="16" max="16" width="9.06640625" style="278"/>
     <col min="17" max="18" width="9.06640625" style="66"/>
@@ -10572,30 +10598,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="68"/>
       <c r="B1"/>
-      <c r="C1" s="283" t="s">
+      <c r="C1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="283" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="286" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="283" t="s">
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="286" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="283" t="s">
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="285"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="288"/>
     </row>
     <row r="2" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="68"/>
@@ -10684,12 +10710,12 @@
       <c r="P3" s="273"/>
       <c r="Q3" s="273"/>
       <c r="R3" s="277"/>
-      <c r="S3" s="288" t="s">
+      <c r="S3" s="291" t="s">
         <v>947</v>
       </c>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="289"/>
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="292"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="68" t="s">
@@ -10750,12 +10776,12 @@
       <c r="P5" s="273"/>
       <c r="Q5" s="273"/>
       <c r="R5" s="277"/>
-      <c r="S5" s="281" t="s">
+      <c r="S5" s="284" t="s">
         <v>873</v>
       </c>
-      <c r="T5" s="281"/>
-      <c r="U5" s="281"/>
-      <c r="V5" s="282"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="284"/>
+      <c r="V5" s="285"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="68" t="s">
@@ -10781,12 +10807,12 @@
       <c r="P6" s="273"/>
       <c r="Q6" s="273"/>
       <c r="R6" s="277"/>
-      <c r="S6" s="281" t="s">
+      <c r="S6" s="284" t="s">
         <v>948</v>
       </c>
-      <c r="T6" s="281"/>
-      <c r="U6" s="281"/>
-      <c r="V6" s="282"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="284"/>
+      <c r="V6" s="285"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="68" t="s">
@@ -10839,10 +10865,10 @@
       <c r="P8" s="273"/>
       <c r="Q8" s="273"/>
       <c r="R8" s="277"/>
-      <c r="S8" s="305"/>
-      <c r="T8" s="304"/>
-      <c r="U8" s="304"/>
-      <c r="V8" s="304"/>
+      <c r="S8" s="308"/>
+      <c r="T8" s="307"/>
+      <c r="U8" s="307"/>
+      <c r="V8" s="307"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="68" t="s">
@@ -11018,12 +11044,12 @@
       <c r="N15" s="269" t="s">
         <v>285</v>
       </c>
-      <c r="O15" s="306" t="s">
+      <c r="O15" s="309" t="s">
         <v>949</v>
       </c>
-      <c r="P15" s="293"/>
-      <c r="Q15" s="293"/>
-      <c r="R15" s="307"/>
+      <c r="P15" s="296"/>
+      <c r="Q15" s="296"/>
+      <c r="R15" s="310"/>
     </row>
     <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="68" t="s">
@@ -13042,39 +13068,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="308"/>
+      <c r="A1" s="279"/>
       <c r="B1" s="266"/>
-      <c r="C1" s="283" t="s">
+      <c r="C1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="283" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="286" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="283" t="s">
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="286" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="283" t="s">
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="285"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="288"/>
       <c r="S1" s="229"/>
       <c r="T1" s="229"/>
       <c r="U1" s="229"/>
       <c r="V1" s="229"/>
     </row>
     <row r="2" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="308"/>
+      <c r="A2" s="279"/>
       <c r="B2" s="266"/>
       <c r="C2" s="44" t="s">
         <v>926</v>
@@ -13130,7 +13156,7 @@
       <c r="V2" s="229"/>
     </row>
     <row r="3" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="308">
+      <c r="A3" s="279">
         <v>0</v>
       </c>
       <c r="B3" s="266" t="s">
@@ -13166,15 +13192,15 @@
       <c r="P3" s="224"/>
       <c r="Q3" s="224"/>
       <c r="R3" s="225"/>
-      <c r="S3" s="287" t="s">
+      <c r="S3" s="290" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="289"/>
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="292"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A4" s="308" t="s">
+      <c r="A4" s="279" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="266"/>
@@ -13210,7 +13236,7 @@
       <c r="V4" s="225"/>
     </row>
     <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A5" s="308" t="s">
+      <c r="A5" s="279" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="266"/>
@@ -13238,15 +13264,15 @@
       <c r="P5" s="224"/>
       <c r="Q5" s="224"/>
       <c r="R5" s="225"/>
-      <c r="S5" s="280" t="s">
+      <c r="S5" s="283" t="s">
         <v>282</v>
       </c>
-      <c r="T5" s="281"/>
-      <c r="U5" s="281"/>
-      <c r="V5" s="282"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="284"/>
+      <c r="V5" s="285"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A6" s="308" t="s">
+      <c r="A6" s="279" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="266"/>
@@ -13274,15 +13300,15 @@
       <c r="P6" s="224"/>
       <c r="Q6" s="224"/>
       <c r="R6" s="225"/>
-      <c r="S6" s="280" t="s">
+      <c r="S6" s="283" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="281"/>
-      <c r="U6" s="281"/>
-      <c r="V6" s="282"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="284"/>
+      <c r="V6" s="285"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A7" s="308" t="s">
+      <c r="A7" s="279" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="266"/>
@@ -13320,7 +13346,7 @@
       <c r="V7" s="225"/>
     </row>
     <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A8" s="308" t="s">
+      <c r="A8" s="279" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="266"/>
@@ -13347,15 +13373,15 @@
         <v>284</v>
       </c>
       <c r="R8" s="225"/>
-      <c r="S8" s="303" t="s">
+      <c r="S8" s="306" t="s">
         <v>955</v>
       </c>
-      <c r="T8" s="304"/>
-      <c r="U8" s="304"/>
-      <c r="V8" s="304"/>
+      <c r="T8" s="307"/>
+      <c r="U8" s="307"/>
+      <c r="V8" s="307"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A9" s="308" t="s">
+      <c r="A9" s="279" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="266" t="s">
@@ -13392,7 +13418,7 @@
       <c r="V9" s="229"/>
     </row>
     <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A10" s="308" t="s">
+      <c r="A10" s="279" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="266"/>
@@ -13432,7 +13458,7 @@
       <c r="V10" s="229"/>
     </row>
     <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A11" s="308" t="s">
+      <c r="A11" s="279" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="266"/>
@@ -13474,7 +13500,7 @@
       <c r="V11" s="229"/>
     </row>
     <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A12" s="308" t="s">
+      <c r="A12" s="279" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="266"/>
@@ -13514,7 +13540,7 @@
       <c r="V12" s="229"/>
     </row>
     <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A13" s="308" t="s">
+      <c r="A13" s="279" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="266"/>
@@ -13549,7 +13575,7 @@
       <c r="V13" s="229"/>
     </row>
     <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="308" t="s">
+      <c r="A14" s="279" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="266"/>
@@ -13583,7 +13609,7 @@
       <c r="V14" s="229"/>
     </row>
     <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="308" t="s">
+      <c r="A15" s="279" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="266"/>
@@ -13617,7 +13643,7 @@
       <c r="V15" s="229"/>
     </row>
     <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" s="308" t="s">
+      <c r="A16" s="279" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="266"/>
@@ -13651,7 +13677,7 @@
       <c r="V16" s="229"/>
     </row>
     <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A17" s="308" t="s">
+      <c r="A17" s="279" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="266"/>
@@ -13689,7 +13715,7 @@
       <c r="V17" s="229"/>
     </row>
     <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A18" s="308" t="s">
+      <c r="A18" s="279" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="266"/>
@@ -13730,7 +13756,7 @@
       <c r="V18" s="229"/>
     </row>
     <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A19" s="308" t="s">
+      <c r="A19" s="279" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="266"/>
@@ -13772,7 +13798,7 @@
       <c r="V19" s="229"/>
     </row>
     <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A20" s="308" t="s">
+      <c r="A20" s="279" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="266"/>
@@ -13812,7 +13838,7 @@
       <c r="V20" s="229"/>
     </row>
     <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A21" s="308" t="s">
+      <c r="A21" s="279" t="s">
         <v>97</v>
       </c>
       <c r="B21" s="266"/>
@@ -13849,7 +13875,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A22" s="308" t="s">
+      <c r="A22" s="279" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="266" t="s">
@@ -13889,7 +13915,7 @@
       <c r="V22" s="229"/>
     </row>
     <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A23" s="308" t="s">
+      <c r="A23" s="279" t="s">
         <v>101</v>
       </c>
       <c r="B23" s="266"/>
@@ -13931,7 +13957,7 @@
       <c r="V23" s="229"/>
     </row>
     <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A24" s="308" t="s">
+      <c r="A24" s="279" t="s">
         <v>103</v>
       </c>
       <c r="B24" s="266"/>
@@ -13973,7 +13999,7 @@
       <c r="V24" s="229"/>
     </row>
     <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A25" s="308" t="s">
+      <c r="A25" s="279" t="s">
         <v>105</v>
       </c>
       <c r="B25" s="266"/>
@@ -14013,7 +14039,7 @@
       <c r="V25" s="229"/>
     </row>
     <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A26" s="308" t="s">
+      <c r="A26" s="279" t="s">
         <v>111</v>
       </c>
       <c r="B26" s="266"/>
@@ -14048,7 +14074,7 @@
       <c r="V26" s="229"/>
     </row>
     <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A27" s="308" t="s">
+      <c r="A27" s="279" t="s">
         <v>112</v>
       </c>
       <c r="B27" s="266"/>
@@ -14076,7 +14102,7 @@
       <c r="V27" s="229"/>
     </row>
     <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A28" s="308" t="s">
+      <c r="A28" s="279" t="s">
         <v>113</v>
       </c>
       <c r="B28" s="266"/>
@@ -14106,7 +14132,7 @@
       <c r="V28" s="229"/>
     </row>
     <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A29" s="308" t="s">
+      <c r="A29" s="279" t="s">
         <v>162</v>
       </c>
       <c r="B29" s="266"/>
@@ -14136,7 +14162,7 @@
       <c r="V29" s="229"/>
     </row>
     <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A30" s="308" t="s">
+      <c r="A30" s="279" t="s">
         <v>163</v>
       </c>
       <c r="B30" s="266"/>
@@ -14170,7 +14196,7 @@
       <c r="V30" s="229"/>
     </row>
     <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A31" s="308" t="s">
+      <c r="A31" s="279" t="s">
         <v>164</v>
       </c>
       <c r="B31" s="266"/>
@@ -14208,7 +14234,7 @@
       <c r="V31" s="229"/>
     </row>
     <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A32" s="308" t="s">
+      <c r="A32" s="279" t="s">
         <v>165</v>
       </c>
       <c r="B32" s="266"/>
@@ -14245,7 +14271,7 @@
       <c r="V32" s="229"/>
     </row>
     <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A33" s="308" t="s">
+      <c r="A33" s="279" t="s">
         <v>166</v>
       </c>
       <c r="B33" s="266"/>
@@ -14282,7 +14308,7 @@
       <c r="V33" s="229"/>
     </row>
     <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A34" s="308" t="s">
+      <c r="A34" s="279" t="s">
         <v>167</v>
       </c>
       <c r="B34" s="266"/>
@@ -14312,7 +14338,7 @@
       <c r="V34" s="229"/>
     </row>
     <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A35" s="308" t="s">
+      <c r="A35" s="279" t="s">
         <v>168</v>
       </c>
       <c r="B35" s="266"/>
@@ -14337,7 +14363,7 @@
       <c r="V35" s="229"/>
     </row>
     <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A36" s="308" t="s">
+      <c r="A36" s="279" t="s">
         <v>169</v>
       </c>
       <c r="B36" s="266"/>
@@ -14361,7 +14387,7 @@
       <c r="V36" s="229"/>
     </row>
     <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A37" s="308" t="s">
+      <c r="A37" s="279" t="s">
         <v>170</v>
       </c>
       <c r="B37" s="266"/>
@@ -14385,7 +14411,7 @@
       <c r="V37" s="229"/>
     </row>
     <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A38" s="308" t="s">
+      <c r="A38" s="279" t="s">
         <v>171</v>
       </c>
       <c r="B38" s="266"/>
@@ -14412,7 +14438,7 @@
       <c r="V38" s="229"/>
     </row>
     <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A39" s="308" t="s">
+      <c r="A39" s="279" t="s">
         <v>334</v>
       </c>
       <c r="B39" s="266"/>
@@ -14442,7 +14468,7 @@
       <c r="V39" s="229"/>
     </row>
     <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A40" s="308" t="s">
+      <c r="A40" s="279" t="s">
         <v>335</v>
       </c>
       <c r="B40" s="266"/>
@@ -14474,7 +14500,7 @@
       <c r="V40" s="229"/>
     </row>
     <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A41" s="308" t="s">
+      <c r="A41" s="279" t="s">
         <v>336</v>
       </c>
       <c r="B41" s="266"/>
@@ -14504,7 +14530,7 @@
       <c r="V41" s="229"/>
     </row>
     <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A42" s="308" t="s">
+      <c r="A42" s="279" t="s">
         <v>337</v>
       </c>
       <c r="B42" s="266"/>
@@ -14530,7 +14556,7 @@
       <c r="V42" s="229"/>
     </row>
     <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A43" s="308" t="s">
+      <c r="A43" s="279" t="s">
         <v>338</v>
       </c>
       <c r="B43" s="266"/>
@@ -14556,7 +14582,7 @@
       <c r="V43" s="229"/>
     </row>
     <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A44" s="308" t="s">
+      <c r="A44" s="279" t="s">
         <v>339</v>
       </c>
       <c r="B44" s="266"/>
@@ -14583,7 +14609,7 @@
       <c r="V44" s="229"/>
     </row>
     <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A45" s="308" t="s">
+      <c r="A45" s="279" t="s">
         <v>340</v>
       </c>
       <c r="B45" s="266"/>
@@ -14611,7 +14637,7 @@
       <c r="V45" s="229"/>
     </row>
     <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A46" s="308" t="s">
+      <c r="A46" s="279" t="s">
         <v>341</v>
       </c>
       <c r="B46" s="266"/>
@@ -14637,7 +14663,7 @@
       <c r="V46" s="229"/>
     </row>
     <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A47" s="308" t="s">
+      <c r="A47" s="279" t="s">
         <v>342</v>
       </c>
       <c r="B47" s="266"/>
@@ -14660,7 +14686,7 @@
       <c r="V47" s="229"/>
     </row>
     <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A48" s="308" t="s">
+      <c r="A48" s="279" t="s">
         <v>343</v>
       </c>
       <c r="B48" s="266"/>
@@ -14684,7 +14710,7 @@
       <c r="V48" s="229"/>
     </row>
     <row r="49" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A49" s="308" t="s">
+      <c r="A49" s="279" t="s">
         <v>344</v>
       </c>
       <c r="B49" s="266"/>
@@ -14708,7 +14734,7 @@
       <c r="V49" s="229"/>
     </row>
     <row r="50" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A50" s="308" t="s">
+      <c r="A50" s="279" t="s">
         <v>345</v>
       </c>
       <c r="B50" s="266"/>
@@ -14732,7 +14758,7 @@
       <c r="V50" s="229"/>
     </row>
     <row r="51" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A51" s="308" t="s">
+      <c r="A51" s="279" t="s">
         <v>346</v>
       </c>
       <c r="B51" s="266"/>
@@ -14755,7 +14781,7 @@
       <c r="V51" s="229"/>
     </row>
     <row r="52" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A52" s="308" t="s">
+      <c r="A52" s="279" t="s">
         <v>347</v>
       </c>
       <c r="B52" s="266"/>
@@ -14778,7 +14804,7 @@
       <c r="V52" s="229"/>
     </row>
     <row r="53" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A53" s="308" t="s">
+      <c r="A53" s="279" t="s">
         <v>348</v>
       </c>
       <c r="B53" s="266"/>
@@ -14802,7 +14828,7 @@
       <c r="V53" s="229"/>
     </row>
     <row r="54" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A54" s="308" t="s">
+      <c r="A54" s="279" t="s">
         <v>349</v>
       </c>
       <c r="B54" s="266"/>
@@ -14826,7 +14852,7 @@
       <c r="V54" s="229"/>
     </row>
     <row r="55" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A55" s="308" t="s">
+      <c r="A55" s="279" t="s">
         <v>350</v>
       </c>
       <c r="B55" s="266"/>
@@ -14850,7 +14876,7 @@
       <c r="V55" s="229"/>
     </row>
     <row r="56" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A56" s="308" t="s">
+      <c r="A56" s="279" t="s">
         <v>351</v>
       </c>
       <c r="B56" s="266"/>
@@ -14874,7 +14900,7 @@
       <c r="V56" s="229"/>
     </row>
     <row r="57" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A57" s="308" t="s">
+      <c r="A57" s="279" t="s">
         <v>352</v>
       </c>
       <c r="B57" s="266"/>
@@ -14897,7 +14923,7 @@
       <c r="V57" s="229"/>
     </row>
     <row r="58" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A58" s="308" t="s">
+      <c r="A58" s="279" t="s">
         <v>353</v>
       </c>
       <c r="B58" s="266"/>
@@ -14920,7 +14946,7 @@
       <c r="V58" s="229"/>
     </row>
     <row r="59" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A59" s="308" t="s">
+      <c r="A59" s="279" t="s">
         <v>354</v>
       </c>
       <c r="B59" s="266"/>
@@ -14944,7 +14970,7 @@
       <c r="V59" s="229"/>
     </row>
     <row r="60" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A60" s="308" t="s">
+      <c r="A60" s="279" t="s">
         <v>355</v>
       </c>
       <c r="B60" s="266"/>
@@ -14968,7 +14994,7 @@
       <c r="V60" s="229"/>
     </row>
     <row r="61" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A61" s="308" t="s">
+      <c r="A61" s="279" t="s">
         <v>356</v>
       </c>
       <c r="B61" s="266"/>
@@ -14992,7 +15018,7 @@
       <c r="V61" s="229"/>
     </row>
     <row r="62" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A62" s="308" t="s">
+      <c r="A62" s="279" t="s">
         <v>357</v>
       </c>
       <c r="B62" s="266"/>
@@ -15016,7 +15042,7 @@
       <c r="V62" s="229"/>
     </row>
     <row r="63" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A63" s="308" t="s">
+      <c r="A63" s="279" t="s">
         <v>358</v>
       </c>
       <c r="B63" s="266"/>
@@ -15040,7 +15066,7 @@
       <c r="V63" s="229"/>
     </row>
     <row r="64" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A64" s="308" t="s">
+      <c r="A64" s="279" t="s">
         <v>359</v>
       </c>
       <c r="B64" s="266"/>
@@ -15064,7 +15090,7 @@
       <c r="V64" s="229"/>
     </row>
     <row r="65" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A65" s="308" t="s">
+      <c r="A65" s="279" t="s">
         <v>360</v>
       </c>
       <c r="B65" s="266"/>
@@ -15087,7 +15113,7 @@
       <c r="V65" s="229"/>
     </row>
     <row r="66" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A66" s="308" t="s">
+      <c r="A66" s="279" t="s">
         <v>361</v>
       </c>
       <c r="B66" s="266"/>
@@ -15111,7 +15137,7 @@
       <c r="V66" s="229"/>
     </row>
     <row r="67" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A67" s="308" t="s">
+      <c r="A67" s="279" t="s">
         <v>362</v>
       </c>
       <c r="B67" s="266"/>
@@ -15135,7 +15161,7 @@
       <c r="V67" s="229"/>
     </row>
     <row r="68" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A68" s="308" t="s">
+      <c r="A68" s="279" t="s">
         <v>363</v>
       </c>
       <c r="B68" s="266"/>
@@ -15159,7 +15185,7 @@
       <c r="V68" s="229"/>
     </row>
     <row r="69" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A69" s="308" t="s">
+      <c r="A69" s="279" t="s">
         <v>364</v>
       </c>
       <c r="B69" s="266"/>
@@ -15183,7 +15209,7 @@
       <c r="V69" s="229"/>
     </row>
     <row r="70" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A70" s="308" t="s">
+      <c r="A70" s="279" t="s">
         <v>365</v>
       </c>
       <c r="B70" s="266"/>
@@ -15206,7 +15232,7 @@
       <c r="V70" s="229"/>
     </row>
     <row r="71" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A71" s="308" t="s">
+      <c r="A71" s="279" t="s">
         <v>366</v>
       </c>
       <c r="B71" s="266"/>
@@ -15229,7 +15255,7 @@
       <c r="V71" s="229"/>
     </row>
     <row r="72" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A72" s="308" t="s">
+      <c r="A72" s="279" t="s">
         <v>368</v>
       </c>
       <c r="B72" s="266"/>
@@ -15253,7 +15279,7 @@
       <c r="V72" s="229"/>
     </row>
     <row r="73" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A73" s="308" t="s">
+      <c r="A73" s="279" t="s">
         <v>369</v>
       </c>
       <c r="B73" s="266"/>
@@ -15277,7 +15303,7 @@
       <c r="V73" s="229"/>
     </row>
     <row r="74" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A74" s="308" t="s">
+      <c r="A74" s="279" t="s">
         <v>370</v>
       </c>
       <c r="B74" s="266"/>
@@ -15301,7 +15327,7 @@
       <c r="V74" s="229"/>
     </row>
     <row r="75" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A75" s="308" t="s">
+      <c r="A75" s="279" t="s">
         <v>371</v>
       </c>
       <c r="B75" s="266"/>
@@ -15325,7 +15351,7 @@
       <c r="V75" s="229"/>
     </row>
     <row r="76" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A76" s="308" t="s">
+      <c r="A76" s="279" t="s">
         <v>372</v>
       </c>
       <c r="B76" s="266"/>
@@ -15349,7 +15375,7 @@
       <c r="V76" s="229"/>
     </row>
     <row r="77" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A77" s="308" t="s">
+      <c r="A77" s="279" t="s">
         <v>373</v>
       </c>
       <c r="B77" s="266"/>
@@ -15372,7 +15398,7 @@
       <c r="V77" s="229"/>
     </row>
     <row r="78" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A78" s="308" t="s">
+      <c r="A78" s="279" t="s">
         <v>374</v>
       </c>
       <c r="B78" s="266"/>
@@ -15395,7 +15421,7 @@
       <c r="V78" s="229"/>
     </row>
     <row r="79" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A79" s="308" t="s">
+      <c r="A79" s="279" t="s">
         <v>375</v>
       </c>
       <c r="B79" s="266"/>
@@ -15419,7 +15445,7 @@
       <c r="V79" s="229"/>
     </row>
     <row r="80" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A80" s="308" t="s">
+      <c r="A80" s="279" t="s">
         <v>376</v>
       </c>
       <c r="B80" s="266"/>
@@ -15443,7 +15469,7 @@
       <c r="V80" s="229"/>
     </row>
     <row r="81" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A81" s="308"/>
+      <c r="A81" s="279"/>
       <c r="B81" s="266"/>
       <c r="C81" s="223"/>
       <c r="D81" s="224"/>
@@ -15465,7 +15491,7 @@
       <c r="V81" s="229"/>
     </row>
     <row r="82" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A82" s="308"/>
+      <c r="A82" s="279"/>
       <c r="B82" s="266"/>
       <c r="C82" s="99"/>
       <c r="D82" s="224"/>
@@ -15487,7 +15513,7 @@
       <c r="V82" s="229"/>
     </row>
     <row r="83" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A83" s="308"/>
+      <c r="A83" s="279"/>
       <c r="B83" s="266"/>
       <c r="C83" s="99"/>
       <c r="E83" s="224"/>
@@ -15508,7 +15534,7 @@
       <c r="V83" s="229"/>
     </row>
     <row r="84" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A84" s="308"/>
+      <c r="A84" s="279"/>
       <c r="B84" s="266"/>
       <c r="C84" s="228"/>
       <c r="E84" s="32"/>
@@ -15529,7 +15555,7 @@
       <c r="V84" s="229"/>
     </row>
     <row r="85" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A85" s="308"/>
+      <c r="A85" s="279"/>
       <c r="B85" s="266"/>
       <c r="C85" s="228"/>
       <c r="E85" s="32"/>
@@ -15551,7 +15577,7 @@
       <c r="V85" s="229"/>
     </row>
     <row r="86" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A86" s="308"/>
+      <c r="A86" s="279"/>
       <c r="B86" s="266"/>
       <c r="C86" s="228"/>
       <c r="E86" s="32"/>
@@ -15573,7 +15599,7 @@
       <c r="V86" s="229"/>
     </row>
     <row r="87" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A87" s="308"/>
+      <c r="A87" s="279"/>
       <c r="B87" s="266"/>
       <c r="C87" s="228"/>
       <c r="E87" s="32"/>
@@ -15595,7 +15621,7 @@
       <c r="V87" s="229"/>
     </row>
     <row r="88" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A88" s="308"/>
+      <c r="A88" s="279"/>
       <c r="B88" s="266"/>
       <c r="C88" s="228"/>
       <c r="E88" s="32"/>
@@ -15617,7 +15643,7 @@
       <c r="V88" s="229"/>
     </row>
     <row r="89" spans="1:22" ht="15" x14ac:dyDescent="0.4">
-      <c r="A89" s="308"/>
+      <c r="A89" s="279"/>
       <c r="B89" s="266"/>
       <c r="C89" s="228"/>
       <c r="E89" s="32"/>
@@ -15684,30 +15710,30 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="68"/>
-      <c r="C1" s="283" t="s">
+      <c r="C1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="283" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="286" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="283" t="s">
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="286" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="283" t="s">
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="285"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="288"/>
       <c r="S1" s="45"/>
       <c r="T1" s="45"/>
       <c r="U1" s="45"/>
@@ -15805,12 +15831,12 @@
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="287" t="s">
+      <c r="S3" s="290" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="289"/>
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="292"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="68" t="s">
@@ -15875,12 +15901,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="280" t="s">
+      <c r="S5" s="283" t="s">
         <v>282</v>
       </c>
-      <c r="T5" s="281"/>
-      <c r="U5" s="281"/>
-      <c r="V5" s="282"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="284"/>
+      <c r="V5" s="285"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="68" t="s">
@@ -15910,12 +15936,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="280" t="s">
+      <c r="S6" s="283" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="281"/>
-      <c r="U6" s="281"/>
-      <c r="V6" s="282"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="284"/>
+      <c r="V6" s="285"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="68" t="s">
@@ -15982,12 +16008,12 @@
         <v>284</v>
       </c>
       <c r="R8" s="41"/>
-      <c r="S8" s="303" t="s">
+      <c r="S8" s="306" t="s">
         <v>378</v>
       </c>
-      <c r="T8" s="304"/>
-      <c r="U8" s="304"/>
-      <c r="V8" s="304"/>
+      <c r="T8" s="307"/>
+      <c r="U8" s="307"/>
+      <c r="V8" s="307"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="68" t="s">
@@ -18471,36 +18497,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="283" t="s">
+      <c r="C1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="286" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="284"/>
-      <c r="K1" s="283" t="s">
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="286" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="284"/>
-      <c r="M1" s="284"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="283" t="s">
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="286" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="284"/>
-      <c r="R1" s="285"/>
-      <c r="Z1" s="283" t="s">
+      <c r="P1" s="287"/>
+      <c r="Q1" s="287"/>
+      <c r="R1" s="288"/>
+      <c r="Z1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="284"/>
-      <c r="AB1" s="284"/>
-      <c r="AC1" s="285"/>
+      <c r="AA1" s="287"/>
+      <c r="AB1" s="287"/>
+      <c r="AC1" s="288"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -18569,33 +18595,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="287" t="s">
+      <c r="C3" s="290" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="287"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="289"/>
+      <c r="D3" s="291"/>
+      <c r="E3" s="291"/>
+      <c r="F3" s="292"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="291"/>
+      <c r="I3" s="291"/>
+      <c r="J3" s="292"/>
       <c r="K3" s="223"/>
       <c r="O3" s="223"/>
       <c r="P3" s="224"/>
       <c r="Q3" s="224"/>
       <c r="R3" s="225"/>
-      <c r="S3" s="287" t="s">
+      <c r="S3" s="290" t="s">
         <v>402</v>
       </c>
-      <c r="T3" s="288"/>
-      <c r="U3" s="288"/>
-      <c r="V3" s="289"/>
-      <c r="Z3" s="287" t="s">
+      <c r="T3" s="291"/>
+      <c r="U3" s="291"/>
+      <c r="V3" s="292"/>
+      <c r="Z3" s="290" t="s">
         <v>265</v>
       </c>
-      <c r="AA3" s="288"/>
-      <c r="AB3" s="288"/>
-      <c r="AC3" s="289"/>
+      <c r="AA3" s="291"/>
+      <c r="AB3" s="291"/>
+      <c r="AC3" s="292"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -18652,12 +18678,12 @@
       <c r="P5" s="224"/>
       <c r="Q5" s="224"/>
       <c r="R5" s="225"/>
-      <c r="S5" s="280" t="s">
+      <c r="S5" s="283" t="s">
         <v>502</v>
       </c>
-      <c r="T5" s="281"/>
-      <c r="U5" s="281"/>
-      <c r="V5" s="282"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="284"/>
+      <c r="V5" s="285"/>
       <c r="W5" s="84" t="s">
         <v>504</v>
       </c>
@@ -18687,12 +18713,12 @@
       <c r="P6" s="224"/>
       <c r="Q6" s="224"/>
       <c r="R6" s="225"/>
-      <c r="S6" s="280" t="s">
+      <c r="S6" s="283" t="s">
         <v>419</v>
       </c>
-      <c r="T6" s="281"/>
-      <c r="U6" s="281"/>
-      <c r="V6" s="282"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="284"/>
+      <c r="V6" s="285"/>
       <c r="Z6" s="223"/>
       <c r="AA6" s="224"/>
       <c r="AB6" s="224"/>
@@ -20092,30 +20118,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="21"/>
-      <c r="B1" s="283" t="s">
+      <c r="B1" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="286" t="s">
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="284"/>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="283" t="s">
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="286" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="284"/>
-      <c r="L1" s="284"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="283" t="s">
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="284"/>
-      <c r="P1" s="284"/>
-      <c r="Q1" s="285"/>
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
+      <c r="Q1" s="288"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
@@ -20202,12 +20228,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="287" t="s">
+      <c r="R3" s="290" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="288"/>
-      <c r="T3" s="288"/>
-      <c r="U3" s="289"/>
+      <c r="S3" s="291"/>
+      <c r="T3" s="291"/>
+      <c r="U3" s="292"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="39" t="s">
@@ -20260,12 +20286,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="280" t="s">
+      <c r="R5" s="283" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="281"/>
-      <c r="T5" s="281"/>
-      <c r="U5" s="282"/>
+      <c r="S5" s="284"/>
+      <c r="T5" s="284"/>
+      <c r="U5" s="285"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
@@ -20287,12 +20313,12 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="34"/>
-      <c r="R6" s="280" t="s">
+      <c r="R6" s="283" t="s">
         <v>262</v>
       </c>
-      <c r="S6" s="281"/>
-      <c r="T6" s="281"/>
-      <c r="U6" s="282"/>
+      <c r="S6" s="284"/>
+      <c r="T6" s="284"/>
+      <c r="U6" s="285"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="39" t="s">
@@ -23752,67 +23778,67 @@
       </c>
     </row>
     <row r="6" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="290" t="s">
+      <c r="B6" s="293" t="s">
         <v>514</v>
       </c>
-      <c r="C6" s="291"/>
-      <c r="D6" s="292"/>
-      <c r="E6" s="290" t="s">
+      <c r="C6" s="294"/>
+      <c r="D6" s="295"/>
+      <c r="E6" s="293" t="s">
         <v>515</v>
       </c>
-      <c r="F6" s="291"/>
-      <c r="G6" s="292"/>
+      <c r="F6" s="294"/>
+      <c r="G6" s="295"/>
     </row>
     <row r="7" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="290" t="s">
+      <c r="B7" s="293" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="291"/>
-      <c r="D7" s="291"/>
-      <c r="E7" s="291"/>
-      <c r="F7" s="291"/>
-      <c r="G7" s="291"/>
-      <c r="H7" s="291"/>
-      <c r="I7" s="291"/>
-      <c r="J7" s="291"/>
-      <c r="K7" s="291"/>
-      <c r="L7" s="291"/>
-      <c r="M7" s="291"/>
-      <c r="N7" s="291"/>
-      <c r="O7" s="291"/>
-      <c r="P7" s="292"/>
-      <c r="Q7" s="290" t="s">
+      <c r="C7" s="294"/>
+      <c r="D7" s="294"/>
+      <c r="E7" s="294"/>
+      <c r="F7" s="294"/>
+      <c r="G7" s="294"/>
+      <c r="H7" s="294"/>
+      <c r="I7" s="294"/>
+      <c r="J7" s="294"/>
+      <c r="K7" s="294"/>
+      <c r="L7" s="294"/>
+      <c r="M7" s="294"/>
+      <c r="N7" s="294"/>
+      <c r="O7" s="294"/>
+      <c r="P7" s="295"/>
+      <c r="Q7" s="293" t="s">
         <v>215</v>
       </c>
-      <c r="R7" s="291"/>
-      <c r="S7" s="291"/>
-      <c r="T7" s="291"/>
-      <c r="U7" s="291"/>
-      <c r="V7" s="291"/>
-      <c r="W7" s="291"/>
-      <c r="X7" s="291"/>
-      <c r="Y7" s="291"/>
-      <c r="Z7" s="291"/>
-      <c r="AA7" s="292"/>
-      <c r="AB7" s="290" t="s">
+      <c r="R7" s="294"/>
+      <c r="S7" s="294"/>
+      <c r="T7" s="294"/>
+      <c r="U7" s="294"/>
+      <c r="V7" s="294"/>
+      <c r="W7" s="294"/>
+      <c r="X7" s="294"/>
+      <c r="Y7" s="294"/>
+      <c r="Z7" s="294"/>
+      <c r="AA7" s="295"/>
+      <c r="AB7" s="293" t="s">
         <v>216</v>
       </c>
-      <c r="AC7" s="291"/>
-      <c r="AD7" s="291"/>
-      <c r="AE7" s="291"/>
-      <c r="AF7" s="291"/>
-      <c r="AG7" s="291"/>
-      <c r="AH7" s="291"/>
-      <c r="AI7" s="291"/>
-      <c r="AJ7" s="291"/>
-      <c r="AK7" s="291"/>
-      <c r="AL7" s="291"/>
-      <c r="AM7" s="291"/>
-      <c r="AN7" s="291"/>
-      <c r="AO7" s="291"/>
-      <c r="AP7" s="291"/>
-      <c r="AQ7" s="291"/>
-      <c r="AR7" s="292"/>
+      <c r="AC7" s="294"/>
+      <c r="AD7" s="294"/>
+      <c r="AE7" s="294"/>
+      <c r="AF7" s="294"/>
+      <c r="AG7" s="294"/>
+      <c r="AH7" s="294"/>
+      <c r="AI7" s="294"/>
+      <c r="AJ7" s="294"/>
+      <c r="AK7" s="294"/>
+      <c r="AL7" s="294"/>
+      <c r="AM7" s="294"/>
+      <c r="AN7" s="294"/>
+      <c r="AO7" s="294"/>
+      <c r="AP7" s="294"/>
+      <c r="AQ7" s="294"/>
+      <c r="AR7" s="295"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.4">
       <c r="E9" s="45"/>
@@ -23886,18 +23912,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B1" s="279" t="s">
+      <c r="B1" s="282" t="s">
         <v>680</v>
       </c>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="282"/>
+      <c r="I1" s="282"/>
+      <c r="J1" s="282"/>
+      <c r="K1" s="282"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
@@ -25021,7 +25047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431E16EB-4173-4BB0-A744-4BFFE60D57DA}">
   <dimension ref="A1:BA82"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B79" sqref="B79"/>
     </sheetView>
@@ -25068,11 +25094,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D1" s="287" t="s">
+      <c r="D1" s="290" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
       <c r="G1" s="63"/>
       <c r="H1" s="59"/>
       <c r="I1" s="92"/>
@@ -25130,12 +25156,12 @@
     </row>
     <row r="5" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="283" t="s">
+      <c r="D6" s="286" t="s">
         <v>619</v>
       </c>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="285"/>
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="288"/>
       <c r="H6" s="122"/>
       <c r="I6" s="94"/>
       <c r="J6" s="94"/>
@@ -25144,27 +25170,27 @@
       <c r="M6" s="94"/>
       <c r="N6" s="94"/>
       <c r="O6" s="94"/>
-      <c r="P6" s="283" t="s">
+      <c r="P6" s="286" t="s">
         <v>620</v>
       </c>
-      <c r="Q6" s="284"/>
-      <c r="R6" s="284"/>
-      <c r="S6" s="285"/>
-      <c r="AF6" s="283" t="s">
+      <c r="Q6" s="287"/>
+      <c r="R6" s="287"/>
+      <c r="S6" s="288"/>
+      <c r="AF6" s="286" t="s">
         <v>1</v>
       </c>
-      <c r="AG6" s="284"/>
-      <c r="AH6" s="284"/>
-      <c r="AI6" s="285"/>
+      <c r="AG6" s="287"/>
+      <c r="AH6" s="287"/>
+      <c r="AI6" s="288"/>
       <c r="AJ6" s="153"/>
-      <c r="AK6" s="283" t="s">
+      <c r="AK6" s="286" t="s">
         <v>618</v>
       </c>
-      <c r="AL6" s="284"/>
-      <c r="AM6" s="284"/>
-      <c r="AN6" s="284"/>
-      <c r="AO6" s="284"/>
-      <c r="AP6" s="285"/>
+      <c r="AL6" s="287"/>
+      <c r="AM6" s="287"/>
+      <c r="AN6" s="287"/>
+      <c r="AO6" s="287"/>
+      <c r="AP6" s="288"/>
     </row>
     <row r="7" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D7" s="35" t="s">
@@ -25242,11 +25268,11 @@
       <c r="J8" s="94"/>
       <c r="K8" s="94"/>
       <c r="L8" s="94"/>
-      <c r="M8" s="294" t="s">
+      <c r="M8" s="297" t="s">
         <v>526</v>
       </c>
-      <c r="N8" s="294"/>
-      <c r="O8" s="294"/>
+      <c r="N8" s="297"/>
+      <c r="O8" s="297"/>
       <c r="P8" s="118"/>
       <c r="Q8" s="119"/>
       <c r="R8" s="119"/>
@@ -25267,12 +25293,12 @@
       <c r="AL8" s="154"/>
       <c r="AM8" s="154"/>
       <c r="AN8" s="154"/>
-      <c r="AQ8" s="280" t="s">
+      <c r="AQ8" s="283" t="s">
         <v>19</v>
       </c>
-      <c r="AR8" s="281"/>
-      <c r="AS8" s="281"/>
-      <c r="AT8" s="282"/>
+      <c r="AR8" s="284"/>
+      <c r="AS8" s="284"/>
+      <c r="AT8" s="285"/>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D9" s="40"/>
@@ -25284,11 +25310,11 @@
       <c r="J9" s="121"/>
       <c r="K9" s="121"/>
       <c r="L9" s="121"/>
-      <c r="M9" s="296" t="s">
+      <c r="M9" s="299" t="s">
         <v>527</v>
       </c>
-      <c r="N9" s="296"/>
-      <c r="O9" s="295"/>
+      <c r="N9" s="299"/>
+      <c r="O9" s="298"/>
       <c r="P9" s="118"/>
       <c r="Q9" s="119"/>
       <c r="R9" s="119"/>
@@ -25330,9 +25356,9 @@
       <c r="J10" s="121"/>
       <c r="K10" s="121"/>
       <c r="L10" s="121"/>
-      <c r="M10" s="293"/>
-      <c r="N10" s="293"/>
-      <c r="O10" s="293"/>
+      <c r="M10" s="296"/>
+      <c r="N10" s="296"/>
+      <c r="O10" s="296"/>
       <c r="P10" s="118"/>
       <c r="Q10" s="119"/>
       <c r="R10" s="119"/>
@@ -25357,12 +25383,12 @@
       <c r="AL10" s="154"/>
       <c r="AM10" s="154"/>
       <c r="AN10" s="154"/>
-      <c r="AQ10" s="280" t="s">
+      <c r="AQ10" s="283" t="s">
         <v>54</v>
       </c>
-      <c r="AR10" s="281"/>
-      <c r="AS10" s="281"/>
-      <c r="AT10" s="282"/>
+      <c r="AR10" s="284"/>
+      <c r="AS10" s="284"/>
+      <c r="AT10" s="285"/>
     </row>
     <row r="11" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="40"/>
@@ -25398,12 +25424,12 @@
       <c r="AL11" s="154"/>
       <c r="AM11" s="154"/>
       <c r="AN11" s="154"/>
-      <c r="AQ11" s="280" t="s">
+      <c r="AQ11" s="283" t="s">
         <v>617</v>
       </c>
-      <c r="AR11" s="281"/>
-      <c r="AS11" s="281"/>
-      <c r="AT11" s="282"/>
+      <c r="AR11" s="284"/>
+      <c r="AS11" s="284"/>
+      <c r="AT11" s="285"/>
       <c r="AU11" s="26" t="s">
         <v>263</v>
       </c>
@@ -25429,11 +25455,11 @@
       <c r="J12" s="94"/>
       <c r="K12" s="94"/>
       <c r="L12" s="94"/>
-      <c r="M12" s="297" t="s">
+      <c r="M12" s="300" t="s">
         <v>525</v>
       </c>
-      <c r="N12" s="297"/>
-      <c r="O12" s="297"/>
+      <c r="N12" s="300"/>
+      <c r="O12" s="300"/>
       <c r="P12" s="118"/>
       <c r="Q12" s="119"/>
       <c r="R12" s="119"/>
@@ -25447,12 +25473,12 @@
       <c r="AL12" s="154"/>
       <c r="AM12" s="154"/>
       <c r="AN12" s="154"/>
-      <c r="AQ12" s="280" t="s">
+      <c r="AQ12" s="283" t="s">
         <v>524</v>
       </c>
-      <c r="AR12" s="281"/>
-      <c r="AS12" s="281"/>
-      <c r="AT12" s="282"/>
+      <c r="AR12" s="284"/>
+      <c r="AS12" s="284"/>
+      <c r="AT12" s="285"/>
       <c r="AV12" s="21" t="s">
         <v>613</v>
       </c>
@@ -25468,12 +25494,12 @@
         <v>520</v>
       </c>
       <c r="C13" s="131"/>
-      <c r="D13" s="283" t="s">
+      <c r="D13" s="286" t="s">
         <v>528</v>
       </c>
-      <c r="E13" s="284"/>
-      <c r="F13" s="284"/>
-      <c r="G13" s="284"/>
+      <c r="E13" s="287"/>
+      <c r="F13" s="287"/>
+      <c r="G13" s="287"/>
       <c r="H13" s="167" t="s">
         <v>631</v>
       </c>
@@ -25496,11 +25522,11 @@
       <c r="O13" s="180" t="s">
         <v>635</v>
       </c>
-      <c r="P13" s="283" t="s">
+      <c r="P13" s="286" t="s">
         <v>529</v>
       </c>
-      <c r="Q13" s="284"/>
-      <c r="R13" s="284"/>
+      <c r="Q13" s="287"/>
+      <c r="R13" s="287"/>
       <c r="S13" s="156"/>
       <c r="T13" s="170" t="s">
         <v>656</v>
@@ -25536,18 +25562,18 @@
       <c r="AH13" s="59"/>
       <c r="AI13" s="43"/>
       <c r="AJ13" s="153"/>
-      <c r="AK13" s="280" t="s">
+      <c r="AK13" s="283" t="s">
         <v>528</v>
       </c>
-      <c r="AL13" s="281"/>
-      <c r="AM13" s="281"/>
-      <c r="AN13" s="281"/>
-      <c r="AQ13" s="280" t="s">
+      <c r="AL13" s="284"/>
+      <c r="AM13" s="284"/>
+      <c r="AN13" s="284"/>
+      <c r="AQ13" s="283" t="s">
         <v>610</v>
       </c>
-      <c r="AR13" s="279"/>
-      <c r="AS13" s="279"/>
-      <c r="AT13" s="279"/>
+      <c r="AR13" s="282"/>
+      <c r="AS13" s="282"/>
+      <c r="AT13" s="282"/>
       <c r="AV13" s="21" t="s">
         <v>614</v>
       </c>
@@ -26239,8 +26265,8 @@
       </c>
       <c r="AO30" s="159"/>
       <c r="AP30" s="161"/>
-      <c r="AR30" s="295"/>
-      <c r="AS30" s="295"/>
+      <c r="AR30" s="298"/>
+      <c r="AS30" s="298"/>
     </row>
     <row r="31" spans="1:52" s="26" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="199" t="s">
@@ -26693,8 +26719,8 @@
         <v>88</v>
       </c>
       <c r="AO40" s="159"/>
-      <c r="AR40" s="293"/>
-      <c r="AS40" s="293"/>
+      <c r="AR40" s="296"/>
+      <c r="AS40" s="296"/>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A41" s="151" t="s">
@@ -26928,8 +26954,8 @@
         <v>633</v>
       </c>
       <c r="AP46" s="161"/>
-      <c r="AR46" s="293"/>
-      <c r="AS46" s="293"/>
+      <c r="AR46" s="296"/>
+      <c r="AS46" s="296"/>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A47" s="151" t="s">
@@ -27014,12 +27040,12 @@
         <v>522</v>
       </c>
       <c r="C49" s="178"/>
-      <c r="D49" s="283" t="s">
+      <c r="D49" s="286" t="s">
         <v>528</v>
       </c>
-      <c r="E49" s="284"/>
-      <c r="F49" s="284"/>
-      <c r="G49" s="284"/>
+      <c r="E49" s="287"/>
+      <c r="F49" s="287"/>
+      <c r="G49" s="287"/>
       <c r="H49" s="167" t="s">
         <v>631</v>
       </c>
@@ -27042,11 +27068,11 @@
       <c r="O49" s="180" t="s">
         <v>635</v>
       </c>
-      <c r="P49" s="283" t="s">
+      <c r="P49" s="286" t="s">
         <v>529</v>
       </c>
-      <c r="Q49" s="284"/>
-      <c r="R49" s="284"/>
+      <c r="Q49" s="287"/>
+      <c r="R49" s="287"/>
       <c r="S49" s="189"/>
       <c r="T49" s="170" t="s">
         <v>656</v>
@@ -28407,11 +28433,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43FEDAF-23E6-469D-8A80-8AB9F6CCCBDB}">
-  <dimension ref="A1:AU188"/>
+  <dimension ref="A1:AU189"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P57" sqref="P57:Q60"/>
+      <selection pane="topRight" activeCell="D187" sqref="D187:D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -28420,7 +28446,7 @@
     <col min="2" max="2" width="9.06640625" style="4"/>
     <col min="3" max="4" width="9.06640625" style="5"/>
     <col min="5" max="5" width="9.06640625" style="6"/>
-    <col min="10" max="10" width="9.06640625" style="4"/>
+    <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.06640625" style="5"/>
     <col min="12" max="12" width="10.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.46484375" style="6" bestFit="1" customWidth="1"/>
@@ -28455,17 +28481,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.4">
-      <c r="B1" s="287" t="s">
+      <c r="B1" s="290" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
       <c r="E1" s="42"/>
-      <c r="F1" s="287" t="s">
+      <c r="F1" s="290" t="s">
         <v>958</v>
       </c>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
       <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.4">
@@ -28508,61 +28534,61 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="298" t="s">
+      <c r="B4" s="301" t="s">
         <v>957</v>
       </c>
-      <c r="C4" s="299"/>
-      <c r="D4" s="299"/>
-      <c r="E4" s="300"/>
-      <c r="F4" s="298" t="s">
+      <c r="C4" s="302"/>
+      <c r="D4" s="302"/>
+      <c r="E4" s="303"/>
+      <c r="F4" s="301" t="s">
         <v>282</v>
       </c>
-      <c r="G4" s="299"/>
-      <c r="H4" s="299"/>
-      <c r="I4" s="300"/>
+      <c r="G4" s="302"/>
+      <c r="H4" s="302"/>
+      <c r="I4" s="303"/>
     </row>
     <row r="5" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="280" t="s">
+      <c r="B5" s="283" t="s">
         <v>869</v>
       </c>
-      <c r="C5" s="281"/>
-      <c r="D5" s="281"/>
-      <c r="E5" s="282"/>
-      <c r="F5" s="280" t="s">
+      <c r="C5" s="284"/>
+      <c r="D5" s="284"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="283" t="s">
         <v>869</v>
       </c>
-      <c r="G5" s="281"/>
-      <c r="H5" s="281"/>
-      <c r="I5" s="282"/>
+      <c r="G5" s="284"/>
+      <c r="H5" s="284"/>
+      <c r="I5" s="285"/>
     </row>
     <row r="6" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="283" t="s">
+      <c r="B6" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="286" t="s">
+      <c r="C6" s="287"/>
+      <c r="D6" s="287"/>
+      <c r="E6" s="288"/>
+      <c r="F6" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="284"/>
-      <c r="H6" s="284"/>
-      <c r="I6" s="284"/>
-      <c r="J6" s="283" t="s">
+      <c r="G6" s="287"/>
+      <c r="H6" s="287"/>
+      <c r="I6" s="287"/>
+      <c r="J6" s="286" t="s">
         <v>184</v>
       </c>
-      <c r="K6" s="284"/>
-      <c r="L6" s="284"/>
-      <c r="M6" s="285"/>
-      <c r="N6" s="283" t="s">
+      <c r="K6" s="287"/>
+      <c r="L6" s="287"/>
+      <c r="M6" s="288"/>
+      <c r="N6" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="O6" s="284"/>
-      <c r="P6" s="284"/>
-      <c r="Q6" s="285"/>
+      <c r="O6" s="287"/>
+      <c r="P6" s="287"/>
+      <c r="Q6" s="288"/>
       <c r="V6" s="55"/>
       <c r="W6" s="56"/>
       <c r="X6" s="56"/>
@@ -28591,24 +28617,24 @@
     </row>
     <row r="7" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="208"/>
-      <c r="B7" s="283" t="s">
+      <c r="B7" s="286" t="s">
         <v>619</v>
       </c>
-      <c r="C7" s="284"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="283" t="s">
+      <c r="C7" s="287"/>
+      <c r="D7" s="287"/>
+      <c r="E7" s="288"/>
+      <c r="F7" s="286" t="s">
         <v>620</v>
       </c>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="283" t="s">
+      <c r="G7" s="287"/>
+      <c r="H7" s="287"/>
+      <c r="I7" s="288"/>
+      <c r="J7" s="286" t="s">
         <v>791</v>
       </c>
-      <c r="K7" s="284"/>
-      <c r="L7" s="284"/>
-      <c r="M7" s="285"/>
+      <c r="K7" s="287"/>
+      <c r="L7" s="287"/>
+      <c r="M7" s="288"/>
       <c r="N7" s="205"/>
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
@@ -28749,7 +28775,9 @@
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="176"/>
+      <c r="J9" s="311" t="s">
+        <v>964</v>
+      </c>
       <c r="K9" s="81"/>
       <c r="L9" s="230" t="s">
         <v>794</v>
@@ -29734,7 +29762,9 @@
       <c r="L57" s="26"/>
       <c r="M57" s="34"/>
       <c r="N57" s="4"/>
-      <c r="P57" s="26"/>
+      <c r="P57" s="26" t="s">
+        <v>963</v>
+      </c>
       <c r="Q57" s="76" t="s">
         <v>880</v>
       </c>
@@ -29889,7 +29919,9 @@
       <c r="G70" s="220"/>
       <c r="H70" s="220"/>
       <c r="I70" s="220"/>
-      <c r="J70" s="231"/>
+      <c r="J70" s="312" t="s">
+        <v>967</v>
+      </c>
       <c r="K70" s="220"/>
       <c r="L70" s="230" t="s">
         <v>795</v>
@@ -30574,7 +30606,6 @@
       <c r="B100" s="33"/>
       <c r="C100" s="26"/>
       <c r="D100" s="26"/>
-      <c r="E100" s="34"/>
       <c r="F100" s="21"/>
       <c r="G100" s="21"/>
       <c r="H100" s="21"/>
@@ -30591,13 +30622,12 @@
         <v>594</v>
       </c>
       <c r="B101" s="33"/>
-      <c r="C101" s="26"/>
       <c r="D101" s="81"/>
-      <c r="E101" s="77" t="s">
-        <v>842</v>
-      </c>
-      <c r="F101" s="73" t="s">
-        <v>573</v>
+      <c r="E101" s="78" t="s">
+        <v>841</v>
+      </c>
+      <c r="F101" s="75" t="s">
+        <v>574</v>
       </c>
       <c r="G101" s="81"/>
       <c r="H101" s="21"/>
@@ -30614,20 +30644,18 @@
         <v>595</v>
       </c>
       <c r="B102" s="33"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="78" t="s">
-        <v>841</v>
-      </c>
-      <c r="E102" s="77" t="s">
-        <v>472</v>
-      </c>
-      <c r="F102" s="73" t="s">
-        <v>575</v>
-      </c>
-      <c r="G102" s="75" t="s">
-        <v>574</v>
-      </c>
-      <c r="H102" s="21"/>
+      <c r="D102" s="77" t="s">
+        <v>842</v>
+      </c>
+      <c r="E102" s="78" t="s">
+        <v>469</v>
+      </c>
+      <c r="F102" s="75" t="s">
+        <v>576</v>
+      </c>
+      <c r="G102" s="73" t="s">
+        <v>573</v>
+      </c>
       <c r="I102" s="81"/>
       <c r="J102" s="33"/>
       <c r="K102" s="26"/>
@@ -30641,20 +30669,18 @@
         <v>596</v>
       </c>
       <c r="B103" s="33"/>
-      <c r="C103" s="26"/>
-      <c r="D103" s="78" t="s">
-        <v>469</v>
-      </c>
-      <c r="E103" s="77" t="s">
-        <v>473</v>
-      </c>
-      <c r="F103" s="73" t="s">
-        <v>577</v>
-      </c>
-      <c r="G103" s="75" t="s">
-        <v>576</v>
-      </c>
-      <c r="H103" s="81"/>
+      <c r="D103" s="77" t="s">
+        <v>472</v>
+      </c>
+      <c r="E103" s="78" t="s">
+        <v>470</v>
+      </c>
+      <c r="F103" s="75" t="s">
+        <v>578</v>
+      </c>
+      <c r="G103" s="73" t="s">
+        <v>575</v>
+      </c>
       <c r="I103" s="81"/>
       <c r="J103" s="33"/>
       <c r="K103" s="26"/>
@@ -30670,15 +30696,14 @@
       </c>
       <c r="B104" s="33"/>
       <c r="C104" s="26"/>
-      <c r="D104" s="78" t="s">
-        <v>470</v>
+      <c r="D104" s="77" t="s">
+        <v>473</v>
       </c>
       <c r="E104" s="82"/>
       <c r="F104" s="81"/>
-      <c r="G104" s="75" t="s">
-        <v>578</v>
-      </c>
-      <c r="H104" s="21"/>
+      <c r="G104" s="73" t="s">
+        <v>577</v>
+      </c>
       <c r="I104" s="21"/>
       <c r="J104" s="33"/>
       <c r="K104" s="26"/>
@@ -30756,7 +30781,7 @@
       <c r="K108" s="26"/>
       <c r="L108" s="26"/>
       <c r="M108" s="76" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c r="N108" s="4"/>
     </row>
@@ -30775,7 +30800,7 @@
       <c r="J109" s="33"/>
       <c r="K109" s="26"/>
       <c r="L109" s="76" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="M109" s="34"/>
       <c r="N109" s="4"/>
@@ -30796,7 +30821,7 @@
       <c r="K110" s="26"/>
       <c r="L110" s="34"/>
       <c r="M110" s="76" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="N110" s="4"/>
     </row>
@@ -30815,7 +30840,7 @@
       <c r="J111" s="33"/>
       <c r="K111" s="26"/>
       <c r="L111" s="76" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="M111" s="34"/>
       <c r="N111" s="4"/>
@@ -30825,10 +30850,9 @@
         <v>605</v>
       </c>
       <c r="B112" s="33"/>
-      <c r="C112" s="26"/>
       <c r="D112" s="26"/>
-      <c r="E112" s="76" t="s">
-        <v>844</v>
+      <c r="E112" s="74" t="s">
+        <v>846</v>
       </c>
       <c r="F112" s="80" t="s">
         <v>850</v>
@@ -30847,12 +30871,11 @@
         <v>801</v>
       </c>
       <c r="B113" s="33"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="74" t="s">
-        <v>846</v>
-      </c>
-      <c r="E113" s="76" t="s">
-        <v>845</v>
+      <c r="D113" s="76" t="s">
+        <v>844</v>
+      </c>
+      <c r="E113" s="74" t="s">
+        <v>847</v>
       </c>
       <c r="F113" s="80" t="s">
         <v>851</v>
@@ -30874,8 +30897,8 @@
       </c>
       <c r="B114" s="33"/>
       <c r="C114" s="26"/>
-      <c r="D114" s="74" t="s">
-        <v>847</v>
+      <c r="D114" s="76" t="s">
+        <v>845</v>
       </c>
       <c r="E114" s="34"/>
       <c r="F114" s="21"/>
@@ -30960,7 +30983,7 @@
       <c r="K118" s="26"/>
       <c r="L118" s="26"/>
       <c r="M118" s="76" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="N118" s="4"/>
     </row>
@@ -30979,9 +31002,9 @@
       <c r="J119" s="33"/>
       <c r="K119" s="26"/>
       <c r="L119" s="76" t="s">
-        <v>906</v>
-      </c>
-      <c r="M119" s="34"/>
+        <v>905</v>
+      </c>
+      <c r="M119" s="26"/>
       <c r="N119" s="4"/>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.4">
@@ -30998,9 +31021,9 @@
       <c r="I120" s="21"/>
       <c r="J120" s="33"/>
       <c r="K120" s="26"/>
-      <c r="L120" s="26"/>
+      <c r="L120" s="34"/>
       <c r="M120" s="76" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="N120" s="4"/>
     </row>
@@ -31019,7 +31042,7 @@
       <c r="J121" s="33"/>
       <c r="K121" s="26"/>
       <c r="L121" s="76" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="M121" s="34"/>
       <c r="N121" s="4"/>
@@ -31031,11 +31054,11 @@
       <c r="B122" s="33"/>
       <c r="C122" s="26"/>
       <c r="D122" s="26"/>
-      <c r="E122" s="76" t="s">
-        <v>905</v>
-      </c>
-      <c r="F122" s="76" t="s">
-        <v>843</v>
+      <c r="E122" s="74" t="s">
+        <v>906</v>
+      </c>
+      <c r="F122" s="74" t="s">
+        <v>919</v>
       </c>
       <c r="G122" s="21"/>
       <c r="H122" s="21"/>
@@ -31052,17 +31075,17 @@
       </c>
       <c r="B123" s="33"/>
       <c r="C123" s="26"/>
-      <c r="D123" s="74" t="s">
-        <v>906</v>
-      </c>
-      <c r="E123" s="76" t="s">
-        <v>903</v>
-      </c>
-      <c r="F123" s="76" t="s">
-        <v>845</v>
-      </c>
-      <c r="G123" s="74" t="s">
-        <v>919</v>
+      <c r="D123" s="76" t="s">
+        <v>905</v>
+      </c>
+      <c r="E123" s="74" t="s">
+        <v>904</v>
+      </c>
+      <c r="F123" s="74" t="s">
+        <v>920</v>
+      </c>
+      <c r="G123" s="76" t="s">
+        <v>843</v>
       </c>
       <c r="H123" s="21"/>
       <c r="I123" s="21"/>
@@ -31078,13 +31101,13 @@
       </c>
       <c r="B124" s="33"/>
       <c r="C124" s="26"/>
-      <c r="D124" s="74" t="s">
-        <v>904</v>
+      <c r="D124" s="76" t="s">
+        <v>903</v>
       </c>
       <c r="E124" s="34"/>
       <c r="F124" s="21"/>
-      <c r="G124" s="74" t="s">
-        <v>920</v>
+      <c r="G124" s="76" t="s">
+        <v>845</v>
       </c>
       <c r="H124" s="21"/>
       <c r="I124" s="21"/>
@@ -31192,9 +31215,9 @@
       <c r="I129" s="21"/>
       <c r="J129" s="33"/>
       <c r="K129" s="26"/>
-      <c r="L129" s="26"/>
+      <c r="L129" s="33"/>
       <c r="M129" s="77" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="N129" s="4"/>
       <c r="P129" s="76" t="s">
@@ -31217,9 +31240,9 @@
       <c r="J130" s="33"/>
       <c r="K130" s="26"/>
       <c r="L130" s="77" t="s">
-        <v>908</v>
-      </c>
-      <c r="M130" s="34"/>
+        <v>909</v>
+      </c>
+      <c r="M130" s="26"/>
       <c r="N130" s="4"/>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.4">
@@ -31236,9 +31259,9 @@
       <c r="I131" s="21"/>
       <c r="J131" s="33"/>
       <c r="K131" s="26"/>
-      <c r="L131" s="34"/>
+      <c r="L131" s="33"/>
       <c r="M131" s="77" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="N131" s="4"/>
     </row>
@@ -31257,9 +31280,9 @@
       <c r="J132" s="33"/>
       <c r="K132" s="26"/>
       <c r="L132" s="77" t="s">
-        <v>910</v>
-      </c>
-      <c r="M132" s="34"/>
+        <v>907</v>
+      </c>
+      <c r="M132" s="26"/>
       <c r="N132" s="4"/>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.4">
@@ -31274,7 +31297,9 @@
       <c r="G133" s="233"/>
       <c r="H133" s="233"/>
       <c r="I133" s="233"/>
-      <c r="J133" s="218"/>
+      <c r="J133" s="312" t="s">
+        <v>965</v>
+      </c>
       <c r="K133" s="219"/>
       <c r="L133" s="219"/>
       <c r="M133" s="232"/>
@@ -31832,7 +31857,9 @@
       <c r="G163" s="220"/>
       <c r="H163" s="219"/>
       <c r="I163" s="219"/>
-      <c r="J163" s="218"/>
+      <c r="J163" s="231" t="s">
+        <v>966</v>
+      </c>
       <c r="K163" s="219"/>
       <c r="L163" s="230" t="s">
         <v>793</v>
@@ -32225,8 +32252,6 @@
     <row r="185" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B185" s="176"/>
       <c r="C185" s="81"/>
-      <c r="D185" s="81"/>
-      <c r="E185" s="82"/>
       <c r="F185" s="81"/>
       <c r="G185" s="81"/>
       <c r="H185" s="81"/>
@@ -32241,7 +32266,9 @@
       <c r="B186" s="176"/>
       <c r="C186" s="81"/>
       <c r="D186" s="81"/>
-      <c r="E186" s="82"/>
+      <c r="E186" s="78" t="s">
+        <v>247</v>
+      </c>
       <c r="F186" s="81"/>
       <c r="G186" s="81"/>
       <c r="H186" s="81"/>
@@ -32255,8 +32282,12 @@
     <row r="187" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B187" s="176"/>
       <c r="C187" s="81"/>
-      <c r="D187" s="81"/>
-      <c r="E187" s="82"/>
+      <c r="D187" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="E187" s="78" t="s">
+        <v>250</v>
+      </c>
       <c r="F187" s="81"/>
       <c r="G187" s="81"/>
       <c r="H187" s="81"/>
@@ -32270,8 +32301,12 @@
     <row r="188" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B188" s="176"/>
       <c r="C188" s="81"/>
-      <c r="D188" s="12"/>
-      <c r="E188" s="110"/>
+      <c r="D188" s="77" t="s">
+        <v>248</v>
+      </c>
+      <c r="E188" s="78" t="s">
+        <v>254</v>
+      </c>
       <c r="F188" s="12"/>
       <c r="G188" s="12"/>
       <c r="H188" s="81"/>
@@ -32282,6 +32317,12 @@
         <v>556</v>
       </c>
       <c r="M188" s="82"/>
+    </row>
+    <row r="189" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="D189" s="77" t="s">
+        <v>251</v>
+      </c>
+      <c r="E189" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -32308,8 +32349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EEE4AC-A0CA-4CB6-8EA7-5A80EBEB6836}">
   <dimension ref="A1:AL108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -32348,17 +32389,17 @@
     <row r="1" spans="1:37" x14ac:dyDescent="0.4">
       <c r="B1" s="260"/>
       <c r="C1" s="260"/>
-      <c r="D1" s="287" t="s">
+      <c r="D1" s="290" t="s">
         <v>258</v>
       </c>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
       <c r="G1" s="42"/>
-      <c r="H1" s="287" t="s">
+      <c r="H1" s="290" t="s">
         <v>958</v>
       </c>
-      <c r="I1" s="288"/>
-      <c r="J1" s="288"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
       <c r="K1" s="42"/>
       <c r="P1" s="55"/>
       <c r="Q1" s="56"/>
@@ -32405,32 +32446,32 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="298" t="s">
+      <c r="D4" s="301" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="299"/>
-      <c r="F4" s="299"/>
-      <c r="G4" s="300"/>
-      <c r="H4" s="298" t="s">
+      <c r="E4" s="302"/>
+      <c r="F4" s="302"/>
+      <c r="G4" s="303"/>
+      <c r="H4" s="301" t="s">
         <v>282</v>
       </c>
-      <c r="I4" s="299"/>
-      <c r="J4" s="299"/>
-      <c r="K4" s="300"/>
+      <c r="I4" s="302"/>
+      <c r="J4" s="302"/>
+      <c r="K4" s="303"/>
     </row>
     <row r="5" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="280" t="s">
+      <c r="D5" s="283" t="s">
         <v>523</v>
       </c>
-      <c r="E5" s="281"/>
-      <c r="F5" s="281"/>
-      <c r="G5" s="282"/>
-      <c r="H5" s="280" t="s">
+      <c r="E5" s="284"/>
+      <c r="F5" s="284"/>
+      <c r="G5" s="285"/>
+      <c r="H5" s="283" t="s">
         <v>869</v>
       </c>
-      <c r="I5" s="281"/>
-      <c r="J5" s="281"/>
-      <c r="K5" s="282"/>
+      <c r="I5" s="284"/>
+      <c r="J5" s="284"/>
+      <c r="K5" s="285"/>
     </row>
     <row r="6" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="208" t="s">
@@ -32438,44 +32479,44 @@
       </c>
       <c r="B6" s="260"/>
       <c r="C6" s="260"/>
-      <c r="D6" s="283" t="s">
+      <c r="D6" s="286" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="285"/>
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="288"/>
       <c r="H6" s="55"/>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
       <c r="K6" s="57"/>
-      <c r="L6" s="286" t="s">
+      <c r="L6" s="289" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="284"/>
-      <c r="N6" s="284"/>
-      <c r="O6" s="284"/>
+      <c r="M6" s="287"/>
+      <c r="N6" s="287"/>
+      <c r="O6" s="287"/>
       <c r="P6" s="55"/>
       <c r="Q6" s="56"/>
       <c r="R6" s="56"/>
       <c r="S6" s="57"/>
-      <c r="T6" s="309"/>
-      <c r="U6" s="283" t="s">
+      <c r="T6" s="280"/>
+      <c r="U6" s="286" t="s">
         <v>184</v>
       </c>
-      <c r="V6" s="284"/>
-      <c r="W6" s="284"/>
-      <c r="X6" s="285"/>
+      <c r="V6" s="287"/>
+      <c r="W6" s="287"/>
+      <c r="X6" s="288"/>
       <c r="Y6" s="56"/>
       <c r="Z6" s="56"/>
       <c r="AA6" s="56"/>
       <c r="AB6" s="56"/>
       <c r="AC6" s="57"/>
-      <c r="AD6" s="283" t="s">
+      <c r="AD6" s="286" t="s">
         <v>187</v>
       </c>
-      <c r="AE6" s="284"/>
-      <c r="AF6" s="284"/>
-      <c r="AG6" s="285"/>
+      <c r="AE6" s="287"/>
+      <c r="AF6" s="287"/>
+      <c r="AG6" s="288"/>
       <c r="AH6" s="212"/>
       <c r="AI6" s="213"/>
       <c r="AJ6" s="213"/>
@@ -32487,45 +32528,45 @@
         <v>930</v>
       </c>
       <c r="C7" s="261"/>
-      <c r="D7" s="283" t="s">
+      <c r="D7" s="286" t="s">
         <v>619</v>
       </c>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="283" t="s">
+      <c r="E7" s="287"/>
+      <c r="F7" s="287"/>
+      <c r="G7" s="288"/>
+      <c r="H7" s="286" t="s">
         <v>835</v>
       </c>
-      <c r="I7" s="284"/>
-      <c r="J7" s="284"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="283" t="s">
+      <c r="I7" s="287"/>
+      <c r="J7" s="287"/>
+      <c r="K7" s="288"/>
+      <c r="L7" s="286" t="s">
         <v>620</v>
       </c>
-      <c r="M7" s="284"/>
-      <c r="N7" s="284"/>
-      <c r="O7" s="285"/>
-      <c r="P7" s="283"/>
-      <c r="Q7" s="284"/>
-      <c r="R7" s="284"/>
-      <c r="S7" s="285"/>
+      <c r="M7" s="287"/>
+      <c r="N7" s="287"/>
+      <c r="O7" s="288"/>
+      <c r="P7" s="286"/>
+      <c r="Q7" s="287"/>
+      <c r="R7" s="287"/>
+      <c r="S7" s="288"/>
       <c r="T7" s="147"/>
-      <c r="U7" s="283" t="s">
+      <c r="U7" s="286" t="s">
         <v>791</v>
       </c>
-      <c r="V7" s="284"/>
-      <c r="W7" s="284"/>
-      <c r="X7" s="285"/>
+      <c r="V7" s="287"/>
+      <c r="W7" s="287"/>
+      <c r="X7" s="288"/>
       <c r="AD7" s="215"/>
       <c r="AE7" s="215"/>
       <c r="AF7" s="215"/>
       <c r="AG7" s="216"/>
-      <c r="AH7" s="283" t="s">
+      <c r="AH7" s="286" t="s">
         <v>836</v>
       </c>
-      <c r="AI7" s="284"/>
-      <c r="AJ7" s="284"/>
-      <c r="AK7" s="285"/>
+      <c r="AI7" s="287"/>
+      <c r="AJ7" s="287"/>
+      <c r="AK7" s="288"/>
     </row>
     <row r="8" spans="1:37" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="208">

</xml_diff>

<commit_message>
220502-v3 cal_en not OK
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140FCD4D-6FE0-4D09-8722-FC50F56EAEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0494F8A2-C46E-4355-83FC-13D606E54459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="5970" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
@@ -5177,6 +5177,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5228,9 +5264,6 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5240,7 +5273,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5252,10 +5294,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5277,51 +5322,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5648,11 +5648,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W1" s="319" t="s">
+      <c r="W1" s="331" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="319"/>
-      <c r="Y1" s="319"/>
+      <c r="X1" s="331"/>
+      <c r="Y1" s="331"/>
       <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
@@ -5667,11 +5667,11 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W3" s="319" t="s">
+      <c r="W3" s="331" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="319"/>
-      <c r="Y3" s="319"/>
+      <c r="X3" s="331"/>
+      <c r="Y3" s="331"/>
       <c r="Z3" s="24" t="s">
         <v>55</v>
       </c>
@@ -6449,57 +6449,57 @@
       <c r="A1" s="220" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="323" t="s">
+      <c r="B1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="326" t="s">
+      <c r="C1" s="336"/>
+      <c r="D1" s="336"/>
+      <c r="E1" s="337"/>
+      <c r="F1" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="324"/>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="323" t="s">
+      <c r="G1" s="336"/>
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="335" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="324"/>
-      <c r="L1" s="324"/>
-      <c r="M1" s="325"/>
-      <c r="N1" s="323" t="s">
+      <c r="K1" s="336"/>
+      <c r="L1" s="336"/>
+      <c r="M1" s="337"/>
+      <c r="N1" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="324"/>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="325"/>
-      <c r="R1" s="327" t="s">
+      <c r="O1" s="336"/>
+      <c r="P1" s="336"/>
+      <c r="Q1" s="337"/>
+      <c r="R1" s="339" t="s">
         <v>258</v>
       </c>
-      <c r="S1" s="328"/>
-      <c r="T1" s="328"/>
+      <c r="S1" s="340"/>
+      <c r="T1" s="340"/>
       <c r="U1" s="42"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="220"/>
-      <c r="B2" s="323" t="s">
+      <c r="B2" s="335" t="s">
         <v>618</v>
       </c>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="325"/>
-      <c r="F2" s="323" t="s">
+      <c r="C2" s="336"/>
+      <c r="D2" s="336"/>
+      <c r="E2" s="337"/>
+      <c r="F2" s="335" t="s">
         <v>619</v>
       </c>
-      <c r="G2" s="324"/>
-      <c r="H2" s="324"/>
-      <c r="I2" s="325"/>
-      <c r="J2" s="323" t="s">
+      <c r="G2" s="336"/>
+      <c r="H2" s="336"/>
+      <c r="I2" s="337"/>
+      <c r="J2" s="335" t="s">
         <v>778</v>
       </c>
-      <c r="K2" s="324"/>
-      <c r="L2" s="324"/>
-      <c r="M2" s="325"/>
+      <c r="K2" s="336"/>
+      <c r="L2" s="336"/>
+      <c r="M2" s="337"/>
       <c r="N2" s="44"/>
       <c r="O2" s="224"/>
       <c r="P2" s="224"/>
@@ -6598,12 +6598,12 @@
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="34"/>
-      <c r="R4" s="341" t="s">
+      <c r="R4" s="355" t="s">
         <v>282</v>
       </c>
-      <c r="S4" s="342"/>
-      <c r="T4" s="342"/>
-      <c r="U4" s="343"/>
+      <c r="S4" s="356"/>
+      <c r="T4" s="356"/>
+      <c r="U4" s="357"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="220" t="s">
@@ -6626,12 +6626,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="320" t="s">
+      <c r="R5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="S5" s="321"/>
-      <c r="T5" s="321"/>
-      <c r="U5" s="322"/>
+      <c r="S5" s="333"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="334"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="220" t="s">
@@ -8301,11 +8301,11 @@
       <c r="K93" s="218"/>
       <c r="L93" s="228"/>
       <c r="M93" s="228"/>
-      <c r="R93" s="327" t="s">
+      <c r="R93" s="339" t="s">
         <v>258</v>
       </c>
-      <c r="S93" s="328"/>
-      <c r="T93" s="328"/>
+      <c r="S93" s="340"/>
+      <c r="T93" s="340"/>
       <c r="U93" s="42"/>
     </row>
     <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -8394,12 +8394,12 @@
       <c r="K96" s="81"/>
       <c r="L96" s="81"/>
       <c r="M96" s="82"/>
-      <c r="R96" s="341" t="s">
+      <c r="R96" s="355" t="s">
         <v>54</v>
       </c>
-      <c r="S96" s="346"/>
-      <c r="T96" s="346"/>
-      <c r="U96" s="347"/>
+      <c r="S96" s="361"/>
+      <c r="T96" s="361"/>
+      <c r="U96" s="362"/>
     </row>
     <row r="97" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="220" t="s">
@@ -8421,12 +8421,12 @@
       <c r="K97" s="81"/>
       <c r="L97" s="81"/>
       <c r="M97" s="82"/>
-      <c r="R97" s="327" t="s">
+      <c r="R97" s="339" t="s">
         <v>856</v>
       </c>
-      <c r="S97" s="328"/>
-      <c r="T97" s="328"/>
-      <c r="U97" s="329"/>
+      <c r="S97" s="340"/>
+      <c r="T97" s="340"/>
+      <c r="U97" s="341"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A98" s="220" t="s">
@@ -8478,11 +8478,11 @@
       <c r="K100" s="81"/>
       <c r="L100" s="81"/>
       <c r="M100" s="82"/>
-      <c r="R100" s="327" t="s">
+      <c r="R100" s="339" t="s">
         <v>857</v>
       </c>
-      <c r="S100" s="328"/>
-      <c r="T100" s="328"/>
+      <c r="S100" s="340"/>
+      <c r="T100" s="340"/>
       <c r="U100" s="42"/>
     </row>
     <row r="101" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -8578,12 +8578,12 @@
       <c r="M103" s="34" t="s">
         <v>472</v>
       </c>
-      <c r="R103" s="341" t="s">
+      <c r="R103" s="355" t="s">
         <v>282</v>
       </c>
-      <c r="S103" s="346"/>
-      <c r="T103" s="346"/>
-      <c r="U103" s="347"/>
+      <c r="S103" s="361"/>
+      <c r="T103" s="361"/>
+      <c r="U103" s="362"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A104" s="220" t="s">
@@ -8600,12 +8600,12 @@
       <c r="L104" s="34" t="s">
         <v>469</v>
       </c>
-      <c r="R104" s="327" t="s">
+      <c r="R104" s="339" t="s">
         <v>856</v>
       </c>
-      <c r="S104" s="328"/>
-      <c r="T104" s="328"/>
-      <c r="U104" s="329"/>
+      <c r="S104" s="340"/>
+      <c r="T104" s="340"/>
+      <c r="U104" s="341"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A105" s="220" t="s">
@@ -8955,12 +8955,12 @@
       <c r="L124" s="34" t="s">
         <v>759</v>
       </c>
-      <c r="R124" s="327" t="s">
+      <c r="R124" s="339" t="s">
         <v>868</v>
       </c>
-      <c r="S124" s="328"/>
-      <c r="T124" s="328"/>
-      <c r="U124" s="329"/>
+      <c r="S124" s="340"/>
+      <c r="T124" s="340"/>
+      <c r="U124" s="341"/>
     </row>
     <row r="125" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="220" t="s">
@@ -9036,23 +9036,23 @@
       <c r="G127" s="75" t="s">
         <v>577</v>
       </c>
-      <c r="R127" s="341" t="s">
+      <c r="R127" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="S127" s="346"/>
-      <c r="T127" s="346"/>
-      <c r="U127" s="347"/>
+      <c r="S127" s="361"/>
+      <c r="T127" s="361"/>
+      <c r="U127" s="362"/>
     </row>
     <row r="128" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="220" t="s">
         <v>869</v>
       </c>
-      <c r="R128" s="323" t="s">
+      <c r="R128" s="335" t="s">
         <v>856</v>
       </c>
-      <c r="S128" s="324"/>
-      <c r="T128" s="324"/>
-      <c r="U128" s="325"/>
+      <c r="S128" s="336"/>
+      <c r="T128" s="336"/>
+      <c r="U128" s="337"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A129" s="220" t="s">
@@ -9107,12 +9107,12 @@
       <c r="F135" s="80" t="s">
         <v>837</v>
       </c>
-      <c r="R135" s="327" t="s">
+      <c r="R135" s="339" t="s">
         <v>888</v>
       </c>
-      <c r="S135" s="328"/>
-      <c r="T135" s="328"/>
-      <c r="U135" s="329"/>
+      <c r="S135" s="340"/>
+      <c r="T135" s="340"/>
+      <c r="U135" s="341"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A136" s="220" t="s">
@@ -9164,23 +9164,23 @@
       <c r="A138" s="220" t="s">
         <v>845</v>
       </c>
-      <c r="R138" s="341" t="s">
+      <c r="R138" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="S138" s="346"/>
-      <c r="T138" s="346"/>
-      <c r="U138" s="347"/>
+      <c r="S138" s="361"/>
+      <c r="T138" s="361"/>
+      <c r="U138" s="362"/>
     </row>
     <row r="139" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="220" t="s">
         <v>846</v>
       </c>
-      <c r="R139" s="323" t="s">
+      <c r="R139" s="335" t="s">
         <v>899</v>
       </c>
-      <c r="S139" s="324"/>
-      <c r="T139" s="324"/>
-      <c r="U139" s="325"/>
+      <c r="S139" s="336"/>
+      <c r="T139" s="336"/>
+      <c r="U139" s="337"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A140" s="220" t="s">
@@ -9229,12 +9229,12 @@
       <c r="F145" s="76" t="s">
         <v>830</v>
       </c>
-      <c r="R145" s="327" t="s">
+      <c r="R145" s="339" t="s">
         <v>898</v>
       </c>
-      <c r="S145" s="328"/>
-      <c r="T145" s="328"/>
-      <c r="U145" s="329"/>
+      <c r="S145" s="340"/>
+      <c r="T145" s="340"/>
+      <c r="U145" s="341"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A146" s="220" t="s">
@@ -9286,12 +9286,12 @@
       <c r="A148" s="220" t="s">
         <v>870</v>
       </c>
-      <c r="R148" s="341" t="s">
+      <c r="R148" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="S148" s="346"/>
-      <c r="T148" s="346"/>
-      <c r="U148" s="347"/>
+      <c r="S148" s="361"/>
+      <c r="T148" s="361"/>
+      <c r="U148" s="362"/>
     </row>
     <row r="149" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="220" t="s">
@@ -9301,12 +9301,12 @@
       <c r="Q149" s="76" t="s">
         <v>861</v>
       </c>
-      <c r="R149" s="323" t="s">
+      <c r="R149" s="335" t="s">
         <v>899</v>
       </c>
-      <c r="S149" s="324"/>
-      <c r="T149" s="324"/>
-      <c r="U149" s="325"/>
+      <c r="S149" s="336"/>
+      <c r="T149" s="336"/>
+      <c r="U149" s="337"/>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A150" s="220" t="s">
@@ -9415,6 +9415,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R138:U138"/>
+    <mergeCell ref="R139:U139"/>
+    <mergeCell ref="R148:U148"/>
+    <mergeCell ref="R149:U149"/>
+    <mergeCell ref="R135:U135"/>
+    <mergeCell ref="R145:U145"/>
+    <mergeCell ref="R128:U128"/>
+    <mergeCell ref="R93:T93"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="R97:U97"/>
+    <mergeCell ref="R100:T100"/>
+    <mergeCell ref="R103:U103"/>
+    <mergeCell ref="R104:U104"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="R127:U127"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="B1:E1"/>
@@ -9425,21 +9440,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="R128:U128"/>
-    <mergeCell ref="R93:T93"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="R97:U97"/>
-    <mergeCell ref="R100:T100"/>
-    <mergeCell ref="R103:U103"/>
-    <mergeCell ref="R104:U104"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="R127:U127"/>
-    <mergeCell ref="R138:U138"/>
-    <mergeCell ref="R139:U139"/>
-    <mergeCell ref="R148:U148"/>
-    <mergeCell ref="R149:U149"/>
-    <mergeCell ref="R135:U135"/>
-    <mergeCell ref="R145:U145"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9476,36 +9476,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="323" t="s">
+      <c r="C1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="326" t="s">
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="324"/>
-      <c r="K1" s="323" t="s">
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="336"/>
+      <c r="K1" s="335" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="323" t="s">
+      <c r="L1" s="336"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="335" t="s">
         <v>955</v>
       </c>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="324"/>
-      <c r="R1" s="325"/>
-      <c r="Z1" s="323" t="s">
+      <c r="P1" s="336"/>
+      <c r="Q1" s="336"/>
+      <c r="R1" s="337"/>
+      <c r="Z1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="324"/>
-      <c r="AB1" s="324"/>
-      <c r="AC1" s="325"/>
+      <c r="AA1" s="336"/>
+      <c r="AB1" s="336"/>
+      <c r="AC1" s="337"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -9574,33 +9574,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="327" t="s">
+      <c r="C3" s="339" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="328"/>
-      <c r="E3" s="328"/>
-      <c r="F3" s="329"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="329"/>
+      <c r="D3" s="340"/>
+      <c r="E3" s="340"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="339"/>
+      <c r="H3" s="340"/>
+      <c r="I3" s="340"/>
+      <c r="J3" s="341"/>
       <c r="K3" s="40"/>
       <c r="O3" s="40"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="327" t="s">
+      <c r="S3" s="339" t="s">
         <v>402</v>
       </c>
-      <c r="T3" s="328"/>
-      <c r="U3" s="328"/>
-      <c r="V3" s="329"/>
-      <c r="Z3" s="327" t="s">
+      <c r="T3" s="340"/>
+      <c r="U3" s="340"/>
+      <c r="V3" s="341"/>
+      <c r="Z3" s="339" t="s">
         <v>265</v>
       </c>
-      <c r="AA3" s="328"/>
-      <c r="AB3" s="328"/>
-      <c r="AC3" s="329"/>
+      <c r="AA3" s="340"/>
+      <c r="AB3" s="340"/>
+      <c r="AC3" s="341"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -9657,12 +9657,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="320" t="s">
+      <c r="S5" s="332" t="s">
         <v>502</v>
       </c>
-      <c r="T5" s="321"/>
-      <c r="U5" s="321"/>
-      <c r="V5" s="322"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="333"/>
+      <c r="V5" s="334"/>
       <c r="W5" s="84" t="s">
         <v>504</v>
       </c>
@@ -9692,12 +9692,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="320" t="s">
+      <c r="S6" s="332" t="s">
         <v>928</v>
       </c>
-      <c r="T6" s="321"/>
-      <c r="U6" s="321"/>
-      <c r="V6" s="322"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="333"/>
+      <c r="V6" s="334"/>
       <c r="Z6" s="221"/>
       <c r="AA6" s="222"/>
       <c r="AB6" s="222"/>
@@ -10203,13 +10203,13 @@
       <c r="R22" s="74" t="s">
         <v>420</v>
       </c>
-      <c r="S22" s="348" t="s">
+      <c r="S22" s="363" t="s">
         <v>938</v>
       </c>
-      <c r="T22" s="350"/>
-      <c r="U22" s="350"/>
-      <c r="V22" s="350"/>
-      <c r="W22" s="350"/>
+      <c r="T22" s="365"/>
+      <c r="U22" s="365"/>
+      <c r="V22" s="365"/>
+      <c r="W22" s="365"/>
       <c r="Z22" s="79" t="s">
         <v>243</v>
       </c>
@@ -10256,12 +10256,12 @@
       <c r="R23" s="74" t="s">
         <v>421</v>
       </c>
-      <c r="S23" s="348" t="s">
+      <c r="S23" s="363" t="s">
         <v>939</v>
       </c>
-      <c r="T23" s="349"/>
-      <c r="U23" s="349"/>
-      <c r="V23" s="349"/>
+      <c r="T23" s="364"/>
+      <c r="U23" s="364"/>
+      <c r="V23" s="364"/>
       <c r="Z23" s="79" t="s">
         <v>245</v>
       </c>
@@ -10354,12 +10354,12 @@
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="320" t="s">
+      <c r="K26" s="332" t="s">
         <v>937</v>
       </c>
-      <c r="L26" s="321"/>
-      <c r="M26" s="321"/>
-      <c r="N26" s="322"/>
+      <c r="L26" s="333"/>
+      <c r="M26" s="333"/>
+      <c r="N26" s="334"/>
       <c r="O26" s="76" t="s">
         <v>434</v>
       </c>
@@ -11069,6 +11069,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="S23:V23"/>
+    <mergeCell ref="S22:W22"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="S6:V6"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="S5:V5"/>
@@ -11077,12 +11083,6 @@
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="S3:V3"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="S23:V23"/>
-    <mergeCell ref="S22:W22"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="S6:V6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11120,30 +11120,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="68"/>
       <c r="B1"/>
-      <c r="C1" s="323" t="s">
+      <c r="C1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="323" t="s">
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="335" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="325"/>
-      <c r="K1" s="323" t="s">
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="337"/>
+      <c r="K1" s="335" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="323" t="s">
+      <c r="L1" s="336"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="324"/>
-      <c r="R1" s="325"/>
+      <c r="P1" s="336"/>
+      <c r="Q1" s="336"/>
+      <c r="R1" s="337"/>
     </row>
     <row r="2" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="68"/>
@@ -11232,12 +11232,12 @@
       <c r="P3" s="271"/>
       <c r="Q3" s="271"/>
       <c r="R3" s="275"/>
-      <c r="S3" s="328" t="s">
+      <c r="S3" s="340" t="s">
         <v>934</v>
       </c>
-      <c r="T3" s="328"/>
-      <c r="U3" s="328"/>
-      <c r="V3" s="329"/>
+      <c r="T3" s="340"/>
+      <c r="U3" s="340"/>
+      <c r="V3" s="341"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="68" t="s">
@@ -11298,12 +11298,12 @@
       <c r="P5" s="271"/>
       <c r="Q5" s="271"/>
       <c r="R5" s="275"/>
-      <c r="S5" s="321" t="s">
+      <c r="S5" s="333" t="s">
         <v>860</v>
       </c>
-      <c r="T5" s="321"/>
-      <c r="U5" s="321"/>
-      <c r="V5" s="322"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="333"/>
+      <c r="V5" s="334"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="68" t="s">
@@ -11329,12 +11329,12 @@
       <c r="P6" s="271"/>
       <c r="Q6" s="271"/>
       <c r="R6" s="275"/>
-      <c r="S6" s="321" t="s">
+      <c r="S6" s="333" t="s">
         <v>935</v>
       </c>
-      <c r="T6" s="321"/>
-      <c r="U6" s="321"/>
-      <c r="V6" s="322"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="333"/>
+      <c r="V6" s="334"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="68" t="s">
@@ -11387,10 +11387,10 @@
       <c r="P8" s="271"/>
       <c r="Q8" s="271"/>
       <c r="R8" s="275"/>
-      <c r="S8" s="350"/>
-      <c r="T8" s="349"/>
-      <c r="U8" s="349"/>
-      <c r="V8" s="349"/>
+      <c r="S8" s="365"/>
+      <c r="T8" s="364"/>
+      <c r="U8" s="364"/>
+      <c r="V8" s="364"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="68" t="s">
@@ -11566,12 +11566,12 @@
       <c r="N15" s="267" t="s">
         <v>285</v>
       </c>
-      <c r="O15" s="351" t="s">
+      <c r="O15" s="366" t="s">
         <v>936</v>
       </c>
-      <c r="P15" s="336"/>
-      <c r="Q15" s="336"/>
-      <c r="R15" s="352"/>
+      <c r="P15" s="351"/>
+      <c r="Q15" s="351"/>
+      <c r="R15" s="367"/>
     </row>
     <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="68" t="s">
@@ -13592,30 +13592,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="277"/>
       <c r="B1" s="264"/>
-      <c r="C1" s="323" t="s">
+      <c r="C1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="323" t="s">
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="335" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="325"/>
-      <c r="K1" s="323" t="s">
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="337"/>
+      <c r="K1" s="335" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="323" t="s">
+      <c r="L1" s="336"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="324"/>
-      <c r="R1" s="325"/>
+      <c r="P1" s="336"/>
+      <c r="Q1" s="336"/>
+      <c r="R1" s="337"/>
       <c r="S1" s="227"/>
       <c r="T1" s="227"/>
       <c r="U1" s="227"/>
@@ -13714,12 +13714,12 @@
       <c r="P3" s="222"/>
       <c r="Q3" s="222"/>
       <c r="R3" s="223"/>
-      <c r="S3" s="327" t="s">
+      <c r="S3" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="328"/>
-      <c r="U3" s="328"/>
-      <c r="V3" s="329"/>
+      <c r="T3" s="340"/>
+      <c r="U3" s="340"/>
+      <c r="V3" s="341"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="277" t="s">
@@ -13788,12 +13788,12 @@
       <c r="P5" s="222"/>
       <c r="Q5" s="222"/>
       <c r="R5" s="223"/>
-      <c r="S5" s="320" t="s">
+      <c r="S5" s="332" t="s">
         <v>282</v>
       </c>
-      <c r="T5" s="321"/>
-      <c r="U5" s="321"/>
-      <c r="V5" s="322"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="333"/>
+      <c r="V5" s="334"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="277" t="s">
@@ -13824,12 +13824,12 @@
       <c r="P6" s="222"/>
       <c r="Q6" s="222"/>
       <c r="R6" s="223"/>
-      <c r="S6" s="320" t="s">
+      <c r="S6" s="332" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="321"/>
-      <c r="U6" s="321"/>
-      <c r="V6" s="322"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="333"/>
+      <c r="V6" s="334"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="277" t="s">
@@ -13897,12 +13897,12 @@
         <v>284</v>
       </c>
       <c r="R8" s="223"/>
-      <c r="S8" s="348" t="s">
+      <c r="S8" s="363" t="s">
         <v>940</v>
       </c>
-      <c r="T8" s="349"/>
-      <c r="U8" s="349"/>
-      <c r="V8" s="349"/>
+      <c r="T8" s="364"/>
+      <c r="U8" s="364"/>
+      <c r="V8" s="364"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="277" t="s">
@@ -16238,30 +16238,30 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="68"/>
-      <c r="C1" s="323" t="s">
+      <c r="C1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="323" t="s">
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="335" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="325"/>
-      <c r="K1" s="323" t="s">
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="337"/>
+      <c r="K1" s="335" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="323" t="s">
+      <c r="L1" s="336"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="324"/>
-      <c r="R1" s="325"/>
+      <c r="P1" s="336"/>
+      <c r="Q1" s="336"/>
+      <c r="R1" s="337"/>
       <c r="S1" s="45"/>
       <c r="T1" s="45"/>
       <c r="U1" s="45"/>
@@ -16359,12 +16359,12 @@
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="41"/>
-      <c r="S3" s="327" t="s">
+      <c r="S3" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="328"/>
-      <c r="U3" s="328"/>
-      <c r="V3" s="329"/>
+      <c r="T3" s="340"/>
+      <c r="U3" s="340"/>
+      <c r="V3" s="341"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="68" t="s">
@@ -16429,12 +16429,12 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="41"/>
-      <c r="S5" s="320" t="s">
+      <c r="S5" s="332" t="s">
         <v>282</v>
       </c>
-      <c r="T5" s="321"/>
-      <c r="U5" s="321"/>
-      <c r="V5" s="322"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="333"/>
+      <c r="V5" s="334"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="68" t="s">
@@ -16464,12 +16464,12 @@
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="41"/>
-      <c r="S6" s="320" t="s">
+      <c r="S6" s="332" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="321"/>
-      <c r="U6" s="321"/>
-      <c r="V6" s="322"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="333"/>
+      <c r="V6" s="334"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="68" t="s">
@@ -16536,12 +16536,12 @@
         <v>284</v>
       </c>
       <c r="R8" s="41"/>
-      <c r="S8" s="348" t="s">
+      <c r="S8" s="363" t="s">
         <v>378</v>
       </c>
-      <c r="T8" s="349"/>
-      <c r="U8" s="349"/>
-      <c r="V8" s="349"/>
+      <c r="T8" s="364"/>
+      <c r="U8" s="364"/>
+      <c r="V8" s="364"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="68" t="s">
@@ -19025,36 +19025,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="21"/>
-      <c r="C1" s="323" t="s">
+      <c r="C1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="326" t="s">
+      <c r="D1" s="336"/>
+      <c r="E1" s="336"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="324"/>
-      <c r="K1" s="323" t="s">
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="336"/>
+      <c r="K1" s="335" t="s">
         <v>442</v>
       </c>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="323" t="s">
+      <c r="L1" s="336"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="335" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="324"/>
-      <c r="R1" s="325"/>
-      <c r="Z1" s="323" t="s">
+      <c r="P1" s="336"/>
+      <c r="Q1" s="336"/>
+      <c r="R1" s="337"/>
+      <c r="Z1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="324"/>
-      <c r="AB1" s="324"/>
-      <c r="AC1" s="325"/>
+      <c r="AA1" s="336"/>
+      <c r="AB1" s="336"/>
+      <c r="AC1" s="337"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="21"/>
@@ -19123,33 +19123,33 @@
       <c r="B3" s="21">
         <v>0</v>
       </c>
-      <c r="C3" s="327" t="s">
+      <c r="C3" s="339" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="328"/>
-      <c r="E3" s="328"/>
-      <c r="F3" s="329"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="329"/>
+      <c r="D3" s="340"/>
+      <c r="E3" s="340"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="339"/>
+      <c r="H3" s="340"/>
+      <c r="I3" s="340"/>
+      <c r="J3" s="341"/>
       <c r="K3" s="221"/>
       <c r="O3" s="221"/>
       <c r="P3" s="222"/>
       <c r="Q3" s="222"/>
       <c r="R3" s="223"/>
-      <c r="S3" s="327" t="s">
+      <c r="S3" s="339" t="s">
         <v>402</v>
       </c>
-      <c r="T3" s="328"/>
-      <c r="U3" s="328"/>
-      <c r="V3" s="329"/>
-      <c r="Z3" s="327" t="s">
+      <c r="T3" s="340"/>
+      <c r="U3" s="340"/>
+      <c r="V3" s="341"/>
+      <c r="Z3" s="339" t="s">
         <v>265</v>
       </c>
-      <c r="AA3" s="328"/>
-      <c r="AB3" s="328"/>
-      <c r="AC3" s="329"/>
+      <c r="AA3" s="340"/>
+      <c r="AB3" s="340"/>
+      <c r="AC3" s="341"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="39" t="s">
@@ -19206,12 +19206,12 @@
       <c r="P5" s="222"/>
       <c r="Q5" s="222"/>
       <c r="R5" s="223"/>
-      <c r="S5" s="320" t="s">
+      <c r="S5" s="332" t="s">
         <v>502</v>
       </c>
-      <c r="T5" s="321"/>
-      <c r="U5" s="321"/>
-      <c r="V5" s="322"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="333"/>
+      <c r="V5" s="334"/>
       <c r="W5" s="84" t="s">
         <v>504</v>
       </c>
@@ -19241,12 +19241,12 @@
       <c r="P6" s="222"/>
       <c r="Q6" s="222"/>
       <c r="R6" s="223"/>
-      <c r="S6" s="320" t="s">
+      <c r="S6" s="332" t="s">
         <v>419</v>
       </c>
-      <c r="T6" s="321"/>
-      <c r="U6" s="321"/>
-      <c r="V6" s="322"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="333"/>
+      <c r="V6" s="334"/>
       <c r="Z6" s="221"/>
       <c r="AA6" s="222"/>
       <c r="AB6" s="222"/>
@@ -20605,17 +20605,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="S5:V5"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="Z3:AC3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20646,30 +20646,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="21"/>
-      <c r="B1" s="323" t="s">
+      <c r="B1" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="326" t="s">
+      <c r="C1" s="336"/>
+      <c r="D1" s="336"/>
+      <c r="E1" s="337"/>
+      <c r="F1" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="324"/>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="323" t="s">
+      <c r="G1" s="336"/>
+      <c r="H1" s="336"/>
+      <c r="I1" s="336"/>
+      <c r="J1" s="335" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="324"/>
-      <c r="L1" s="324"/>
-      <c r="M1" s="325"/>
-      <c r="N1" s="323" t="s">
+      <c r="K1" s="336"/>
+      <c r="L1" s="336"/>
+      <c r="M1" s="337"/>
+      <c r="N1" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="324"/>
-      <c r="P1" s="324"/>
-      <c r="Q1" s="325"/>
+      <c r="O1" s="336"/>
+      <c r="P1" s="336"/>
+      <c r="Q1" s="337"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="21"/>
@@ -20756,12 +20756,12 @@
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
       <c r="Q3" s="41"/>
-      <c r="R3" s="327" t="s">
+      <c r="R3" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="328"/>
-      <c r="T3" s="328"/>
-      <c r="U3" s="329"/>
+      <c r="S3" s="340"/>
+      <c r="T3" s="340"/>
+      <c r="U3" s="341"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="39" t="s">
@@ -20814,12 +20814,12 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="320" t="s">
+      <c r="R5" s="332" t="s">
         <v>54</v>
       </c>
-      <c r="S5" s="321"/>
-      <c r="T5" s="321"/>
-      <c r="U5" s="322"/>
+      <c r="S5" s="333"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="334"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
@@ -20841,12 +20841,12 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="34"/>
-      <c r="R6" s="320" t="s">
+      <c r="R6" s="332" t="s">
         <v>262</v>
       </c>
-      <c r="S6" s="321"/>
-      <c r="T6" s="321"/>
-      <c r="U6" s="322"/>
+      <c r="S6" s="333"/>
+      <c r="T6" s="333"/>
+      <c r="U6" s="334"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="39" t="s">
@@ -22476,67 +22476,67 @@
       </c>
     </row>
     <row r="6" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="330" t="s">
+      <c r="B6" s="342" t="s">
         <v>514</v>
       </c>
-      <c r="C6" s="331"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="330" t="s">
+      <c r="C6" s="343"/>
+      <c r="D6" s="344"/>
+      <c r="E6" s="342" t="s">
         <v>515</v>
       </c>
-      <c r="F6" s="331"/>
-      <c r="G6" s="332"/>
+      <c r="F6" s="343"/>
+      <c r="G6" s="344"/>
     </row>
     <row r="7" spans="1:44" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="330" t="s">
+      <c r="B7" s="342" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="331"/>
-      <c r="D7" s="331"/>
-      <c r="E7" s="331"/>
-      <c r="F7" s="331"/>
-      <c r="G7" s="331"/>
-      <c r="H7" s="331"/>
-      <c r="I7" s="331"/>
-      <c r="J7" s="331"/>
-      <c r="K7" s="331"/>
-      <c r="L7" s="331"/>
-      <c r="M7" s="331"/>
-      <c r="N7" s="331"/>
-      <c r="O7" s="331"/>
-      <c r="P7" s="332"/>
-      <c r="Q7" s="330" t="s">
+      <c r="C7" s="343"/>
+      <c r="D7" s="343"/>
+      <c r="E7" s="343"/>
+      <c r="F7" s="343"/>
+      <c r="G7" s="343"/>
+      <c r="H7" s="343"/>
+      <c r="I7" s="343"/>
+      <c r="J7" s="343"/>
+      <c r="K7" s="343"/>
+      <c r="L7" s="343"/>
+      <c r="M7" s="343"/>
+      <c r="N7" s="343"/>
+      <c r="O7" s="343"/>
+      <c r="P7" s="344"/>
+      <c r="Q7" s="342" t="s">
         <v>215</v>
       </c>
-      <c r="R7" s="331"/>
-      <c r="S7" s="331"/>
-      <c r="T7" s="331"/>
-      <c r="U7" s="331"/>
-      <c r="V7" s="331"/>
-      <c r="W7" s="331"/>
-      <c r="X7" s="331"/>
-      <c r="Y7" s="331"/>
-      <c r="Z7" s="331"/>
-      <c r="AA7" s="332"/>
-      <c r="AB7" s="330" t="s">
+      <c r="R7" s="343"/>
+      <c r="S7" s="343"/>
+      <c r="T7" s="343"/>
+      <c r="U7" s="343"/>
+      <c r="V7" s="343"/>
+      <c r="W7" s="343"/>
+      <c r="X7" s="343"/>
+      <c r="Y7" s="343"/>
+      <c r="Z7" s="343"/>
+      <c r="AA7" s="344"/>
+      <c r="AB7" s="342" t="s">
         <v>216</v>
       </c>
-      <c r="AC7" s="331"/>
-      <c r="AD7" s="331"/>
-      <c r="AE7" s="331"/>
-      <c r="AF7" s="331"/>
-      <c r="AG7" s="331"/>
-      <c r="AH7" s="331"/>
-      <c r="AI7" s="331"/>
-      <c r="AJ7" s="331"/>
-      <c r="AK7" s="331"/>
-      <c r="AL7" s="331"/>
-      <c r="AM7" s="331"/>
-      <c r="AN7" s="331"/>
-      <c r="AO7" s="331"/>
-      <c r="AP7" s="331"/>
-      <c r="AQ7" s="331"/>
-      <c r="AR7" s="332"/>
+      <c r="AC7" s="343"/>
+      <c r="AD7" s="343"/>
+      <c r="AE7" s="343"/>
+      <c r="AF7" s="343"/>
+      <c r="AG7" s="343"/>
+      <c r="AH7" s="343"/>
+      <c r="AI7" s="343"/>
+      <c r="AJ7" s="343"/>
+      <c r="AK7" s="343"/>
+      <c r="AL7" s="343"/>
+      <c r="AM7" s="343"/>
+      <c r="AN7" s="343"/>
+      <c r="AO7" s="343"/>
+      <c r="AP7" s="343"/>
+      <c r="AQ7" s="343"/>
+      <c r="AR7" s="344"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.4">
       <c r="E9" s="45"/>
@@ -24458,18 +24458,18 @@
       <c r="AB1" s="280"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="B2" s="319" t="s">
+      <c r="B2" s="331" t="s">
         <v>672</v>
       </c>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
-      <c r="G2" s="319"/>
-      <c r="H2" s="319"/>
-      <c r="I2" s="319"/>
-      <c r="J2" s="319"/>
-      <c r="K2" s="319"/>
+      <c r="C2" s="331"/>
+      <c r="D2" s="331"/>
+      <c r="E2" s="331"/>
+      <c r="F2" s="331"/>
+      <c r="G2" s="331"/>
+      <c r="H2" s="331"/>
+      <c r="I2" s="331"/>
+      <c r="J2" s="331"/>
+      <c r="K2" s="331"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
@@ -24750,15 +24750,15 @@
       <c r="O12" s="21">
         <v>1</v>
       </c>
-      <c r="V12" s="319" t="s">
+      <c r="V12" s="331" t="s">
         <v>1056</v>
       </c>
-      <c r="W12" s="319"/>
-      <c r="X12" s="319"/>
-      <c r="Y12" s="319"/>
-      <c r="Z12" s="319"/>
-      <c r="AA12" s="319"/>
-      <c r="AB12" s="319"/>
+      <c r="W12" s="331"/>
+      <c r="X12" s="331"/>
+      <c r="Y12" s="331"/>
+      <c r="Z12" s="331"/>
+      <c r="AA12" s="331"/>
+      <c r="AB12" s="331"/>
       <c r="AC12" s="201"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.4">
@@ -26786,18 +26786,18 @@
       <c r="A83" s="289" t="s">
         <v>1015</v>
       </c>
-      <c r="B83" s="327" t="s">
+      <c r="B83" s="339" t="s">
         <v>1016</v>
       </c>
-      <c r="C83" s="328"/>
-      <c r="D83" s="328"/>
-      <c r="E83" s="329"/>
-      <c r="G83" s="333" t="s">
+      <c r="C83" s="340"/>
+      <c r="D83" s="340"/>
+      <c r="E83" s="341"/>
+      <c r="G83" s="345" t="s">
         <v>1017</v>
       </c>
-      <c r="H83" s="334"/>
-      <c r="I83" s="334"/>
-      <c r="J83" s="335"/>
+      <c r="H83" s="346"/>
+      <c r="I83" s="346"/>
+      <c r="J83" s="347"/>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B84" s="33" t="s">
@@ -29497,11 +29497,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D1" s="327" t="s">
+      <c r="D1" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="328"/>
-      <c r="F1" s="328"/>
+      <c r="E1" s="340"/>
+      <c r="F1" s="340"/>
       <c r="G1" s="42"/>
       <c r="H1" s="59"/>
       <c r="I1" s="92"/>
@@ -29543,12 +29543,12 @@
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D3" s="320" t="s">
+      <c r="D3" s="332" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="322"/>
+      <c r="E3" s="333"/>
+      <c r="F3" s="333"/>
+      <c r="G3" s="334"/>
       <c r="H3" s="119"/>
       <c r="I3" s="121"/>
       <c r="J3" s="121"/>
@@ -29557,12 +29557,12 @@
     </row>
     <row r="5" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="323" t="s">
+      <c r="D6" s="335" t="s">
         <v>618</v>
       </c>
-      <c r="E6" s="324"/>
-      <c r="F6" s="324"/>
-      <c r="G6" s="325"/>
+      <c r="E6" s="336"/>
+      <c r="F6" s="336"/>
+      <c r="G6" s="337"/>
       <c r="H6" s="122"/>
       <c r="I6" s="94"/>
       <c r="J6" s="94"/>
@@ -29571,27 +29571,27 @@
       <c r="M6" s="94"/>
       <c r="N6" s="94"/>
       <c r="O6" s="94"/>
-      <c r="P6" s="323" t="s">
+      <c r="P6" s="335" t="s">
         <v>619</v>
       </c>
-      <c r="Q6" s="324"/>
-      <c r="R6" s="324"/>
-      <c r="S6" s="325"/>
-      <c r="AF6" s="323" t="s">
+      <c r="Q6" s="336"/>
+      <c r="R6" s="336"/>
+      <c r="S6" s="337"/>
+      <c r="AF6" s="335" t="s">
         <v>1</v>
       </c>
-      <c r="AG6" s="324"/>
-      <c r="AH6" s="324"/>
-      <c r="AI6" s="325"/>
+      <c r="AG6" s="336"/>
+      <c r="AH6" s="336"/>
+      <c r="AI6" s="337"/>
       <c r="AJ6" s="153"/>
-      <c r="AK6" s="323" t="s">
+      <c r="AK6" s="335" t="s">
         <v>617</v>
       </c>
-      <c r="AL6" s="324"/>
-      <c r="AM6" s="324"/>
-      <c r="AN6" s="324"/>
-      <c r="AO6" s="324"/>
-      <c r="AP6" s="325"/>
+      <c r="AL6" s="336"/>
+      <c r="AM6" s="336"/>
+      <c r="AN6" s="336"/>
+      <c r="AO6" s="336"/>
+      <c r="AP6" s="337"/>
     </row>
     <row r="7" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D7" s="44" t="s">
@@ -29669,11 +29669,11 @@
       <c r="J8" s="94"/>
       <c r="K8" s="94"/>
       <c r="L8" s="94"/>
-      <c r="M8" s="337" t="s">
+      <c r="M8" s="348" t="s">
         <v>525</v>
       </c>
-      <c r="N8" s="337"/>
-      <c r="O8" s="337"/>
+      <c r="N8" s="348"/>
+      <c r="O8" s="348"/>
       <c r="P8" s="118"/>
       <c r="Q8" s="119"/>
       <c r="R8" s="119"/>
@@ -29694,12 +29694,12 @@
       <c r="AL8" s="154"/>
       <c r="AM8" s="154"/>
       <c r="AN8" s="154"/>
-      <c r="AQ8" s="320" t="s">
+      <c r="AQ8" s="332" t="s">
         <v>19</v>
       </c>
-      <c r="AR8" s="321"/>
-      <c r="AS8" s="321"/>
-      <c r="AT8" s="322"/>
+      <c r="AR8" s="333"/>
+      <c r="AS8" s="333"/>
+      <c r="AT8" s="334"/>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D9" s="284"/>
@@ -29711,11 +29711,11 @@
       <c r="J9" s="121"/>
       <c r="K9" s="121"/>
       <c r="L9" s="121"/>
-      <c r="M9" s="339" t="s">
+      <c r="M9" s="350" t="s">
         <v>526</v>
       </c>
-      <c r="N9" s="339"/>
-      <c r="O9" s="338"/>
+      <c r="N9" s="350"/>
+      <c r="O9" s="349"/>
       <c r="P9" s="118"/>
       <c r="Q9" s="119"/>
       <c r="R9" s="119"/>
@@ -29757,9 +29757,9 @@
       <c r="J10" s="121"/>
       <c r="K10" s="121"/>
       <c r="L10" s="121"/>
-      <c r="M10" s="336"/>
-      <c r="N10" s="336"/>
-      <c r="O10" s="336"/>
+      <c r="M10" s="351"/>
+      <c r="N10" s="351"/>
+      <c r="O10" s="351"/>
       <c r="P10" s="118"/>
       <c r="Q10" s="119"/>
       <c r="R10" s="119"/>
@@ -29784,12 +29784,12 @@
       <c r="AL10" s="154"/>
       <c r="AM10" s="154"/>
       <c r="AN10" s="154"/>
-      <c r="AQ10" s="320" t="s">
+      <c r="AQ10" s="332" t="s">
         <v>54</v>
       </c>
-      <c r="AR10" s="321"/>
-      <c r="AS10" s="321"/>
-      <c r="AT10" s="322"/>
+      <c r="AR10" s="333"/>
+      <c r="AS10" s="333"/>
+      <c r="AT10" s="334"/>
     </row>
     <row r="11" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="284"/>
@@ -29825,12 +29825,12 @@
       <c r="AL11" s="154"/>
       <c r="AM11" s="154"/>
       <c r="AN11" s="154"/>
-      <c r="AQ11" s="320" t="s">
+      <c r="AQ11" s="332" t="s">
         <v>616</v>
       </c>
-      <c r="AR11" s="321"/>
-      <c r="AS11" s="321"/>
-      <c r="AT11" s="322"/>
+      <c r="AR11" s="333"/>
+      <c r="AS11" s="333"/>
+      <c r="AT11" s="334"/>
       <c r="AU11" s="26" t="s">
         <v>263</v>
       </c>
@@ -29856,11 +29856,11 @@
       <c r="J12" s="94"/>
       <c r="K12" s="94"/>
       <c r="L12" s="94"/>
-      <c r="M12" s="340" t="s">
+      <c r="M12" s="352" t="s">
         <v>524</v>
       </c>
-      <c r="N12" s="340"/>
-      <c r="O12" s="340"/>
+      <c r="N12" s="352"/>
+      <c r="O12" s="352"/>
       <c r="P12" s="118"/>
       <c r="Q12" s="119"/>
       <c r="R12" s="119"/>
@@ -29874,12 +29874,12 @@
       <c r="AL12" s="154"/>
       <c r="AM12" s="154"/>
       <c r="AN12" s="154"/>
-      <c r="AQ12" s="320" t="s">
+      <c r="AQ12" s="332" t="s">
         <v>523</v>
       </c>
-      <c r="AR12" s="321"/>
-      <c r="AS12" s="321"/>
-      <c r="AT12" s="322"/>
+      <c r="AR12" s="333"/>
+      <c r="AS12" s="333"/>
+      <c r="AT12" s="334"/>
       <c r="AV12" s="21" t="s">
         <v>612</v>
       </c>
@@ -29895,12 +29895,12 @@
         <v>520</v>
       </c>
       <c r="C13" s="131"/>
-      <c r="D13" s="323" t="s">
+      <c r="D13" s="335" t="s">
         <v>527</v>
       </c>
-      <c r="E13" s="324"/>
-      <c r="F13" s="324"/>
-      <c r="G13" s="325"/>
+      <c r="E13" s="336"/>
+      <c r="F13" s="336"/>
+      <c r="G13" s="337"/>
       <c r="H13" s="167" t="s">
         <v>630</v>
       </c>
@@ -29923,11 +29923,11 @@
       <c r="O13" s="180" t="s">
         <v>634</v>
       </c>
-      <c r="P13" s="323" t="s">
+      <c r="P13" s="335" t="s">
         <v>528</v>
       </c>
-      <c r="Q13" s="324"/>
-      <c r="R13" s="324"/>
+      <c r="Q13" s="336"/>
+      <c r="R13" s="336"/>
       <c r="S13" s="156"/>
       <c r="T13" s="170" t="s">
         <v>655</v>
@@ -29963,18 +29963,18 @@
       <c r="AH13" s="59"/>
       <c r="AI13" s="43"/>
       <c r="AJ13" s="153"/>
-      <c r="AK13" s="320" t="s">
+      <c r="AK13" s="332" t="s">
         <v>527</v>
       </c>
-      <c r="AL13" s="321"/>
-      <c r="AM13" s="321"/>
-      <c r="AN13" s="321"/>
-      <c r="AQ13" s="320" t="s">
+      <c r="AL13" s="333"/>
+      <c r="AM13" s="333"/>
+      <c r="AN13" s="333"/>
+      <c r="AQ13" s="332" t="s">
         <v>609</v>
       </c>
-      <c r="AR13" s="319"/>
-      <c r="AS13" s="319"/>
-      <c r="AT13" s="319"/>
+      <c r="AR13" s="331"/>
+      <c r="AS13" s="331"/>
+      <c r="AT13" s="331"/>
       <c r="AV13" s="21" t="s">
         <v>613</v>
       </c>
@@ -30668,8 +30668,8 @@
       </c>
       <c r="AO30" s="159"/>
       <c r="AP30" s="161"/>
-      <c r="AR30" s="338"/>
-      <c r="AS30" s="338"/>
+      <c r="AR30" s="349"/>
+      <c r="AS30" s="349"/>
     </row>
     <row r="31" spans="1:52" s="26" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="198" t="s">
@@ -31117,8 +31117,8 @@
         <v>88</v>
       </c>
       <c r="AO40" s="159"/>
-      <c r="AR40" s="336"/>
-      <c r="AS40" s="336"/>
+      <c r="AR40" s="351"/>
+      <c r="AS40" s="351"/>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A41" s="151" t="s">
@@ -31349,8 +31349,8 @@
         <v>632</v>
       </c>
       <c r="AP46" s="161"/>
-      <c r="AR46" s="336"/>
-      <c r="AS46" s="336"/>
+      <c r="AR46" s="351"/>
+      <c r="AS46" s="351"/>
     </row>
     <row r="47" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="151" t="s">
@@ -31400,12 +31400,12 @@
         <v>522</v>
       </c>
       <c r="C48" s="178"/>
-      <c r="D48" s="323" t="s">
+      <c r="D48" s="335" t="s">
         <v>527</v>
       </c>
-      <c r="E48" s="324"/>
-      <c r="F48" s="324"/>
-      <c r="G48" s="325"/>
+      <c r="E48" s="336"/>
+      <c r="F48" s="336"/>
+      <c r="G48" s="337"/>
       <c r="H48" s="167" t="s">
         <v>630</v>
       </c>
@@ -31428,11 +31428,11 @@
       <c r="O48" s="180" t="s">
         <v>634</v>
       </c>
-      <c r="P48" s="323" t="s">
+      <c r="P48" s="335" t="s">
         <v>528</v>
       </c>
-      <c r="Q48" s="324"/>
-      <c r="R48" s="324"/>
+      <c r="Q48" s="336"/>
+      <c r="R48" s="336"/>
       <c r="S48" s="189"/>
       <c r="T48" s="170" t="s">
         <v>655</v>
@@ -32772,6 +32772,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="AR46:AS46"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="AR40:AS40"/>
+    <mergeCell ref="AQ11:AT11"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="D6:G6"/>
@@ -32788,13 +32795,6 @@
     <mergeCell ref="AK13:AN13"/>
     <mergeCell ref="AQ10:AT10"/>
     <mergeCell ref="AQ8:AT8"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="AR46:AS46"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="AR40:AS40"/>
-    <mergeCell ref="AQ11:AT11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32856,44 +32856,44 @@
     <row r="1" spans="1:45" x14ac:dyDescent="0.4">
       <c r="B1" s="258"/>
       <c r="C1" s="258"/>
-      <c r="D1" s="327" t="s">
+      <c r="D1" s="339" t="s">
         <v>258</v>
       </c>
-      <c r="E1" s="328"/>
-      <c r="F1" s="328"/>
+      <c r="E1" s="340"/>
+      <c r="F1" s="340"/>
       <c r="G1" s="42"/>
       <c r="H1" s="132"/>
-      <c r="I1" s="327" t="s">
+      <c r="I1" s="339" t="s">
         <v>942</v>
       </c>
-      <c r="J1" s="328"/>
-      <c r="K1" s="328"/>
+      <c r="J1" s="340"/>
+      <c r="K1" s="340"/>
       <c r="L1" s="63"/>
-      <c r="M1" s="360"/>
-      <c r="N1" s="327" t="s">
+      <c r="M1" s="323"/>
+      <c r="N1" s="339" t="s">
         <v>1003</v>
       </c>
-      <c r="O1" s="328"/>
-      <c r="P1" s="328"/>
+      <c r="O1" s="340"/>
+      <c r="P1" s="340"/>
       <c r="Q1" s="42"/>
-      <c r="R1" s="327" t="s">
+      <c r="R1" s="339" t="s">
         <v>1006</v>
       </c>
-      <c r="S1" s="328"/>
-      <c r="T1" s="328"/>
+      <c r="S1" s="340"/>
+      <c r="T1" s="340"/>
       <c r="U1" s="63"/>
-      <c r="V1" s="356"/>
+      <c r="V1" s="320"/>
       <c r="W1" s="278"/>
       <c r="X1" s="278"/>
-      <c r="Y1" s="357"/>
+      <c r="Y1" s="321"/>
       <c r="Z1" s="313"/>
       <c r="AA1" s="313"/>
       <c r="AB1" s="313"/>
-      <c r="AC1" s="327" t="s">
+      <c r="AC1" s="339" t="s">
         <v>1007</v>
       </c>
-      <c r="AD1" s="328"/>
-      <c r="AE1" s="328"/>
+      <c r="AD1" s="340"/>
+      <c r="AE1" s="340"/>
       <c r="AF1" s="63"/>
       <c r="AG1" s="312"/>
       <c r="AH1" s="56"/>
@@ -32919,7 +32919,7 @@
         <v>858</v>
       </c>
       <c r="L2" s="59"/>
-      <c r="M2" s="361"/>
+      <c r="M2" s="324"/>
       <c r="N2" s="311"/>
       <c r="O2" s="285" t="s">
         <v>259</v>
@@ -32965,7 +32965,7 @@
         <v>281</v>
       </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="362"/>
+      <c r="M3" s="325"/>
       <c r="N3" s="311" t="s">
         <v>51</v>
       </c>
@@ -32997,72 +32997,72 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="341" t="s">
+      <c r="D4" s="355" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="342"/>
-      <c r="F4" s="342"/>
-      <c r="G4" s="343"/>
+      <c r="E4" s="356"/>
+      <c r="F4" s="356"/>
+      <c r="G4" s="357"/>
       <c r="H4" s="94"/>
-      <c r="I4" s="341" t="s">
+      <c r="I4" s="355" t="s">
         <v>282</v>
       </c>
-      <c r="J4" s="342"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="343"/>
+      <c r="J4" s="356"/>
+      <c r="K4" s="356"/>
+      <c r="L4" s="357"/>
       <c r="M4" s="245"/>
-      <c r="N4" s="341" t="s">
+      <c r="N4" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="O4" s="342"/>
-      <c r="P4" s="342"/>
-      <c r="Q4" s="343"/>
-      <c r="R4" s="341" t="s">
+      <c r="O4" s="356"/>
+      <c r="P4" s="356"/>
+      <c r="Q4" s="357"/>
+      <c r="R4" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="S4" s="342"/>
-      <c r="T4" s="342"/>
-      <c r="U4" s="343"/>
-      <c r="AC4" s="341" t="s">
+      <c r="S4" s="356"/>
+      <c r="T4" s="356"/>
+      <c r="U4" s="357"/>
+      <c r="AC4" s="355" t="s">
         <v>860</v>
       </c>
-      <c r="AD4" s="342"/>
-      <c r="AE4" s="342"/>
-      <c r="AF4" s="343"/>
+      <c r="AD4" s="356"/>
+      <c r="AE4" s="356"/>
+      <c r="AF4" s="357"/>
     </row>
     <row r="5" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="320" t="s">
+      <c r="D5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="E5" s="321"/>
-      <c r="F5" s="321"/>
-      <c r="G5" s="322"/>
+      <c r="E5" s="333"/>
+      <c r="F5" s="333"/>
+      <c r="G5" s="334"/>
       <c r="H5" s="314"/>
-      <c r="I5" s="320" t="s">
+      <c r="I5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="J5" s="321"/>
-      <c r="K5" s="321"/>
-      <c r="L5" s="322"/>
+      <c r="J5" s="333"/>
+      <c r="K5" s="333"/>
+      <c r="L5" s="334"/>
       <c r="M5" s="99"/>
-      <c r="N5" s="320" t="s">
+      <c r="N5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="O5" s="321"/>
-      <c r="P5" s="321"/>
-      <c r="Q5" s="322"/>
-      <c r="R5" s="320" t="s">
+      <c r="O5" s="333"/>
+      <c r="P5" s="333"/>
+      <c r="Q5" s="334"/>
+      <c r="R5" s="332" t="s">
         <v>899</v>
       </c>
-      <c r="S5" s="321"/>
-      <c r="T5" s="321"/>
-      <c r="U5" s="322"/>
-      <c r="AC5" s="320" t="s">
+      <c r="S5" s="333"/>
+      <c r="T5" s="333"/>
+      <c r="U5" s="334"/>
+      <c r="AC5" s="332" t="s">
         <v>899</v>
       </c>
-      <c r="AD5" s="321"/>
-      <c r="AE5" s="321"/>
-      <c r="AF5" s="322"/>
+      <c r="AD5" s="333"/>
+      <c r="AE5" s="333"/>
+      <c r="AF5" s="334"/>
     </row>
     <row r="6" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="206" t="s">
@@ -33070,52 +33070,52 @@
       </c>
       <c r="B6" s="258"/>
       <c r="C6" s="258"/>
-      <c r="D6" s="323" t="s">
+      <c r="D6" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="324"/>
-      <c r="F6" s="324"/>
-      <c r="G6" s="325"/>
+      <c r="E6" s="336"/>
+      <c r="F6" s="336"/>
+      <c r="G6" s="337"/>
       <c r="H6" s="313"/>
       <c r="I6" s="55"/>
       <c r="J6" s="56"/>
       <c r="K6" s="56"/>
       <c r="L6" s="56"/>
-      <c r="M6" s="363"/>
-      <c r="N6" s="326" t="s">
+      <c r="M6" s="326"/>
+      <c r="N6" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="324"/>
-      <c r="P6" s="324"/>
-      <c r="Q6" s="324"/>
+      <c r="O6" s="336"/>
+      <c r="P6" s="336"/>
+      <c r="Q6" s="336"/>
       <c r="R6" s="55"/>
       <c r="S6" s="56"/>
       <c r="T6" s="56"/>
       <c r="U6" s="56"/>
-      <c r="V6" s="356"/>
+      <c r="V6" s="320"/>
       <c r="W6" s="278"/>
       <c r="X6" s="278"/>
-      <c r="Y6" s="357"/>
+      <c r="Y6" s="321"/>
       <c r="Z6" s="313"/>
       <c r="AA6" s="313"/>
       <c r="AB6" s="313"/>
-      <c r="AC6" s="323" t="s">
+      <c r="AC6" s="335" t="s">
         <v>1047</v>
       </c>
-      <c r="AD6" s="324"/>
-      <c r="AE6" s="324"/>
-      <c r="AF6" s="325"/>
+      <c r="AD6" s="336"/>
+      <c r="AE6" s="336"/>
+      <c r="AF6" s="337"/>
       <c r="AG6" s="312"/>
       <c r="AH6" s="56"/>
       <c r="AI6" s="56"/>
       <c r="AJ6" s="56"/>
       <c r="AK6" s="57"/>
-      <c r="AL6" s="323" t="s">
+      <c r="AL6" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="AM6" s="324"/>
-      <c r="AN6" s="324"/>
-      <c r="AO6" s="325"/>
+      <c r="AM6" s="336"/>
+      <c r="AN6" s="336"/>
+      <c r="AO6" s="337"/>
       <c r="AP6" s="210"/>
       <c r="AQ6" s="211"/>
       <c r="AR6" s="211"/>
@@ -33127,45 +33127,45 @@
         <v>917</v>
       </c>
       <c r="C7" s="259"/>
-      <c r="D7" s="323" t="s">
+      <c r="D7" s="335" t="s">
         <v>618</v>
       </c>
-      <c r="E7" s="324"/>
-      <c r="F7" s="324"/>
-      <c r="G7" s="325"/>
+      <c r="E7" s="336"/>
+      <c r="F7" s="336"/>
+      <c r="G7" s="337"/>
       <c r="H7" s="147"/>
-      <c r="I7" s="323" t="s">
+      <c r="I7" s="335" t="s">
         <v>822</v>
       </c>
-      <c r="J7" s="324"/>
-      <c r="K7" s="324"/>
-      <c r="L7" s="325"/>
-      <c r="M7" s="364"/>
-      <c r="N7" s="323" t="s">
+      <c r="J7" s="336"/>
+      <c r="K7" s="336"/>
+      <c r="L7" s="337"/>
+      <c r="M7" s="327"/>
+      <c r="N7" s="335" t="s">
         <v>619</v>
       </c>
-      <c r="O7" s="324"/>
-      <c r="P7" s="324"/>
-      <c r="Q7" s="325"/>
-      <c r="R7" s="323"/>
-      <c r="S7" s="324"/>
-      <c r="T7" s="324"/>
-      <c r="U7" s="325"/>
+      <c r="O7" s="336"/>
+      <c r="P7" s="336"/>
+      <c r="Q7" s="337"/>
+      <c r="R7" s="335"/>
+      <c r="S7" s="336"/>
+      <c r="T7" s="336"/>
+      <c r="U7" s="337"/>
       <c r="V7" s="358" t="s">
         <v>1048</v>
       </c>
-      <c r="W7" s="354"/>
-      <c r="X7" s="354"/>
-      <c r="Y7" s="355"/>
+      <c r="W7" s="359"/>
+      <c r="X7" s="359"/>
+      <c r="Y7" s="360"/>
       <c r="Z7" s="147"/>
       <c r="AA7" s="147"/>
       <c r="AB7" s="147"/>
-      <c r="AC7" s="323" t="s">
+      <c r="AC7" s="335" t="s">
         <v>1005</v>
       </c>
-      <c r="AD7" s="324"/>
-      <c r="AE7" s="324"/>
-      <c r="AF7" s="325"/>
+      <c r="AD7" s="336"/>
+      <c r="AE7" s="336"/>
+      <c r="AF7" s="337"/>
       <c r="AG7" s="44"/>
       <c r="AH7" s="28"/>
       <c r="AI7" s="28"/>
@@ -33175,12 +33175,12 @@
       <c r="AM7" s="213"/>
       <c r="AN7" s="213"/>
       <c r="AO7" s="214"/>
-      <c r="AP7" s="323" t="s">
+      <c r="AP7" s="335" t="s">
         <v>823</v>
       </c>
-      <c r="AQ7" s="324"/>
-      <c r="AR7" s="324"/>
-      <c r="AS7" s="325"/>
+      <c r="AQ7" s="336"/>
+      <c r="AR7" s="336"/>
+      <c r="AS7" s="337"/>
     </row>
     <row r="8" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="206">
@@ -33202,7 +33202,7 @@
       <c r="G8" s="245" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="353"/>
+      <c r="H8" s="319"/>
       <c r="I8" s="234" t="s">
         <v>629</v>
       </c>
@@ -33273,7 +33273,7 @@
       <c r="AF8" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="AG8" s="353" t="s">
+      <c r="AG8" s="319" t="s">
         <v>1046</v>
       </c>
       <c r="AH8" s="26" t="s">
@@ -33326,25 +33326,25 @@
       <c r="F9" s="285"/>
       <c r="G9" s="286"/>
       <c r="H9" s="314"/>
-      <c r="I9" s="344" t="s">
+      <c r="I9" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J9" s="345"/>
-      <c r="K9" s="345"/>
-      <c r="L9" s="345"/>
-      <c r="M9" s="365" t="s">
+      <c r="J9" s="354"/>
+      <c r="K9" s="354"/>
+      <c r="L9" s="354"/>
+      <c r="M9" s="328" t="s">
         <v>964</v>
       </c>
       <c r="N9" s="285"/>
       <c r="O9" s="285"/>
       <c r="P9" s="285"/>
       <c r="Q9" s="285"/>
-      <c r="R9" s="344" t="s">
+      <c r="R9" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="S9" s="345"/>
-      <c r="T9" s="345"/>
-      <c r="U9" s="345"/>
+      <c r="S9" s="354"/>
+      <c r="T9" s="354"/>
+      <c r="U9" s="354"/>
       <c r="AC9" s="284"/>
       <c r="AD9" s="285"/>
       <c r="AE9" s="285"/>
@@ -33551,12 +33551,12 @@
         <v>575</v>
       </c>
       <c r="H15" s="81"/>
-      <c r="I15" s="344" t="s">
+      <c r="I15" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J15" s="345"/>
-      <c r="K15" s="345"/>
-      <c r="L15" s="345"/>
+      <c r="J15" s="354"/>
+      <c r="K15" s="354"/>
+      <c r="L15" s="354"/>
       <c r="M15" s="99"/>
       <c r="N15" s="74" t="s">
         <v>155</v>
@@ -33566,12 +33566,12 @@
       </c>
       <c r="P15" s="26"/>
       <c r="Q15" s="21"/>
-      <c r="R15" s="344" t="s">
+      <c r="R15" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="S15" s="345"/>
-      <c r="T15" s="345"/>
-      <c r="U15" s="345"/>
+      <c r="S15" s="354"/>
+      <c r="T15" s="354"/>
+      <c r="U15" s="354"/>
       <c r="AC15" s="176"/>
       <c r="AD15" s="81"/>
       <c r="AE15" s="12"/>
@@ -33659,7 +33659,7 @@
       <c r="U17" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="AB17" s="359"/>
+      <c r="AB17" s="322"/>
       <c r="AC17" s="176"/>
       <c r="AD17" s="81"/>
       <c r="AE17" s="12"/>
@@ -33886,12 +33886,12 @@
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="81"/>
-      <c r="I23" s="344" t="s">
+      <c r="I23" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J23" s="345"/>
-      <c r="K23" s="345"/>
-      <c r="L23" s="345"/>
+      <c r="J23" s="354"/>
+      <c r="K23" s="354"/>
+      <c r="L23" s="354"/>
       <c r="M23" s="164"/>
       <c r="O23" s="78" t="s">
         <v>242</v>
@@ -33902,12 +33902,12 @@
       <c r="Q23" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="R23" s="344" t="s">
+      <c r="R23" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="S23" s="345"/>
-      <c r="T23" s="345"/>
-      <c r="U23" s="345"/>
+      <c r="S23" s="354"/>
+      <c r="T23" s="354"/>
+      <c r="U23" s="354"/>
       <c r="X23" s="34"/>
       <c r="Y23" s="34" t="s">
         <v>470</v>
@@ -34086,7 +34086,7 @@
         <v>573</v>
       </c>
       <c r="H28" s="81"/>
-      <c r="M28" s="366"/>
+      <c r="M28" s="329"/>
       <c r="N28" s="78" t="s">
         <v>252</v>
       </c>
@@ -34126,7 +34126,7 @@
         <v>575</v>
       </c>
       <c r="H29" s="81"/>
-      <c r="M29" s="366"/>
+      <c r="M29" s="329"/>
       <c r="N29" s="78" t="s">
         <v>255</v>
       </c>
@@ -34170,7 +34170,7 @@
         <v>577</v>
       </c>
       <c r="H30" s="81"/>
-      <c r="M30" s="366"/>
+      <c r="M30" s="329"/>
       <c r="N30" s="78" t="s">
         <v>257</v>
       </c>
@@ -34211,12 +34211,12 @@
       <c r="F31" s="73" t="s">
         <v>576</v>
       </c>
-      <c r="I31" s="344" t="s">
+      <c r="I31" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J31" s="345"/>
-      <c r="K31" s="345"/>
-      <c r="L31" s="345"/>
+      <c r="J31" s="354"/>
+      <c r="K31" s="354"/>
+      <c r="L31" s="354"/>
       <c r="M31" s="164"/>
       <c r="O31" s="78" t="s">
         <v>256</v>
@@ -34227,12 +34227,12 @@
       <c r="Q31" s="78" t="s">
         <v>246</v>
       </c>
-      <c r="R31" s="344" t="s">
+      <c r="R31" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="S31" s="345"/>
-      <c r="T31" s="345"/>
-      <c r="U31" s="345"/>
+      <c r="S31" s="354"/>
+      <c r="T31" s="354"/>
+      <c r="U31" s="354"/>
       <c r="X31" s="34"/>
       <c r="Y31" s="34" t="s">
         <v>742</v>
@@ -34264,7 +34264,7 @@
       <c r="L32" s="75" t="s">
         <v>573</v>
       </c>
-      <c r="M32" s="366"/>
+      <c r="M32" s="329"/>
       <c r="N32" s="81"/>
       <c r="O32" s="81"/>
       <c r="P32" s="78" t="s">
@@ -34306,7 +34306,7 @@
       <c r="L33" s="75" t="s">
         <v>575</v>
       </c>
-      <c r="M33" s="366"/>
+      <c r="M33" s="329"/>
       <c r="Q33" s="78" t="s">
         <v>251</v>
       </c>
@@ -34341,7 +34341,7 @@
       <c r="L34" s="75" t="s">
         <v>577</v>
       </c>
-      <c r="M34" s="366"/>
+      <c r="M34" s="329"/>
       <c r="P34" s="81"/>
       <c r="Q34" s="81"/>
       <c r="U34" s="78" t="s">
@@ -34373,7 +34373,7 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="110"/>
-      <c r="M35" s="366"/>
+      <c r="M35" s="329"/>
       <c r="N35" s="233" t="s">
         <v>784</v>
       </c>
@@ -34408,7 +34408,7 @@
         <v>573</v>
       </c>
       <c r="H36" s="81"/>
-      <c r="M36" s="366"/>
+      <c r="M36" s="329"/>
       <c r="N36" s="78" t="s">
         <v>463</v>
       </c>
@@ -34448,7 +34448,7 @@
         <v>575</v>
       </c>
       <c r="H37" s="81"/>
-      <c r="M37" s="366"/>
+      <c r="M37" s="329"/>
       <c r="N37" s="78" t="s">
         <v>464</v>
       </c>
@@ -34485,7 +34485,7 @@
         <v>577</v>
       </c>
       <c r="H38" s="81"/>
-      <c r="M38" s="366"/>
+      <c r="M38" s="329"/>
       <c r="N38" s="78" t="s">
         <v>264</v>
       </c>
@@ -34521,12 +34521,12 @@
       <c r="F39" s="73" t="s">
         <v>576</v>
       </c>
-      <c r="I39" s="344" t="s">
+      <c r="I39" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J39" s="345"/>
-      <c r="K39" s="345"/>
-      <c r="L39" s="345"/>
+      <c r="J39" s="354"/>
+      <c r="K39" s="354"/>
+      <c r="L39" s="354"/>
       <c r="M39" s="164"/>
       <c r="N39" s="12"/>
       <c r="O39" s="78" t="s">
@@ -34534,12 +34534,12 @@
       </c>
       <c r="P39" s="81"/>
       <c r="Q39" s="81"/>
-      <c r="R39" s="344" t="s">
+      <c r="R39" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="S39" s="345"/>
-      <c r="T39" s="345"/>
-      <c r="U39" s="345"/>
+      <c r="S39" s="354"/>
+      <c r="T39" s="354"/>
+      <c r="U39" s="354"/>
       <c r="X39" s="34"/>
       <c r="Y39" s="34" t="s">
         <v>746</v>
@@ -34569,7 +34569,7 @@
       <c r="L40" s="78" t="s">
         <v>468</v>
       </c>
-      <c r="M40" s="366"/>
+      <c r="M40" s="329"/>
       <c r="N40" s="12"/>
       <c r="O40" s="81"/>
       <c r="P40" s="81"/>
@@ -34608,7 +34608,7 @@
       <c r="L41" s="78" t="s">
         <v>469</v>
       </c>
-      <c r="M41" s="366"/>
+      <c r="M41" s="329"/>
       <c r="N41" s="81"/>
       <c r="O41" s="81"/>
       <c r="P41" s="81"/>
@@ -34642,7 +34642,7 @@
       <c r="L42" s="78" t="s">
         <v>470</v>
       </c>
-      <c r="M42" s="366"/>
+      <c r="M42" s="329"/>
       <c r="U42" s="75" t="s">
         <v>577</v>
       </c>
@@ -34670,7 +34670,7 @@
       <c r="B43" s="164">
         <v>5</v>
       </c>
-      <c r="M43" s="366"/>
+      <c r="M43" s="329"/>
       <c r="X43" s="34"/>
       <c r="Y43" s="34" t="s">
         <v>760</v>
@@ -34785,13 +34785,13 @@
       </c>
       <c r="G47" s="82"/>
       <c r="H47" s="81"/>
-      <c r="I47" s="344" t="s">
+      <c r="I47" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J47" s="345"/>
-      <c r="K47" s="345"/>
-      <c r="L47" s="345"/>
-      <c r="M47" s="367"/>
+      <c r="J47" s="354"/>
+      <c r="K47" s="354"/>
+      <c r="L47" s="354"/>
+      <c r="M47" s="330"/>
       <c r="N47" s="81"/>
       <c r="O47" s="73" t="s">
         <v>576</v>
@@ -34986,13 +34986,13 @@
       <c r="B59" s="164">
         <v>1</v>
       </c>
-      <c r="I59" s="344" t="s">
+      <c r="I59" s="353" t="s">
         <v>1002</v>
       </c>
-      <c r="J59" s="345"/>
-      <c r="K59" s="345"/>
-      <c r="L59" s="345"/>
-      <c r="M59" s="367"/>
+      <c r="J59" s="354"/>
+      <c r="K59" s="354"/>
+      <c r="L59" s="354"/>
+      <c r="M59" s="330"/>
       <c r="AE59" s="76" t="s">
         <v>892</v>
       </c>
@@ -35387,6 +35387,31 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="AP7:AS7"/>
+    <mergeCell ref="AL6:AO6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="V7:Y7"/>
     <mergeCell ref="I59:L59"/>
     <mergeCell ref="I47:L47"/>
     <mergeCell ref="R1:T1"/>
@@ -35400,31 +35425,6 @@
     <mergeCell ref="I23:L23"/>
     <mergeCell ref="I31:L31"/>
     <mergeCell ref="I39:L39"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="AP7:AS7"/>
-    <mergeCell ref="AL6:AO6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="N5:Q5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35481,17 +35481,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.4">
-      <c r="B1" s="327" t="s">
+      <c r="B1" s="339" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="328"/>
-      <c r="D1" s="328"/>
+      <c r="C1" s="340"/>
+      <c r="D1" s="340"/>
       <c r="E1" s="42"/>
-      <c r="F1" s="327" t="s">
+      <c r="F1" s="339" t="s">
         <v>942</v>
       </c>
-      <c r="G1" s="328"/>
-      <c r="H1" s="328"/>
+      <c r="G1" s="340"/>
+      <c r="H1" s="340"/>
       <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.4">
@@ -35534,61 +35534,61 @@
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="341" t="s">
+      <c r="B4" s="355" t="s">
         <v>941</v>
       </c>
-      <c r="C4" s="342"/>
-      <c r="D4" s="342"/>
-      <c r="E4" s="343"/>
-      <c r="F4" s="341" t="s">
+      <c r="C4" s="356"/>
+      <c r="D4" s="356"/>
+      <c r="E4" s="357"/>
+      <c r="F4" s="355" t="s">
         <v>282</v>
       </c>
-      <c r="G4" s="342"/>
-      <c r="H4" s="342"/>
-      <c r="I4" s="343"/>
+      <c r="G4" s="356"/>
+      <c r="H4" s="356"/>
+      <c r="I4" s="357"/>
     </row>
     <row r="5" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="320" t="s">
+      <c r="B5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="C5" s="321"/>
-      <c r="D5" s="321"/>
-      <c r="E5" s="322"/>
-      <c r="F5" s="320" t="s">
+      <c r="C5" s="333"/>
+      <c r="D5" s="333"/>
+      <c r="E5" s="334"/>
+      <c r="F5" s="332" t="s">
         <v>856</v>
       </c>
-      <c r="G5" s="321"/>
-      <c r="H5" s="321"/>
-      <c r="I5" s="322"/>
+      <c r="G5" s="333"/>
+      <c r="H5" s="333"/>
+      <c r="I5" s="334"/>
     </row>
     <row r="6" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="206" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="323" t="s">
+      <c r="B6" s="335" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="324"/>
-      <c r="D6" s="324"/>
-      <c r="E6" s="325"/>
-      <c r="F6" s="326" t="s">
+      <c r="C6" s="336"/>
+      <c r="D6" s="336"/>
+      <c r="E6" s="337"/>
+      <c r="F6" s="338" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="324"/>
-      <c r="H6" s="324"/>
-      <c r="I6" s="324"/>
-      <c r="J6" s="323" t="s">
+      <c r="G6" s="336"/>
+      <c r="H6" s="336"/>
+      <c r="I6" s="336"/>
+      <c r="J6" s="335" t="s">
         <v>184</v>
       </c>
-      <c r="K6" s="324"/>
-      <c r="L6" s="324"/>
-      <c r="M6" s="325"/>
-      <c r="N6" s="323" t="s">
+      <c r="K6" s="336"/>
+      <c r="L6" s="336"/>
+      <c r="M6" s="337"/>
+      <c r="N6" s="335" t="s">
         <v>187</v>
       </c>
-      <c r="O6" s="324"/>
-      <c r="P6" s="324"/>
-      <c r="Q6" s="325"/>
+      <c r="O6" s="336"/>
+      <c r="P6" s="336"/>
+      <c r="Q6" s="337"/>
       <c r="V6" s="55"/>
       <c r="W6" s="56"/>
       <c r="X6" s="56"/>
@@ -35617,24 +35617,24 @@
     </row>
     <row r="7" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="206"/>
-      <c r="B7" s="323" t="s">
+      <c r="B7" s="335" t="s">
         <v>618</v>
       </c>
-      <c r="C7" s="324"/>
-      <c r="D7" s="324"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="323" t="s">
+      <c r="C7" s="336"/>
+      <c r="D7" s="336"/>
+      <c r="E7" s="337"/>
+      <c r="F7" s="335" t="s">
         <v>619</v>
       </c>
-      <c r="G7" s="324"/>
-      <c r="H7" s="324"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="323" t="s">
+      <c r="G7" s="336"/>
+      <c r="H7" s="336"/>
+      <c r="I7" s="337"/>
+      <c r="J7" s="335" t="s">
         <v>778</v>
       </c>
-      <c r="K7" s="324"/>
-      <c r="L7" s="324"/>
-      <c r="M7" s="325"/>
+      <c r="K7" s="336"/>
+      <c r="L7" s="336"/>
+      <c r="M7" s="337"/>
       <c r="N7" s="203"/>
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
@@ -39326,6 +39326,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B4:E4"/>
@@ -39334,11 +39339,6 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
220505-v5 OK to sim, some problems in base addr gen
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDCA582-A67D-47B3-BAF9-FAC2F2684549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACC0ADC-7661-4D26-B359-0855AFA29A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="1" activeTab="9" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="1" activeTab="8" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD1,2" sheetId="3" r:id="rId1"/>
@@ -5540,6 +5540,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5554,33 +5578,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5590,6 +5590,9 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5598,9 +5601,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6733,8 +6733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE96E198-A134-4E8D-93D2-A301FB776858}">
   <dimension ref="A1:X163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -6766,25 +6766,25 @@
       <c r="C1" s="361"/>
       <c r="D1" s="349"/>
       <c r="E1" s="351"/>
-      <c r="F1" s="373" t="s">
+      <c r="F1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="375"/>
-      <c r="J1" s="373" t="s">
+      <c r="G1" s="371"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="372"/>
+      <c r="J1" s="370" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="375"/>
+      <c r="K1" s="371"/>
+      <c r="L1" s="371"/>
+      <c r="M1" s="372"/>
       <c r="N1" s="323"/>
-      <c r="O1" s="373" t="s">
+      <c r="O1" s="370" t="s">
         <v>383</v>
       </c>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="374"/>
-      <c r="R1" s="375"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="371"/>
+      <c r="R1" s="372"/>
       <c r="S1" s="324"/>
       <c r="T1" s="324"/>
     </row>
@@ -6888,12 +6888,12 @@
       <c r="T3" s="328" t="s">
         <v>932</v>
       </c>
-      <c r="U3" s="378" t="s">
+      <c r="U3" s="374" t="s">
         <v>832</v>
       </c>
-      <c r="V3" s="378"/>
-      <c r="W3" s="378"/>
-      <c r="X3" s="381"/>
+      <c r="V3" s="374"/>
+      <c r="W3" s="374"/>
+      <c r="X3" s="375"/>
     </row>
     <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="241" t="s">
@@ -6963,12 +6963,12 @@
       <c r="Q5" s="240"/>
       <c r="R5" s="49"/>
       <c r="S5" s="332"/>
-      <c r="U5" s="371" t="s">
+      <c r="U5" s="379" t="s">
         <v>761</v>
       </c>
-      <c r="V5" s="371"/>
-      <c r="W5" s="371"/>
-      <c r="X5" s="372"/>
+      <c r="V5" s="379"/>
+      <c r="W5" s="379"/>
+      <c r="X5" s="380"/>
     </row>
     <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="241" t="s">
@@ -6997,12 +6997,12 @@
       <c r="N6" s="335"/>
       <c r="Q6" s="240"/>
       <c r="R6" s="49"/>
-      <c r="U6" s="371" t="s">
+      <c r="U6" s="379" t="s">
         <v>833</v>
       </c>
-      <c r="V6" s="371"/>
-      <c r="W6" s="371"/>
-      <c r="X6" s="372"/>
+      <c r="V6" s="379"/>
+      <c r="W6" s="379"/>
+      <c r="X6" s="380"/>
     </row>
     <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="241" t="s">
@@ -9303,34 +9303,34 @@
     <row r="1" spans="1:33" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C1" s="349"/>
       <c r="D1" s="351"/>
-      <c r="E1" s="373" t="s">
+      <c r="E1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="374"/>
-      <c r="G1" s="374"/>
-      <c r="H1" s="375"/>
-      <c r="I1" s="373" t="s">
+      <c r="F1" s="371"/>
+      <c r="G1" s="371"/>
+      <c r="H1" s="372"/>
+      <c r="I1" s="370" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="374"/>
-      <c r="K1" s="374"/>
-      <c r="L1" s="375"/>
+      <c r="J1" s="371"/>
+      <c r="K1" s="371"/>
+      <c r="L1" s="372"/>
       <c r="M1" s="323"/>
       <c r="N1" s="325"/>
-      <c r="O1" s="373" t="s">
+      <c r="O1" s="370" t="s">
         <v>383</v>
       </c>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="374"/>
-      <c r="R1" s="375"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="371"/>
+      <c r="R1" s="372"/>
       <c r="S1" s="324"/>
       <c r="T1" s="324"/>
-      <c r="U1" s="373" t="s">
+      <c r="U1" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="V1" s="374"/>
-      <c r="W1" s="374"/>
-      <c r="X1" s="375"/>
+      <c r="V1" s="371"/>
+      <c r="W1" s="371"/>
+      <c r="X1" s="372"/>
       <c r="Y1" s="40"/>
       <c r="Z1" s="40"/>
       <c r="AA1" s="40"/>
@@ -9440,12 +9440,12 @@
       <c r="V3" s="33"/>
       <c r="W3" s="33"/>
       <c r="X3" s="36"/>
-      <c r="Y3" s="377" t="s">
+      <c r="Y3" s="373" t="s">
         <v>17</v>
       </c>
-      <c r="Z3" s="378"/>
-      <c r="AA3" s="378"/>
-      <c r="AB3" s="381"/>
+      <c r="Z3" s="374"/>
+      <c r="AA3" s="374"/>
+      <c r="AB3" s="375"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A4" s="241" t="s">
@@ -9518,12 +9518,12 @@
       <c r="V5" s="33"/>
       <c r="W5" s="33"/>
       <c r="X5" s="36"/>
-      <c r="Y5" s="370" t="s">
+      <c r="Y5" s="378" t="s">
         <v>236</v>
       </c>
-      <c r="Z5" s="371"/>
-      <c r="AA5" s="371"/>
-      <c r="AB5" s="372"/>
+      <c r="Z5" s="379"/>
+      <c r="AA5" s="379"/>
+      <c r="AB5" s="380"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A6" s="241" t="s">
@@ -9556,12 +9556,12 @@
       <c r="V6" s="33"/>
       <c r="W6" s="33"/>
       <c r="X6" s="36"/>
-      <c r="Y6" s="370" t="s">
+      <c r="Y6" s="378" t="s">
         <v>237</v>
       </c>
-      <c r="Z6" s="371"/>
-      <c r="AA6" s="371"/>
-      <c r="AB6" s="372"/>
+      <c r="Z6" s="379"/>
+      <c r="AA6" s="379"/>
+      <c r="AB6" s="380"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A7" s="241" t="s">
@@ -12002,30 +12002,30 @@
     <row r="1" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="241"/>
       <c r="B1" s="228"/>
-      <c r="C1" s="373" t="s">
+      <c r="C1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="375"/>
-      <c r="G1" s="373" t="s">
+      <c r="D1" s="371"/>
+      <c r="E1" s="371"/>
+      <c r="F1" s="372"/>
+      <c r="G1" s="370" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="375"/>
-      <c r="K1" s="373" t="s">
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
+      <c r="J1" s="372"/>
+      <c r="K1" s="370" t="s">
         <v>383</v>
       </c>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
-      <c r="N1" s="375"/>
-      <c r="O1" s="373" t="s">
+      <c r="L1" s="371"/>
+      <c r="M1" s="371"/>
+      <c r="N1" s="372"/>
+      <c r="O1" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="374"/>
-      <c r="R1" s="375"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="371"/>
+      <c r="R1" s="372"/>
       <c r="S1" s="191"/>
       <c r="T1" s="191"/>
       <c r="U1" s="191"/>
@@ -12124,12 +12124,12 @@
       <c r="P3" s="186"/>
       <c r="Q3" s="186"/>
       <c r="R3" s="187"/>
-      <c r="S3" s="377" t="s">
+      <c r="S3" s="373" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="378"/>
-      <c r="U3" s="378"/>
-      <c r="V3" s="381"/>
+      <c r="T3" s="374"/>
+      <c r="U3" s="374"/>
+      <c r="V3" s="375"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="241" t="s">
@@ -12198,12 +12198,12 @@
       <c r="P5" s="186"/>
       <c r="Q5" s="186"/>
       <c r="R5" s="187"/>
-      <c r="S5" s="370" t="s">
+      <c r="S5" s="378" t="s">
         <v>236</v>
       </c>
-      <c r="T5" s="371"/>
-      <c r="U5" s="371"/>
-      <c r="V5" s="372"/>
+      <c r="T5" s="379"/>
+      <c r="U5" s="379"/>
+      <c r="V5" s="380"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="241" t="s">
@@ -12234,12 +12234,12 @@
       <c r="P6" s="186"/>
       <c r="Q6" s="186"/>
       <c r="R6" s="187"/>
-      <c r="S6" s="370" t="s">
+      <c r="S6" s="378" t="s">
         <v>237</v>
       </c>
-      <c r="T6" s="371"/>
-      <c r="U6" s="371"/>
-      <c r="V6" s="372"/>
+      <c r="T6" s="379"/>
+      <c r="U6" s="379"/>
+      <c r="V6" s="380"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="241" t="s">
@@ -14846,36 +14846,36 @@
   <sheetData>
     <row r="1" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="18"/>
-      <c r="C1" s="373" t="s">
+      <c r="C1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="375"/>
-      <c r="G1" s="376" t="s">
+      <c r="D1" s="371"/>
+      <c r="E1" s="371"/>
+      <c r="F1" s="372"/>
+      <c r="G1" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="374"/>
-      <c r="K1" s="373" t="s">
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
+      <c r="J1" s="371"/>
+      <c r="K1" s="370" t="s">
         <v>383</v>
       </c>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
-      <c r="N1" s="375"/>
-      <c r="O1" s="373" t="s">
+      <c r="L1" s="371"/>
+      <c r="M1" s="371"/>
+      <c r="N1" s="372"/>
+      <c r="O1" s="370" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="374"/>
-      <c r="R1" s="375"/>
-      <c r="Z1" s="373" t="s">
+      <c r="P1" s="371"/>
+      <c r="Q1" s="371"/>
+      <c r="R1" s="372"/>
+      <c r="Z1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="AA1" s="374"/>
-      <c r="AB1" s="374"/>
-      <c r="AC1" s="375"/>
+      <c r="AA1" s="371"/>
+      <c r="AB1" s="371"/>
+      <c r="AC1" s="372"/>
     </row>
     <row r="2" spans="2:29" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="18"/>
@@ -14944,33 +14944,33 @@
       <c r="B3" s="18">
         <v>0</v>
       </c>
-      <c r="C3" s="377" t="s">
+      <c r="C3" s="373" t="s">
         <v>219</v>
       </c>
-      <c r="D3" s="378"/>
-      <c r="E3" s="378"/>
-      <c r="F3" s="381"/>
-      <c r="G3" s="377"/>
-      <c r="H3" s="378"/>
-      <c r="I3" s="378"/>
-      <c r="J3" s="381"/>
+      <c r="D3" s="374"/>
+      <c r="E3" s="374"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="373"/>
+      <c r="H3" s="374"/>
+      <c r="I3" s="374"/>
+      <c r="J3" s="375"/>
       <c r="K3" s="185"/>
       <c r="O3" s="185"/>
       <c r="P3" s="186"/>
       <c r="Q3" s="186"/>
       <c r="R3" s="187"/>
-      <c r="S3" s="377" t="s">
+      <c r="S3" s="373" t="s">
         <v>343</v>
       </c>
-      <c r="T3" s="378"/>
-      <c r="U3" s="378"/>
-      <c r="V3" s="381"/>
-      <c r="Z3" s="377" t="s">
+      <c r="T3" s="374"/>
+      <c r="U3" s="374"/>
+      <c r="V3" s="375"/>
+      <c r="Z3" s="373" t="s">
         <v>219</v>
       </c>
-      <c r="AA3" s="378"/>
-      <c r="AB3" s="378"/>
-      <c r="AC3" s="381"/>
+      <c r="AA3" s="374"/>
+      <c r="AB3" s="374"/>
+      <c r="AC3" s="375"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="34" t="s">
@@ -15027,12 +15027,12 @@
       <c r="P5" s="186"/>
       <c r="Q5" s="186"/>
       <c r="R5" s="187"/>
-      <c r="S5" s="370" t="s">
+      <c r="S5" s="378" t="s">
         <v>443</v>
       </c>
-      <c r="T5" s="371"/>
-      <c r="U5" s="371"/>
-      <c r="V5" s="372"/>
+      <c r="T5" s="379"/>
+      <c r="U5" s="379"/>
+      <c r="V5" s="380"/>
       <c r="W5" s="64" t="s">
         <v>445</v>
       </c>
@@ -15062,12 +15062,12 @@
       <c r="P6" s="186"/>
       <c r="Q6" s="186"/>
       <c r="R6" s="187"/>
-      <c r="S6" s="370" t="s">
+      <c r="S6" s="378" t="s">
         <v>360</v>
       </c>
-      <c r="T6" s="371"/>
-      <c r="U6" s="371"/>
-      <c r="V6" s="372"/>
+      <c r="T6" s="379"/>
+      <c r="U6" s="379"/>
+      <c r="V6" s="380"/>
       <c r="Z6" s="185"/>
       <c r="AA6" s="186"/>
       <c r="AB6" s="186"/>
@@ -16426,17 +16426,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="S5:V5"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="Z3:AC3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16471,57 +16471,57 @@
       <c r="A1" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="373" t="s">
+      <c r="B1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="374"/>
-      <c r="D1" s="374"/>
-      <c r="E1" s="375"/>
-      <c r="F1" s="376" t="s">
+      <c r="C1" s="371"/>
+      <c r="D1" s="371"/>
+      <c r="E1" s="372"/>
+      <c r="F1" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="373" t="s">
+      <c r="G1" s="371"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
+      <c r="J1" s="370" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="375"/>
-      <c r="N1" s="373" t="s">
+      <c r="K1" s="371"/>
+      <c r="L1" s="371"/>
+      <c r="M1" s="372"/>
+      <c r="N1" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="O1" s="374"/>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="375"/>
-      <c r="R1" s="377" t="s">
+      <c r="O1" s="371"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="372"/>
+      <c r="R1" s="373" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="378"/>
-      <c r="T1" s="378"/>
+      <c r="S1" s="374"/>
+      <c r="T1" s="374"/>
       <c r="U1" s="37"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="184"/>
-      <c r="B2" s="373" t="s">
+      <c r="B2" s="370" t="s">
         <v>535</v>
       </c>
-      <c r="C2" s="374"/>
-      <c r="D2" s="374"/>
-      <c r="E2" s="375"/>
-      <c r="F2" s="373" t="s">
+      <c r="C2" s="371"/>
+      <c r="D2" s="371"/>
+      <c r="E2" s="372"/>
+      <c r="F2" s="370" t="s">
         <v>536</v>
       </c>
-      <c r="G2" s="374"/>
-      <c r="H2" s="374"/>
-      <c r="I2" s="375"/>
-      <c r="J2" s="373" t="s">
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
+      <c r="I2" s="372"/>
+      <c r="J2" s="370" t="s">
         <v>679</v>
       </c>
-      <c r="K2" s="374"/>
-      <c r="L2" s="374"/>
-      <c r="M2" s="375"/>
+      <c r="K2" s="371"/>
+      <c r="L2" s="371"/>
+      <c r="M2" s="372"/>
       <c r="N2" s="39"/>
       <c r="O2" s="188"/>
       <c r="P2" s="188"/>
@@ -16623,9 +16623,9 @@
       <c r="R4" s="367" t="s">
         <v>236</v>
       </c>
-      <c r="S4" s="368"/>
-      <c r="T4" s="368"/>
-      <c r="U4" s="369"/>
+      <c r="S4" s="376"/>
+      <c r="T4" s="376"/>
+      <c r="U4" s="377"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="184" t="s">
@@ -16648,12 +16648,12 @@
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
       <c r="Q5" s="29"/>
-      <c r="R5" s="370" t="s">
+      <c r="R5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="S5" s="371"/>
-      <c r="T5" s="371"/>
-      <c r="U5" s="372"/>
+      <c r="S5" s="379"/>
+      <c r="T5" s="379"/>
+      <c r="U5" s="380"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="184" t="s">
@@ -18323,11 +18323,11 @@
       <c r="K93" s="182"/>
       <c r="L93" s="192"/>
       <c r="M93" s="192"/>
-      <c r="R93" s="377" t="s">
+      <c r="R93" s="373" t="s">
         <v>213</v>
       </c>
-      <c r="S93" s="378"/>
-      <c r="T93" s="378"/>
+      <c r="S93" s="374"/>
+      <c r="T93" s="374"/>
       <c r="U93" s="37"/>
     </row>
     <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -18419,9 +18419,9 @@
       <c r="R96" s="367" t="s">
         <v>51</v>
       </c>
-      <c r="S96" s="379"/>
-      <c r="T96" s="379"/>
-      <c r="U96" s="380"/>
+      <c r="S96" s="368"/>
+      <c r="T96" s="368"/>
+      <c r="U96" s="369"/>
     </row>
     <row r="97" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="184" t="s">
@@ -18443,12 +18443,12 @@
       <c r="K97" s="61"/>
       <c r="L97" s="61"/>
       <c r="M97" s="62"/>
-      <c r="R97" s="377" t="s">
+      <c r="R97" s="373" t="s">
         <v>757</v>
       </c>
-      <c r="S97" s="378"/>
-      <c r="T97" s="378"/>
-      <c r="U97" s="381"/>
+      <c r="S97" s="374"/>
+      <c r="T97" s="374"/>
+      <c r="U97" s="375"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A98" s="184" t="s">
@@ -18500,11 +18500,11 @@
       <c r="K100" s="61"/>
       <c r="L100" s="61"/>
       <c r="M100" s="62"/>
-      <c r="R100" s="377" t="s">
+      <c r="R100" s="373" t="s">
         <v>758</v>
       </c>
-      <c r="S100" s="378"/>
-      <c r="T100" s="378"/>
+      <c r="S100" s="374"/>
+      <c r="T100" s="374"/>
       <c r="U100" s="37"/>
     </row>
     <row r="101" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -18603,9 +18603,9 @@
       <c r="R103" s="367" t="s">
         <v>236</v>
       </c>
-      <c r="S103" s="379"/>
-      <c r="T103" s="379"/>
-      <c r="U103" s="380"/>
+      <c r="S103" s="368"/>
+      <c r="T103" s="368"/>
+      <c r="U103" s="369"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A104" s="184" t="s">
@@ -18622,12 +18622,12 @@
       <c r="L104" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="R104" s="377" t="s">
+      <c r="R104" s="373" t="s">
         <v>757</v>
       </c>
-      <c r="S104" s="378"/>
-      <c r="T104" s="378"/>
-      <c r="U104" s="381"/>
+      <c r="S104" s="374"/>
+      <c r="T104" s="374"/>
+      <c r="U104" s="375"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A105" s="184" t="s">
@@ -18977,12 +18977,12 @@
       <c r="L124" s="29" t="s">
         <v>662</v>
       </c>
-      <c r="R124" s="377" t="s">
+      <c r="R124" s="373" t="s">
         <v>769</v>
       </c>
-      <c r="S124" s="378"/>
-      <c r="T124" s="378"/>
-      <c r="U124" s="381"/>
+      <c r="S124" s="374"/>
+      <c r="T124" s="374"/>
+      <c r="U124" s="375"/>
     </row>
     <row r="125" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="184" t="s">
@@ -19061,20 +19061,20 @@
       <c r="R127" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="S127" s="379"/>
-      <c r="T127" s="379"/>
-      <c r="U127" s="380"/>
+      <c r="S127" s="368"/>
+      <c r="T127" s="368"/>
+      <c r="U127" s="369"/>
     </row>
     <row r="128" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="184" t="s">
         <v>770</v>
       </c>
-      <c r="R128" s="373" t="s">
+      <c r="R128" s="370" t="s">
         <v>757</v>
       </c>
-      <c r="S128" s="374"/>
-      <c r="T128" s="374"/>
-      <c r="U128" s="375"/>
+      <c r="S128" s="371"/>
+      <c r="T128" s="371"/>
+      <c r="U128" s="372"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A129" s="184" t="s">
@@ -19129,12 +19129,12 @@
       <c r="F135" s="60" t="s">
         <v>738</v>
       </c>
-      <c r="R135" s="377" t="s">
+      <c r="R135" s="373" t="s">
         <v>789</v>
       </c>
-      <c r="S135" s="378"/>
-      <c r="T135" s="378"/>
-      <c r="U135" s="381"/>
+      <c r="S135" s="374"/>
+      <c r="T135" s="374"/>
+      <c r="U135" s="375"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A136" s="184" t="s">
@@ -19189,20 +19189,20 @@
       <c r="R138" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="S138" s="379"/>
-      <c r="T138" s="379"/>
-      <c r="U138" s="380"/>
+      <c r="S138" s="368"/>
+      <c r="T138" s="368"/>
+      <c r="U138" s="369"/>
     </row>
     <row r="139" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="184" t="s">
         <v>747</v>
       </c>
-      <c r="R139" s="373" t="s">
+      <c r="R139" s="370" t="s">
         <v>800</v>
       </c>
-      <c r="S139" s="374"/>
-      <c r="T139" s="374"/>
-      <c r="U139" s="375"/>
+      <c r="S139" s="371"/>
+      <c r="T139" s="371"/>
+      <c r="U139" s="372"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A140" s="184" t="s">
@@ -19251,12 +19251,12 @@
       <c r="F145" s="56" t="s">
         <v>731</v>
       </c>
-      <c r="R145" s="377" t="s">
+      <c r="R145" s="373" t="s">
         <v>799</v>
       </c>
-      <c r="S145" s="378"/>
-      <c r="T145" s="378"/>
-      <c r="U145" s="381"/>
+      <c r="S145" s="374"/>
+      <c r="T145" s="374"/>
+      <c r="U145" s="375"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A146" s="184" t="s">
@@ -19311,9 +19311,9 @@
       <c r="R148" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="S148" s="379"/>
-      <c r="T148" s="379"/>
-      <c r="U148" s="380"/>
+      <c r="S148" s="368"/>
+      <c r="T148" s="368"/>
+      <c r="U148" s="369"/>
     </row>
     <row r="149" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="184" t="s">
@@ -19323,12 +19323,12 @@
       <c r="Q149" s="56" t="s">
         <v>762</v>
       </c>
-      <c r="R149" s="373" t="s">
+      <c r="R149" s="370" t="s">
         <v>800</v>
       </c>
-      <c r="S149" s="374"/>
-      <c r="T149" s="374"/>
-      <c r="U149" s="375"/>
+      <c r="S149" s="371"/>
+      <c r="T149" s="371"/>
+      <c r="U149" s="372"/>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A150" s="184" t="s">
@@ -19437,21 +19437,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R138:U138"/>
-    <mergeCell ref="R139:U139"/>
-    <mergeCell ref="R148:U148"/>
-    <mergeCell ref="R149:U149"/>
-    <mergeCell ref="R135:U135"/>
-    <mergeCell ref="R145:U145"/>
-    <mergeCell ref="R128:U128"/>
-    <mergeCell ref="R93:T93"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="R97:U97"/>
-    <mergeCell ref="R100:T100"/>
-    <mergeCell ref="R103:U103"/>
-    <mergeCell ref="R104:U104"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="R127:U127"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="B1:E1"/>
@@ -19462,6 +19447,21 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="R128:U128"/>
+    <mergeCell ref="R93:T93"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="R97:U97"/>
+    <mergeCell ref="R100:T100"/>
+    <mergeCell ref="R103:U103"/>
+    <mergeCell ref="R104:U104"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="R127:U127"/>
+    <mergeCell ref="R138:U138"/>
+    <mergeCell ref="R139:U139"/>
+    <mergeCell ref="R148:U148"/>
+    <mergeCell ref="R149:U149"/>
+    <mergeCell ref="R135:U135"/>
+    <mergeCell ref="R145:U145"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19492,30 +19492,30 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18"/>
-      <c r="B1" s="373" t="s">
+      <c r="B1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="374"/>
-      <c r="D1" s="374"/>
-      <c r="E1" s="375"/>
-      <c r="F1" s="376" t="s">
+      <c r="C1" s="371"/>
+      <c r="D1" s="371"/>
+      <c r="E1" s="372"/>
+      <c r="F1" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
-      <c r="J1" s="373" t="s">
+      <c r="G1" s="371"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
+      <c r="J1" s="370" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="375"/>
-      <c r="N1" s="373" t="s">
+      <c r="K1" s="371"/>
+      <c r="L1" s="371"/>
+      <c r="M1" s="372"/>
+      <c r="N1" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="O1" s="374"/>
-      <c r="P1" s="374"/>
-      <c r="Q1" s="375"/>
+      <c r="O1" s="371"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="372"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="18"/>
@@ -19602,12 +19602,12 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="36"/>
-      <c r="R3" s="377" t="s">
+      <c r="R3" s="373" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="378"/>
-      <c r="T3" s="378"/>
-      <c r="U3" s="381"/>
+      <c r="S3" s="374"/>
+      <c r="T3" s="374"/>
+      <c r="U3" s="375"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="34" t="s">
@@ -19660,12 +19660,12 @@
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
       <c r="Q5" s="29"/>
-      <c r="R5" s="370" t="s">
+      <c r="R5" s="378" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="371"/>
-      <c r="T5" s="371"/>
-      <c r="U5" s="372"/>
+      <c r="S5" s="379"/>
+      <c r="T5" s="379"/>
+      <c r="U5" s="380"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="34" t="s">
@@ -19687,12 +19687,12 @@
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
       <c r="Q6" s="29"/>
-      <c r="R6" s="370" t="s">
+      <c r="R6" s="378" t="s">
         <v>216</v>
       </c>
-      <c r="S6" s="371"/>
-      <c r="T6" s="371"/>
-      <c r="U6" s="372"/>
+      <c r="S6" s="379"/>
+      <c r="T6" s="379"/>
+      <c r="U6" s="380"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="34" t="s">
@@ -23342,12 +23342,12 @@
       <c r="A89" s="253" t="s">
         <v>898</v>
       </c>
-      <c r="B89" s="377" t="s">
+      <c r="B89" s="373" t="s">
         <v>899</v>
       </c>
-      <c r="C89" s="378"/>
-      <c r="D89" s="378"/>
-      <c r="E89" s="381"/>
+      <c r="C89" s="374"/>
+      <c r="D89" s="374"/>
+      <c r="E89" s="375"/>
       <c r="G89" s="382" t="s">
         <v>900</v>
       </c>
@@ -26053,11 +26053,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D1" s="377" t="s">
+      <c r="D1" s="373" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="378"/>
-      <c r="F1" s="378"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="374"/>
       <c r="G1" s="37"/>
       <c r="H1" s="45"/>
       <c r="I1" s="68"/>
@@ -26099,12 +26099,12 @@
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D3" s="370" t="s">
+      <c r="D3" s="378" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="371"/>
-      <c r="F3" s="371"/>
-      <c r="G3" s="372"/>
+      <c r="E3" s="379"/>
+      <c r="F3" s="379"/>
+      <c r="G3" s="380"/>
       <c r="H3" s="85"/>
       <c r="I3" s="87"/>
       <c r="J3" s="87"/>
@@ -26113,12 +26113,12 @@
     </row>
     <row r="5" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="373" t="s">
+      <c r="D6" s="370" t="s">
         <v>535</v>
       </c>
-      <c r="E6" s="374"/>
-      <c r="F6" s="374"/>
-      <c r="G6" s="375"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
+      <c r="G6" s="372"/>
       <c r="H6" s="88"/>
       <c r="I6" s="70"/>
       <c r="J6" s="70"/>
@@ -26127,27 +26127,27 @@
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
       <c r="O6" s="70"/>
-      <c r="P6" s="373" t="s">
+      <c r="P6" s="370" t="s">
         <v>536</v>
       </c>
-      <c r="Q6" s="374"/>
-      <c r="R6" s="374"/>
-      <c r="S6" s="375"/>
-      <c r="AF6" s="373" t="s">
+      <c r="Q6" s="371"/>
+      <c r="R6" s="371"/>
+      <c r="S6" s="372"/>
+      <c r="AF6" s="370" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="374"/>
-      <c r="AH6" s="374"/>
-      <c r="AI6" s="375"/>
+      <c r="AG6" s="371"/>
+      <c r="AH6" s="371"/>
+      <c r="AI6" s="372"/>
       <c r="AJ6" s="119"/>
-      <c r="AK6" s="373" t="s">
+      <c r="AK6" s="370" t="s">
         <v>534</v>
       </c>
-      <c r="AL6" s="374"/>
-      <c r="AM6" s="374"/>
-      <c r="AN6" s="374"/>
-      <c r="AO6" s="374"/>
-      <c r="AP6" s="375"/>
+      <c r="AL6" s="371"/>
+      <c r="AM6" s="371"/>
+      <c r="AN6" s="371"/>
+      <c r="AO6" s="371"/>
+      <c r="AP6" s="372"/>
     </row>
     <row r="7" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D7" s="39" t="s">
@@ -26225,11 +26225,11 @@
       <c r="J8" s="70"/>
       <c r="K8" s="70"/>
       <c r="L8" s="70"/>
-      <c r="M8" s="385" t="s">
+      <c r="M8" s="386" t="s">
         <v>460</v>
       </c>
-      <c r="N8" s="385"/>
-      <c r="O8" s="385"/>
+      <c r="N8" s="386"/>
+      <c r="O8" s="386"/>
       <c r="P8" s="84"/>
       <c r="Q8" s="85"/>
       <c r="R8" s="85"/>
@@ -26250,12 +26250,12 @@
       <c r="AL8" s="120"/>
       <c r="AM8" s="120"/>
       <c r="AN8" s="120"/>
-      <c r="AQ8" s="370" t="s">
+      <c r="AQ8" s="378" t="s">
         <v>17</v>
       </c>
-      <c r="AR8" s="371"/>
-      <c r="AS8" s="371"/>
-      <c r="AT8" s="372"/>
+      <c r="AR8" s="379"/>
+      <c r="AS8" s="379"/>
+      <c r="AT8" s="380"/>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D9" s="248"/>
@@ -26267,11 +26267,11 @@
       <c r="J9" s="87"/>
       <c r="K9" s="87"/>
       <c r="L9" s="87"/>
-      <c r="M9" s="387" t="s">
+      <c r="M9" s="388" t="s">
         <v>461</v>
       </c>
-      <c r="N9" s="387"/>
-      <c r="O9" s="386"/>
+      <c r="N9" s="388"/>
+      <c r="O9" s="387"/>
       <c r="P9" s="84"/>
       <c r="Q9" s="85"/>
       <c r="R9" s="85"/>
@@ -26313,9 +26313,9 @@
       <c r="J10" s="87"/>
       <c r="K10" s="87"/>
       <c r="L10" s="87"/>
-      <c r="M10" s="388"/>
-      <c r="N10" s="388"/>
-      <c r="O10" s="388"/>
+      <c r="M10" s="385"/>
+      <c r="N10" s="385"/>
+      <c r="O10" s="385"/>
       <c r="P10" s="84"/>
       <c r="Q10" s="85"/>
       <c r="R10" s="85"/>
@@ -26340,12 +26340,12 @@
       <c r="AL10" s="120"/>
       <c r="AM10" s="120"/>
       <c r="AN10" s="120"/>
-      <c r="AQ10" s="370" t="s">
+      <c r="AQ10" s="378" t="s">
         <v>51</v>
       </c>
-      <c r="AR10" s="371"/>
-      <c r="AS10" s="371"/>
-      <c r="AT10" s="372"/>
+      <c r="AR10" s="379"/>
+      <c r="AS10" s="379"/>
+      <c r="AT10" s="380"/>
     </row>
     <row r="11" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="248"/>
@@ -26381,12 +26381,12 @@
       <c r="AL11" s="120"/>
       <c r="AM11" s="120"/>
       <c r="AN11" s="120"/>
-      <c r="AQ11" s="370" t="s">
+      <c r="AQ11" s="378" t="s">
         <v>533</v>
       </c>
-      <c r="AR11" s="371"/>
-      <c r="AS11" s="371"/>
-      <c r="AT11" s="372"/>
+      <c r="AR11" s="379"/>
+      <c r="AS11" s="379"/>
+      <c r="AT11" s="380"/>
       <c r="AU11" s="23" t="s">
         <v>217</v>
       </c>
@@ -26430,12 +26430,12 @@
       <c r="AL12" s="120"/>
       <c r="AM12" s="120"/>
       <c r="AN12" s="120"/>
-      <c r="AQ12" s="370" t="s">
+      <c r="AQ12" s="378" t="s">
         <v>458</v>
       </c>
-      <c r="AR12" s="371"/>
-      <c r="AS12" s="371"/>
-      <c r="AT12" s="372"/>
+      <c r="AR12" s="379"/>
+      <c r="AS12" s="379"/>
+      <c r="AT12" s="380"/>
       <c r="AV12" s="18" t="s">
         <v>529</v>
       </c>
@@ -26451,12 +26451,12 @@
         <v>455</v>
       </c>
       <c r="C13" s="97"/>
-      <c r="D13" s="373" t="s">
+      <c r="D13" s="370" t="s">
         <v>462</v>
       </c>
-      <c r="E13" s="374"/>
-      <c r="F13" s="374"/>
-      <c r="G13" s="375"/>
+      <c r="E13" s="371"/>
+      <c r="F13" s="371"/>
+      <c r="G13" s="372"/>
       <c r="H13" s="133" t="s">
         <v>547</v>
       </c>
@@ -26479,11 +26479,11 @@
       <c r="O13" s="146" t="s">
         <v>551</v>
       </c>
-      <c r="P13" s="373" t="s">
+      <c r="P13" s="370" t="s">
         <v>993</v>
       </c>
-      <c r="Q13" s="374"/>
-      <c r="R13" s="374"/>
+      <c r="Q13" s="371"/>
+      <c r="R13" s="371"/>
       <c r="S13" s="122"/>
       <c r="T13" s="136" t="s">
         <v>572</v>
@@ -26519,13 +26519,13 @@
       <c r="AH13" s="45"/>
       <c r="AI13" s="38"/>
       <c r="AJ13" s="119"/>
-      <c r="AK13" s="370" t="s">
+      <c r="AK13" s="378" t="s">
         <v>462</v>
       </c>
-      <c r="AL13" s="371"/>
-      <c r="AM13" s="371"/>
-      <c r="AN13" s="371"/>
-      <c r="AQ13" s="370" t="s">
+      <c r="AL13" s="379"/>
+      <c r="AM13" s="379"/>
+      <c r="AN13" s="379"/>
+      <c r="AQ13" s="378" t="s">
         <v>526</v>
       </c>
       <c r="AR13" s="366"/>
@@ -27226,8 +27226,8 @@
       </c>
       <c r="AO30" s="125"/>
       <c r="AP30" s="127"/>
-      <c r="AR30" s="386"/>
-      <c r="AS30" s="386"/>
+      <c r="AR30" s="387"/>
+      <c r="AS30" s="387"/>
     </row>
     <row r="31" spans="1:52" s="23" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="163" t="s">
@@ -27681,8 +27681,8 @@
         <v>85</v>
       </c>
       <c r="AO40" s="125"/>
-      <c r="AR40" s="388"/>
-      <c r="AS40" s="388"/>
+      <c r="AR40" s="385"/>
+      <c r="AS40" s="385"/>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A41" s="117" t="s">
@@ -27910,8 +27910,8 @@
         <v>549</v>
       </c>
       <c r="AP46" s="127"/>
-      <c r="AR46" s="388"/>
-      <c r="AS46" s="388"/>
+      <c r="AR46" s="385"/>
+      <c r="AS46" s="385"/>
     </row>
     <row r="47" spans="1:45" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="117" t="s">
@@ -27990,12 +27990,12 @@
         <v>457</v>
       </c>
       <c r="C48" s="144"/>
-      <c r="D48" s="373" t="s">
+      <c r="D48" s="370" t="s">
         <v>462</v>
       </c>
-      <c r="E48" s="374"/>
-      <c r="F48" s="374"/>
-      <c r="G48" s="375"/>
+      <c r="E48" s="371"/>
+      <c r="F48" s="371"/>
+      <c r="G48" s="372"/>
       <c r="H48" s="182"/>
       <c r="I48" s="182"/>
       <c r="J48" s="182"/>
@@ -28004,11 +28004,11 @@
       <c r="M48" s="259"/>
       <c r="N48" s="259"/>
       <c r="O48" s="259"/>
-      <c r="P48" s="373" t="s">
+      <c r="P48" s="370" t="s">
         <v>463</v>
       </c>
-      <c r="Q48" s="374"/>
-      <c r="R48" s="374"/>
+      <c r="Q48" s="371"/>
+      <c r="R48" s="371"/>
       <c r="S48" s="154"/>
       <c r="Z48" s="151" t="s">
         <v>548</v>
@@ -29324,13 +29324,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="AR46:AS46"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="AR40:AS40"/>
-    <mergeCell ref="AQ11:AT11"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="D6:G6"/>
@@ -29347,6 +29340,13 @@
     <mergeCell ref="AK13:AN13"/>
     <mergeCell ref="AQ10:AT10"/>
     <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="AR46:AS46"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="AR40:AS40"/>
+    <mergeCell ref="AQ11:AT11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29404,17 +29404,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.4">
-      <c r="B1" s="377" t="s">
+      <c r="B1" s="373" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="378"/>
-      <c r="D1" s="378"/>
+      <c r="C1" s="374"/>
+      <c r="D1" s="374"/>
       <c r="E1" s="37"/>
-      <c r="F1" s="377" t="s">
+      <c r="F1" s="373" t="s">
         <v>836</v>
       </c>
-      <c r="G1" s="378"/>
-      <c r="H1" s="378"/>
+      <c r="G1" s="374"/>
+      <c r="H1" s="374"/>
       <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.4">
@@ -29460,58 +29460,58 @@
       <c r="B4" s="367" t="s">
         <v>835</v>
       </c>
-      <c r="C4" s="368"/>
-      <c r="D4" s="368"/>
-      <c r="E4" s="369"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="377"/>
       <c r="F4" s="367" t="s">
         <v>236</v>
       </c>
-      <c r="G4" s="368"/>
-      <c r="H4" s="368"/>
-      <c r="I4" s="369"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
+      <c r="I4" s="377"/>
     </row>
     <row r="5" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="370" t="s">
+      <c r="B5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="C5" s="371"/>
-      <c r="D5" s="371"/>
-      <c r="E5" s="372"/>
-      <c r="F5" s="370" t="s">
+      <c r="C5" s="379"/>
+      <c r="D5" s="379"/>
+      <c r="E5" s="380"/>
+      <c r="F5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="G5" s="371"/>
-      <c r="H5" s="371"/>
-      <c r="I5" s="372"/>
+      <c r="G5" s="379"/>
+      <c r="H5" s="379"/>
+      <c r="I5" s="380"/>
     </row>
     <row r="6" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="373" t="s">
+      <c r="B6" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="374"/>
-      <c r="D6" s="374"/>
-      <c r="E6" s="375"/>
-      <c r="F6" s="376" t="s">
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="372"/>
+      <c r="F6" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="374"/>
-      <c r="H6" s="374"/>
-      <c r="I6" s="374"/>
-      <c r="J6" s="373" t="s">
+      <c r="G6" s="371"/>
+      <c r="H6" s="371"/>
+      <c r="I6" s="371"/>
+      <c r="J6" s="370" t="s">
         <v>178</v>
       </c>
-      <c r="K6" s="374"/>
-      <c r="L6" s="374"/>
-      <c r="M6" s="375"/>
-      <c r="N6" s="373" t="s">
+      <c r="K6" s="371"/>
+      <c r="L6" s="371"/>
+      <c r="M6" s="372"/>
+      <c r="N6" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="O6" s="374"/>
-      <c r="P6" s="374"/>
-      <c r="Q6" s="375"/>
+      <c r="O6" s="371"/>
+      <c r="P6" s="371"/>
+      <c r="Q6" s="372"/>
       <c r="V6" s="41"/>
       <c r="W6" s="42"/>
       <c r="X6" s="42"/>
@@ -29540,24 +29540,24 @@
     </row>
     <row r="7" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="170"/>
-      <c r="B7" s="373" t="s">
+      <c r="B7" s="370" t="s">
         <v>535</v>
       </c>
-      <c r="C7" s="374"/>
-      <c r="D7" s="374"/>
-      <c r="E7" s="375"/>
-      <c r="F7" s="373" t="s">
+      <c r="C7" s="371"/>
+      <c r="D7" s="371"/>
+      <c r="E7" s="372"/>
+      <c r="F7" s="370" t="s">
         <v>536</v>
       </c>
-      <c r="G7" s="374"/>
-      <c r="H7" s="374"/>
-      <c r="I7" s="375"/>
-      <c r="J7" s="373" t="s">
+      <c r="G7" s="371"/>
+      <c r="H7" s="371"/>
+      <c r="I7" s="372"/>
+      <c r="J7" s="370" t="s">
         <v>679</v>
       </c>
-      <c r="K7" s="374"/>
-      <c r="L7" s="374"/>
-      <c r="M7" s="375"/>
+      <c r="K7" s="371"/>
+      <c r="L7" s="371"/>
+      <c r="M7" s="372"/>
       <c r="N7" s="167"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
@@ -33249,11 +33249,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B4:E4"/>
@@ -33262,6 +33257,11 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33324,31 +33324,31 @@
       <c r="B1" s="222"/>
       <c r="C1" s="222"/>
       <c r="D1" s="319"/>
-      <c r="E1" s="377" t="s">
+      <c r="E1" s="373" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="378"/>
-      <c r="G1" s="378"/>
+      <c r="F1" s="374"/>
+      <c r="G1" s="374"/>
       <c r="H1" s="37"/>
       <c r="I1" s="98"/>
-      <c r="J1" s="377" t="s">
+      <c r="J1" s="373" t="s">
         <v>836</v>
       </c>
-      <c r="K1" s="378"/>
-      <c r="L1" s="378"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="374"/>
       <c r="M1" s="47"/>
       <c r="N1" s="281"/>
-      <c r="O1" s="377" t="s">
+      <c r="O1" s="373" t="s">
         <v>886</v>
       </c>
-      <c r="P1" s="378"/>
-      <c r="Q1" s="378"/>
+      <c r="P1" s="374"/>
+      <c r="Q1" s="374"/>
       <c r="R1" s="37"/>
-      <c r="S1" s="377" t="s">
+      <c r="S1" s="373" t="s">
         <v>889</v>
       </c>
-      <c r="T1" s="378"/>
-      <c r="U1" s="378"/>
+      <c r="T1" s="374"/>
+      <c r="U1" s="374"/>
       <c r="V1" s="47"/>
       <c r="W1" s="279"/>
       <c r="X1" s="242"/>
@@ -33357,11 +33357,11 @@
       <c r="AA1" s="273"/>
       <c r="AB1" s="273"/>
       <c r="AC1" s="273"/>
-      <c r="AD1" s="377" t="s">
+      <c r="AD1" s="373" t="s">
         <v>890</v>
       </c>
-      <c r="AE1" s="378"/>
-      <c r="AF1" s="378"/>
+      <c r="AE1" s="374"/>
+      <c r="AF1" s="374"/>
       <c r="AG1" s="37"/>
       <c r="AH1" s="345"/>
       <c r="AI1" s="42"/>
@@ -33468,69 +33468,69 @@
       <c r="E4" s="367" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="368"/>
-      <c r="G4" s="368"/>
-      <c r="H4" s="369"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="377"/>
       <c r="I4" s="70"/>
       <c r="J4" s="367" t="s">
         <v>236</v>
       </c>
-      <c r="K4" s="368"/>
-      <c r="L4" s="368"/>
-      <c r="M4" s="369"/>
+      <c r="K4" s="376"/>
+      <c r="L4" s="376"/>
+      <c r="M4" s="377"/>
       <c r="N4" s="209"/>
       <c r="O4" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="P4" s="368"/>
-      <c r="Q4" s="368"/>
-      <c r="R4" s="369"/>
+      <c r="P4" s="376"/>
+      <c r="Q4" s="376"/>
+      <c r="R4" s="377"/>
       <c r="S4" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="T4" s="368"/>
-      <c r="U4" s="368"/>
-      <c r="V4" s="369"/>
+      <c r="T4" s="376"/>
+      <c r="U4" s="376"/>
+      <c r="V4" s="377"/>
       <c r="AD4" s="367" t="s">
         <v>761</v>
       </c>
-      <c r="AE4" s="368"/>
-      <c r="AF4" s="368"/>
-      <c r="AG4" s="369"/>
+      <c r="AE4" s="376"/>
+      <c r="AF4" s="376"/>
+      <c r="AG4" s="377"/>
     </row>
     <row r="5" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E5" s="370" t="s">
+      <c r="E5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="F5" s="371"/>
-      <c r="G5" s="371"/>
-      <c r="H5" s="372"/>
+      <c r="F5" s="379"/>
+      <c r="G5" s="379"/>
+      <c r="H5" s="380"/>
       <c r="I5" s="274"/>
-      <c r="J5" s="370" t="s">
+      <c r="J5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="K5" s="371"/>
-      <c r="L5" s="371"/>
-      <c r="M5" s="372"/>
+      <c r="K5" s="379"/>
+      <c r="L5" s="379"/>
+      <c r="M5" s="380"/>
       <c r="N5" s="71"/>
-      <c r="O5" s="370" t="s">
+      <c r="O5" s="378" t="s">
         <v>757</v>
       </c>
-      <c r="P5" s="371"/>
-      <c r="Q5" s="371"/>
-      <c r="R5" s="372"/>
-      <c r="S5" s="370" t="s">
+      <c r="P5" s="379"/>
+      <c r="Q5" s="379"/>
+      <c r="R5" s="380"/>
+      <c r="S5" s="378" t="s">
         <v>800</v>
       </c>
-      <c r="T5" s="371"/>
-      <c r="U5" s="371"/>
-      <c r="V5" s="372"/>
-      <c r="AD5" s="370" t="s">
+      <c r="T5" s="379"/>
+      <c r="U5" s="379"/>
+      <c r="V5" s="380"/>
+      <c r="AD5" s="378" t="s">
         <v>800</v>
       </c>
-      <c r="AE5" s="371"/>
-      <c r="AF5" s="371"/>
-      <c r="AG5" s="372"/>
+      <c r="AE5" s="379"/>
+      <c r="AF5" s="379"/>
+      <c r="AG5" s="380"/>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="170" t="s">
@@ -33539,24 +33539,24 @@
       <c r="B6" s="222"/>
       <c r="C6" s="222"/>
       <c r="D6" s="319"/>
-      <c r="E6" s="373" t="s">
+      <c r="E6" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="374"/>
-      <c r="G6" s="374"/>
-      <c r="H6" s="375"/>
+      <c r="F6" s="371"/>
+      <c r="G6" s="371"/>
+      <c r="H6" s="372"/>
       <c r="I6" s="273"/>
       <c r="J6" s="41"/>
       <c r="K6" s="42"/>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
       <c r="N6" s="284"/>
-      <c r="O6" s="376" t="s">
+      <c r="O6" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="P6" s="374"/>
-      <c r="Q6" s="374"/>
-      <c r="R6" s="374"/>
+      <c r="P6" s="371"/>
+      <c r="Q6" s="371"/>
+      <c r="R6" s="371"/>
       <c r="S6" s="41"/>
       <c r="T6" s="42"/>
       <c r="U6" s="42"/>
@@ -33568,23 +33568,23 @@
       <c r="AA6" s="273"/>
       <c r="AB6" s="273"/>
       <c r="AC6" s="273"/>
-      <c r="AD6" s="373" t="s">
+      <c r="AD6" s="370" t="s">
         <v>930</v>
       </c>
-      <c r="AE6" s="374"/>
-      <c r="AF6" s="374"/>
-      <c r="AG6" s="375"/>
+      <c r="AE6" s="371"/>
+      <c r="AF6" s="371"/>
+      <c r="AG6" s="372"/>
       <c r="AH6" s="345"/>
       <c r="AI6" s="42"/>
       <c r="AJ6" s="42"/>
       <c r="AK6" s="42"/>
       <c r="AL6" s="43"/>
-      <c r="AM6" s="373" t="s">
+      <c r="AM6" s="370" t="s">
         <v>181</v>
       </c>
-      <c r="AN6" s="374"/>
-      <c r="AO6" s="374"/>
-      <c r="AP6" s="375"/>
+      <c r="AN6" s="371"/>
+      <c r="AO6" s="371"/>
+      <c r="AP6" s="372"/>
       <c r="AQ6" s="174"/>
       <c r="AR6" s="175"/>
       <c r="AS6" s="175"/>
@@ -33601,30 +33601,30 @@
       <c r="D7" s="305" t="s">
         <v>1042</v>
       </c>
-      <c r="E7" s="373" t="s">
+      <c r="E7" s="370" t="s">
         <v>535</v>
       </c>
-      <c r="F7" s="374"/>
-      <c r="G7" s="374"/>
-      <c r="H7" s="375"/>
+      <c r="F7" s="371"/>
+      <c r="G7" s="371"/>
+      <c r="H7" s="372"/>
       <c r="I7" s="113"/>
-      <c r="J7" s="373" t="s">
+      <c r="J7" s="370" t="s">
         <v>723</v>
       </c>
-      <c r="K7" s="374"/>
-      <c r="L7" s="374"/>
-      <c r="M7" s="375"/>
+      <c r="K7" s="371"/>
+      <c r="L7" s="371"/>
+      <c r="M7" s="372"/>
       <c r="N7" s="285"/>
-      <c r="O7" s="373" t="s">
+      <c r="O7" s="370" t="s">
         <v>536</v>
       </c>
-      <c r="P7" s="374"/>
-      <c r="Q7" s="374"/>
-      <c r="R7" s="375"/>
-      <c r="S7" s="373"/>
-      <c r="T7" s="374"/>
-      <c r="U7" s="374"/>
-      <c r="V7" s="375"/>
+      <c r="P7" s="371"/>
+      <c r="Q7" s="371"/>
+      <c r="R7" s="372"/>
+      <c r="S7" s="370"/>
+      <c r="T7" s="371"/>
+      <c r="U7" s="371"/>
+      <c r="V7" s="372"/>
       <c r="W7" s="392" t="s">
         <v>931</v>
       </c>
@@ -33634,12 +33634,12 @@
       <c r="AA7" s="113"/>
       <c r="AB7" s="113"/>
       <c r="AC7" s="113"/>
-      <c r="AD7" s="373" t="s">
+      <c r="AD7" s="370" t="s">
         <v>888</v>
       </c>
-      <c r="AE7" s="374"/>
-      <c r="AF7" s="374"/>
-      <c r="AG7" s="375"/>
+      <c r="AE7" s="371"/>
+      <c r="AF7" s="371"/>
+      <c r="AG7" s="372"/>
       <c r="AH7" s="341"/>
       <c r="AI7" s="25"/>
       <c r="AJ7" s="25"/>
@@ -33649,12 +33649,12 @@
       <c r="AN7" s="177"/>
       <c r="AO7" s="177"/>
       <c r="AP7" s="178"/>
-      <c r="AQ7" s="373" t="s">
+      <c r="AQ7" s="370" t="s">
         <v>724</v>
       </c>
-      <c r="AR7" s="374"/>
-      <c r="AS7" s="374"/>
-      <c r="AT7" s="375"/>
+      <c r="AR7" s="371"/>
+      <c r="AS7" s="371"/>
+      <c r="AT7" s="372"/>
     </row>
     <row r="8" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="170">
@@ -35875,30 +35875,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="AQ7:AT7"/>
-    <mergeCell ref="AM6:AP6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="AD7:AG7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="S7:V7"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD1:AF1"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AD5:AG5"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W7:Z7"/>
     <mergeCell ref="J58:M58"/>
     <mergeCell ref="J46:M46"/>
     <mergeCell ref="S1:U1"/>
@@ -35911,6 +35887,30 @@
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="J30:M30"/>
     <mergeCell ref="J38:M38"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="W7:Z7"/>
+    <mergeCell ref="AQ7:AT7"/>
+    <mergeCell ref="AM6:AP6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="AD7:AG7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35921,11 +35921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6F30D8-4F74-43CF-B0A2-082294AF7E0E}">
   <dimension ref="A1:AN64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32:D33"/>
+      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -35968,40 +35968,40 @@
       <c r="D1" s="349"/>
       <c r="E1" s="350"/>
       <c r="F1" s="351"/>
-      <c r="G1" s="373" t="s">
+      <c r="G1" s="370" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="374"/>
-      <c r="I1" s="374"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="371"/>
       <c r="J1" s="395"/>
-      <c r="K1" s="376" t="s">
+      <c r="K1" s="381" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="374"/>
-      <c r="M1" s="374"/>
-      <c r="N1" s="374"/>
+      <c r="L1" s="371"/>
+      <c r="M1" s="371"/>
+      <c r="N1" s="371"/>
       <c r="O1" s="296"/>
       <c r="P1" s="295"/>
       <c r="Q1" s="296"/>
       <c r="R1" s="297"/>
-      <c r="S1" s="373" t="s">
+      <c r="S1" s="370" t="s">
         <v>383</v>
       </c>
-      <c r="T1" s="374"/>
-      <c r="U1" s="374"/>
-      <c r="V1" s="375"/>
+      <c r="T1" s="371"/>
+      <c r="U1" s="371"/>
+      <c r="V1" s="372"/>
       <c r="W1" s="296"/>
       <c r="X1" s="296"/>
       <c r="AA1" s="41"/>
       <c r="AB1" s="42"/>
       <c r="AC1" s="42"/>
       <c r="AD1" s="43"/>
-      <c r="AK1" s="373" t="s">
+      <c r="AK1" s="370" t="s">
         <v>848</v>
       </c>
-      <c r="AL1" s="374"/>
-      <c r="AM1" s="374"/>
-      <c r="AN1" s="375"/>
+      <c r="AL1" s="371"/>
+      <c r="AM1" s="371"/>
+      <c r="AN1" s="372"/>
     </row>
     <row r="2" spans="1:40" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="18"/>
@@ -36092,10 +36092,10 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="37"/>
-      <c r="K3" s="377"/>
-      <c r="L3" s="378"/>
-      <c r="M3" s="378"/>
-      <c r="N3" s="381"/>
+      <c r="K3" s="373"/>
+      <c r="L3" s="374"/>
+      <c r="M3" s="374"/>
+      <c r="N3" s="375"/>
       <c r="O3" s="298" t="s">
         <v>1025</v>
       </c>
@@ -36141,14 +36141,18 @@
       <c r="F4" s="336"/>
       <c r="G4" s="44"/>
       <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
+      <c r="I4" s="352" t="s">
+        <v>951</v>
+      </c>
       <c r="J4" s="38"/>
       <c r="K4" s="303"/>
       <c r="L4" s="303"/>
       <c r="M4" s="303"/>
       <c r="N4" s="303"/>
       <c r="O4" s="303"/>
-      <c r="P4" s="259"/>
+      <c r="P4" s="302" t="s">
+        <v>1008</v>
+      </c>
       <c r="Q4" s="259"/>
       <c r="R4" s="311"/>
       <c r="S4" s="303"/>
@@ -36180,16 +36184,20 @@
       <c r="G5" s="44"/>
       <c r="H5" s="45"/>
       <c r="I5" s="352" t="s">
-        <v>951</v>
-      </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="303"/>
-      <c r="L5" s="303"/>
-      <c r="M5" s="303"/>
-      <c r="N5" s="303"/>
+        <v>116</v>
+      </c>
+      <c r="J5" s="352" t="s">
+        <v>952</v>
+      </c>
+      <c r="K5" s="60" t="s">
+        <v>344</v>
+      </c>
+      <c r="L5" s="18"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
       <c r="O5" s="303"/>
       <c r="P5" s="302" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="Q5" s="303"/>
       <c r="R5" s="304"/>
@@ -36219,22 +36227,26 @@
       <c r="G6" s="302"/>
       <c r="H6" s="303"/>
       <c r="I6" s="352" t="s">
-        <v>116</v>
+        <v>196</v>
       </c>
       <c r="J6" s="352" t="s">
-        <v>952</v>
+        <v>114</v>
       </c>
       <c r="K6" s="60" t="s">
-        <v>344</v>
-      </c>
-      <c r="L6" s="18"/>
+        <v>345</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>349</v>
+      </c>
       <c r="M6" s="33"/>
       <c r="N6" s="33"/>
       <c r="O6" s="303"/>
       <c r="P6" s="302" t="s">
-        <v>1009</v>
-      </c>
-      <c r="Q6" s="303"/>
+        <v>1010</v>
+      </c>
+      <c r="Q6" s="302">
+        <v>0</v>
+      </c>
       <c r="R6" s="304"/>
       <c r="S6" s="303"/>
       <c r="AB6" s="23" t="s">
@@ -36270,25 +36282,27 @@
       <c r="G7" s="302"/>
       <c r="H7" s="303"/>
       <c r="I7" s="352" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J7" s="352" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L7" s="60" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
-      <c r="O7" s="303"/>
+      <c r="O7" s="315" t="s">
+        <v>344</v>
+      </c>
       <c r="P7" s="302" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="Q7" s="302">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="304"/>
       <c r="S7" s="303"/>
@@ -36327,27 +36341,27 @@
       <c r="G8" s="302"/>
       <c r="H8" s="303"/>
       <c r="I8" s="352" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="J8" s="352" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L8" s="60" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M8" s="33"/>
       <c r="N8" s="33"/>
       <c r="O8" s="315" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="P8" s="302" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="Q8" s="302">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="304"/>
       <c r="S8" s="149" t="s">
@@ -36388,27 +36402,24 @@
       <c r="G9" s="302"/>
       <c r="H9" s="303"/>
       <c r="I9" s="352" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="J9" s="352" t="s">
-        <v>200</v>
+        <v>283</v>
       </c>
       <c r="K9" s="60" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M9" s="33"/>
       <c r="N9" s="33"/>
       <c r="O9" s="315" t="s">
-        <v>345</v>
-      </c>
-      <c r="P9" s="302" t="s">
-        <v>1012</v>
+        <v>346</v>
       </c>
       <c r="Q9" s="302">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R9" s="304"/>
       <c r="S9" s="149" t="s">
@@ -36445,24 +36456,22 @@
       </c>
       <c r="E10" s="333"/>
       <c r="I10" s="352" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="J10" s="352" t="s">
-        <v>283</v>
-      </c>
-      <c r="K10" s="60" t="s">
-        <v>348</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="K10" s="18"/>
       <c r="L10" s="60" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M10" s="33"/>
       <c r="N10" s="33"/>
       <c r="O10" s="315" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q10" s="302">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R10" s="304"/>
       <c r="S10" s="28"/>
@@ -36480,7 +36489,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:40" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="34" t="s">
         <v>53</v>
       </c>
@@ -36492,24 +36501,19 @@
         <v>1085</v>
       </c>
       <c r="I11" s="352" t="s">
-        <v>273</v>
-      </c>
-      <c r="J11" s="352" t="s">
-        <v>281</v>
-      </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="60" t="s">
-        <v>353</v>
-      </c>
+        <v>1084</v>
+      </c>
+      <c r="J11" s="312" t="s">
+        <v>282</v>
+      </c>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="315" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="P11" s="302"/>
-      <c r="Q11" s="302">
-        <v>4</v>
-      </c>
       <c r="R11" s="304"/>
       <c r="S11" s="28"/>
       <c r="U11" s="54" t="s">
@@ -36531,23 +36535,13 @@
       <c r="AG11" s="47"/>
       <c r="AH11" s="37"/>
     </row>
-    <row r="12" spans="1:40" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A12" s="34" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="322"/>
-      <c r="I12" s="352" t="s">
-        <v>1084</v>
-      </c>
-      <c r="J12" s="312" t="s">
-        <v>282</v>
-      </c>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="315" t="s">
-        <v>348</v>
+      <c r="J12" s="352" t="s">
+        <v>953</v>
       </c>
       <c r="P12" s="316"/>
       <c r="Q12" s="317"/>
@@ -36573,9 +36567,6 @@
         <v>57</v>
       </c>
       <c r="B13" s="322"/>
-      <c r="J13" s="352" t="s">
-        <v>953</v>
-      </c>
       <c r="Q13" s="303"/>
       <c r="R13" s="29"/>
       <c r="S13" s="23"/>

</xml_diff>

<commit_message>
220507-v6 cov_L  l_k_base_addr need revise
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9BACD5-5AF8-41E9-B233-0A2C80866032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541FA03-ADF4-4FE2-859B-6AB5F85629BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="2" activeTab="10" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="2" activeTab="8" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD1,2" sheetId="3" r:id="rId1"/>
@@ -7091,7 +7091,7 @@
   <dimension ref="A1:AQ54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A49" sqref="A49:XFD49"/>
@@ -8160,8 +8160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6F30D8-4F74-43CF-B0A2-082294AF7E0E}">
   <dimension ref="A1:BB84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A65" sqref="A65:XFD65"/>
@@ -40646,9 +40646,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B6D41B-A83C-4B0F-AB4E-45A43C474451}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R6" sqref="R6:R7"/>
+      <selection pane="topRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
220709-v4 problrms with NEW3
</commit_message>
<xml_diff>
--- a/EKF-SLAM时序图.xlsx
+++ b/EKF-SLAM时序图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958AA280-8B67-4955-858A-A63F852CE1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F33F968-F8CF-4BE1-AFCC-E0E54C5B526F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="1965" windowWidth="9585" windowHeight="6000" firstSheet="7" activeTab="14" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="7" activeTab="14" xr2:uid="{95158FA3-8CE8-4C65-B2CC-718C905F7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD1,2" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5253" uniqueCount="1209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5301" uniqueCount="1220">
   <si>
     <t>M</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4121,10 +4121,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>CB_addra_new</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>TB_addra_new</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -4168,14 +4164,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>init_prd</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>CBa_NL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PRD_NL_1</t>
   </si>
   <si>
@@ -4216,78 +4204,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PRD_NL_3</t>
+  </si>
+  <si>
+    <t>lk_x(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lk_y(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lk_x(0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lk_y(0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>x_hat</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>y_hat</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>theta_hat</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>cos_gamma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sin_gamma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rk_cos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-rk_sin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dx_d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dy_d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dx_d2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dy_d2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRD_NL_3</t>
-  </si>
-  <si>
-    <t>l_k_base+3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lk_x(1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lk_y(1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lk_x(0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lk_y(0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x_hat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y_hat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4307,7 +4247,110 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>seq_cnt_dout_sel</t>
+    <t>NL_RCV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NL_SEND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CB dout/din</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBa din</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sel_new=CBa_NL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sel=Cba_NL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sel=CBb_NL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEW_NL_3</t>
+  </si>
+  <si>
+    <t>Gxi_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gz_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gz_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gxi_23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gz_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gz_22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hxi_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hz_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hz_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hxi_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hxi_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hxi_22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hz_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hz_22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vt(1,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vt(2,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CB_addr_new</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4772,7 +4815,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="453">
+  <cellXfs count="457">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6015,10 +6058,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6033,33 +6107,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6069,6 +6119,9 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6078,9 +6131,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6129,7 +6179,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -6454,11 +6509,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W1" s="413" t="s">
+      <c r="W1" s="416" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="413"/>
-      <c r="Y1" s="413"/>
+      <c r="X1" s="416"/>
+      <c r="Y1" s="416"/>
       <c r="Z1" s="22"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.4">
@@ -6473,11 +6528,11 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="W3" s="413" t="s">
+      <c r="W3" s="416" t="s">
         <v>50</v>
       </c>
-      <c r="X3" s="413"/>
-      <c r="Y3" s="413"/>
+      <c r="X3" s="416"/>
+      <c r="Y3" s="416"/>
       <c r="Z3" s="21" t="s">
         <v>51</v>
       </c>
@@ -7235,7 +7290,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -7256,27 +7311,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D1" s="445" t="s">
+      <c r="D1" s="448" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="446"/>
-      <c r="F1" s="446"/>
-      <c r="G1" s="447"/>
-      <c r="H1" s="445" t="s">
+      <c r="E1" s="449"/>
+      <c r="F1" s="449"/>
+      <c r="G1" s="450"/>
+      <c r="H1" s="448" t="s">
         <v>1108</v>
       </c>
-      <c r="I1" s="446"/>
-      <c r="J1" s="446"/>
-      <c r="K1" s="447"/>
+      <c r="I1" s="449"/>
+      <c r="J1" s="449"/>
+      <c r="K1" s="450"/>
       <c r="L1" s="406"/>
       <c r="M1" s="408"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="445" t="s">
+      <c r="O1" s="448" t="s">
         <v>1136</v>
       </c>
-      <c r="P1" s="446"/>
-      <c r="Q1" s="446"/>
-      <c r="R1" s="447"/>
+      <c r="P1" s="449"/>
+      <c r="Q1" s="449"/>
+      <c r="R1" s="450"/>
     </row>
     <row r="2" spans="1:18" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="344" t="s">
@@ -7338,10 +7393,10 @@
       <c r="A3" s="154" t="s">
         <v>966</v>
       </c>
-      <c r="D3" s="424"/>
-      <c r="E3" s="425"/>
-      <c r="F3" s="425"/>
-      <c r="G3" s="428"/>
+      <c r="D3" s="423"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="425"/>
       <c r="L3" s="401"/>
       <c r="M3" s="103" t="s">
         <v>966</v>
@@ -8167,10 +8222,10 @@
       <c r="A41" s="154" t="s">
         <v>1138</v>
       </c>
-      <c r="D41" s="424"/>
-      <c r="E41" s="425"/>
-      <c r="F41" s="425"/>
-      <c r="G41" s="428"/>
+      <c r="D41" s="423"/>
+      <c r="E41" s="424"/>
+      <c r="F41" s="424"/>
+      <c r="G41" s="425"/>
       <c r="L41" s="401"/>
       <c r="M41" s="103" t="s">
         <v>1138</v>
@@ -8443,10 +8498,10 @@
   <dimension ref="A1:BB84"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3:C5"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -8488,8 +8543,8 @@
       </c>
       <c r="H1" s="421"/>
       <c r="I1" s="421"/>
-      <c r="J1" s="448"/>
-      <c r="K1" s="423" t="s">
+      <c r="J1" s="451"/>
+      <c r="K1" s="431" t="s">
         <v>1120</v>
       </c>
       <c r="L1" s="421"/>
@@ -8606,12 +8661,12 @@
         <v>977</v>
       </c>
       <c r="P3" s="28"/>
-      <c r="X3" s="425" t="s">
+      <c r="X3" s="424" t="s">
         <v>1156</v>
       </c>
-      <c r="Y3" s="425"/>
-      <c r="Z3" s="425"/>
-      <c r="AA3" s="428"/>
+      <c r="Y3" s="424"/>
+      <c r="Z3" s="424"/>
+      <c r="AA3" s="425"/>
       <c r="AD3" s="35"/>
       <c r="AE3" s="33"/>
       <c r="AF3" s="33"/>
@@ -8676,12 +8731,12 @@
       <c r="O5" s="287">
         <v>1</v>
       </c>
-      <c r="X5" s="417" t="s">
+      <c r="X5" s="428" t="s">
         <v>758</v>
       </c>
-      <c r="Y5" s="418"/>
-      <c r="Z5" s="418"/>
-      <c r="AA5" s="419"/>
+      <c r="Y5" s="429"/>
+      <c r="Z5" s="429"/>
+      <c r="AA5" s="430"/>
       <c r="AD5" s="287"/>
       <c r="AE5" s="288"/>
       <c r="AF5" s="288"/>
@@ -8720,12 +8775,12 @@
       <c r="O6" s="287">
         <v>2</v>
       </c>
-      <c r="X6" s="417" t="s">
+      <c r="X6" s="428" t="s">
         <v>1153</v>
       </c>
-      <c r="Y6" s="418"/>
-      <c r="Z6" s="418"/>
-      <c r="AA6" s="419"/>
+      <c r="Y6" s="429"/>
+      <c r="Z6" s="429"/>
+      <c r="AA6" s="430"/>
       <c r="AD6" s="35"/>
       <c r="AE6" s="33"/>
       <c r="AF6" s="33"/>
@@ -8763,12 +8818,12 @@
       <c r="O7" s="287">
         <v>3</v>
       </c>
-      <c r="X7" s="417" t="s">
+      <c r="X7" s="428" t="s">
         <v>1154</v>
       </c>
-      <c r="Y7" s="418"/>
-      <c r="Z7" s="418"/>
-      <c r="AA7" s="419"/>
+      <c r="Y7" s="429"/>
+      <c r="Z7" s="429"/>
+      <c r="AA7" s="430"/>
       <c r="AB7" s="64" t="s">
         <v>442</v>
       </c>
@@ -8815,12 +8870,12 @@
       <c r="O8" s="287">
         <v>4</v>
       </c>
-      <c r="X8" s="417" t="s">
+      <c r="X8" s="428" t="s">
         <v>1155</v>
       </c>
-      <c r="Y8" s="418"/>
-      <c r="Z8" s="418"/>
-      <c r="AA8" s="419"/>
+      <c r="Y8" s="429"/>
+      <c r="Z8" s="429"/>
+      <c r="AA8" s="430"/>
       <c r="AD8" s="35"/>
       <c r="AE8" s="33"/>
       <c r="AF8" s="33"/>
@@ -8858,12 +8913,12 @@
       <c r="O9" s="287"/>
       <c r="V9" s="311"/>
       <c r="W9" s="311"/>
-      <c r="X9" s="417" t="s">
+      <c r="X9" s="428" t="s">
         <v>1118</v>
       </c>
-      <c r="Y9" s="418"/>
-      <c r="Z9" s="418"/>
-      <c r="AA9" s="419"/>
+      <c r="Y9" s="429"/>
+      <c r="Z9" s="429"/>
+      <c r="AA9" s="430"/>
     </row>
     <row r="10" spans="1:33" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="34" t="s">
@@ -8899,12 +8954,12 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="244"/>
-      <c r="X10" s="417" t="s">
+      <c r="X10" s="428" t="s">
         <v>1119</v>
       </c>
-      <c r="Y10" s="418"/>
-      <c r="Z10" s="418"/>
-      <c r="AA10" s="419"/>
+      <c r="Y10" s="429"/>
+      <c r="Z10" s="429"/>
+      <c r="AA10" s="430"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A11" s="34" t="s">
@@ -10696,17 +10751,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="X3:AA3"/>
     <mergeCell ref="X10:AA10"/>
     <mergeCell ref="X5:AA5"/>
     <mergeCell ref="X6:AA6"/>
     <mergeCell ref="X7:AA7"/>
     <mergeCell ref="X8:AA8"/>
     <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="X3:AA3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10718,7 +10773,7 @@
   <dimension ref="A1:Z163"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -10758,7 +10813,7 @@
       <c r="G1" s="421"/>
       <c r="H1" s="421"/>
       <c r="I1" s="422"/>
-      <c r="J1" s="423" t="s">
+      <c r="J1" s="431" t="s">
         <v>1120</v>
       </c>
       <c r="K1" s="421"/>
@@ -10882,12 +10937,12 @@
       </c>
       <c r="Q3" s="230"/>
       <c r="R3" s="49"/>
-      <c r="W3" s="425" t="s">
+      <c r="W3" s="424" t="s">
         <v>1156</v>
       </c>
-      <c r="X3" s="425"/>
-      <c r="Y3" s="425"/>
-      <c r="Z3" s="428"/>
+      <c r="X3" s="424"/>
+      <c r="Y3" s="424"/>
+      <c r="Z3" s="425"/>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="231" t="s">
@@ -10957,12 +11012,12 @@
       <c r="Q5" s="230"/>
       <c r="R5" s="49"/>
       <c r="S5" s="309"/>
-      <c r="W5" s="417" t="s">
+      <c r="W5" s="428" t="s">
         <v>758</v>
       </c>
-      <c r="X5" s="418"/>
-      <c r="Y5" s="418"/>
-      <c r="Z5" s="419"/>
+      <c r="X5" s="429"/>
+      <c r="Y5" s="429"/>
+      <c r="Z5" s="430"/>
     </row>
     <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="231" t="s">
@@ -10991,12 +11046,12 @@
       <c r="N6" s="312"/>
       <c r="Q6" s="230"/>
       <c r="R6" s="49"/>
-      <c r="W6" s="417" t="s">
+      <c r="W6" s="428" t="s">
         <v>1153</v>
       </c>
-      <c r="X6" s="418"/>
-      <c r="Y6" s="418"/>
-      <c r="Z6" s="419"/>
+      <c r="X6" s="429"/>
+      <c r="Y6" s="429"/>
+      <c r="Z6" s="430"/>
     </row>
     <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="231" t="s">
@@ -11028,12 +11083,12 @@
       <c r="N7" s="312"/>
       <c r="Q7" s="230"/>
       <c r="R7" s="49"/>
-      <c r="W7" s="417" t="s">
+      <c r="W7" s="428" t="s">
         <v>1154</v>
       </c>
-      <c r="X7" s="418"/>
-      <c r="Y7" s="418"/>
-      <c r="Z7" s="419"/>
+      <c r="X7" s="429"/>
+      <c r="Y7" s="429"/>
+      <c r="Z7" s="430"/>
     </row>
     <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="231" t="s">
@@ -11061,12 +11116,12 @@
       <c r="N8" s="312"/>
       <c r="Q8" s="230"/>
       <c r="R8" s="49"/>
-      <c r="W8" s="417" t="s">
+      <c r="W8" s="428" t="s">
         <v>1155</v>
       </c>
-      <c r="X8" s="418"/>
-      <c r="Y8" s="418"/>
-      <c r="Z8" s="419"/>
+      <c r="X8" s="429"/>
+      <c r="Y8" s="429"/>
+      <c r="Z8" s="430"/>
     </row>
     <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="231" t="s">
@@ -11094,12 +11149,12 @@
       <c r="N9" s="312"/>
       <c r="Q9" s="230"/>
       <c r="R9" s="49"/>
-      <c r="W9" s="417" t="s">
+      <c r="W9" s="428" t="s">
         <v>1118</v>
       </c>
-      <c r="X9" s="418"/>
-      <c r="Y9" s="418"/>
-      <c r="Z9" s="419"/>
+      <c r="X9" s="429"/>
+      <c r="Y9" s="429"/>
+      <c r="Z9" s="430"/>
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="231" t="s">
@@ -11124,12 +11179,12 @@
       <c r="N10" s="312"/>
       <c r="Q10" s="230"/>
       <c r="R10" s="49"/>
-      <c r="W10" s="417" t="s">
+      <c r="W10" s="428" t="s">
         <v>1119</v>
       </c>
-      <c r="X10" s="418"/>
-      <c r="Y10" s="418"/>
-      <c r="Z10" s="419"/>
+      <c r="X10" s="429"/>
+      <c r="Y10" s="429"/>
+      <c r="Z10" s="430"/>
     </row>
     <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="231" t="s">
@@ -13464,10 +13519,10 @@
   <dimension ref="A1:AM90"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A10"/>
+      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -13666,12 +13721,12 @@
       <c r="T3" s="348"/>
       <c r="U3" s="348"/>
       <c r="V3" s="349"/>
-      <c r="AE3" s="424" t="s">
+      <c r="AE3" s="423" t="s">
         <v>1115</v>
       </c>
-      <c r="AF3" s="425"/>
-      <c r="AG3" s="425"/>
-      <c r="AH3" s="428"/>
+      <c r="AF3" s="424"/>
+      <c r="AG3" s="424"/>
+      <c r="AH3" s="425"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A4" s="368" t="s">
@@ -13752,12 +13807,12 @@
       <c r="U5" s="348"/>
       <c r="V5" s="349"/>
       <c r="AA5" s="313"/>
-      <c r="AE5" s="417" t="s">
+      <c r="AE5" s="428" t="s">
         <v>234</v>
       </c>
-      <c r="AF5" s="418"/>
-      <c r="AG5" s="418"/>
-      <c r="AH5" s="419"/>
+      <c r="AF5" s="429"/>
+      <c r="AG5" s="429"/>
+      <c r="AH5" s="430"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A6" s="368" t="s">
@@ -13796,12 +13851,12 @@
       <c r="U6" s="348"/>
       <c r="V6" s="349"/>
       <c r="AA6" s="313"/>
-      <c r="AE6" s="417" t="s">
+      <c r="AE6" s="428" t="s">
         <v>1114</v>
       </c>
-      <c r="AF6" s="418"/>
-      <c r="AG6" s="418"/>
-      <c r="AH6" s="419"/>
+      <c r="AF6" s="429"/>
+      <c r="AG6" s="429"/>
+      <c r="AH6" s="430"/>
     </row>
     <row r="7" spans="1:39" ht="12.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="368" t="s">
@@ -13842,12 +13897,12 @@
       <c r="U7" s="348"/>
       <c r="V7" s="349"/>
       <c r="AA7" s="313"/>
-      <c r="AE7" s="417" t="s">
+      <c r="AE7" s="428" t="s">
         <v>1112</v>
       </c>
-      <c r="AF7" s="418"/>
-      <c r="AG7" s="418"/>
-      <c r="AH7" s="419"/>
+      <c r="AF7" s="429"/>
+      <c r="AG7" s="429"/>
+      <c r="AH7" s="430"/>
       <c r="AJ7" s="347"/>
       <c r="AK7" s="348"/>
       <c r="AL7" s="348"/>
@@ -13879,7 +13934,7 @@
         <v>229</v>
       </c>
       <c r="P8" s="294" t="s">
-        <v>230</v>
+        <v>1217</v>
       </c>
       <c r="Q8" s="368" t="s">
         <v>6</v>
@@ -13892,12 +13947,12 @@
       <c r="U8" s="348"/>
       <c r="V8" s="349"/>
       <c r="AA8" s="313"/>
-      <c r="AE8" s="417" t="s">
+      <c r="AE8" s="428" t="s">
         <v>1113</v>
       </c>
-      <c r="AF8" s="418"/>
-      <c r="AG8" s="418"/>
-      <c r="AH8" s="419"/>
+      <c r="AF8" s="429"/>
+      <c r="AG8" s="429"/>
+      <c r="AH8" s="430"/>
       <c r="AJ8" s="347"/>
       <c r="AK8" s="348"/>
       <c r="AL8" s="348"/>
@@ -13927,7 +13982,7 @@
       <c r="N9" s="348"/>
       <c r="O9" s="348"/>
       <c r="P9" s="294" t="s">
-        <v>231</v>
+        <v>1218</v>
       </c>
       <c r="Q9" s="368" t="s">
         <v>8</v>
@@ -13942,12 +13997,12 @@
       <c r="U9" s="348"/>
       <c r="V9" s="349"/>
       <c r="AA9" s="313"/>
-      <c r="AE9" s="417" t="s">
+      <c r="AE9" s="428" t="s">
         <v>1111</v>
       </c>
-      <c r="AF9" s="418"/>
-      <c r="AG9" s="418"/>
-      <c r="AH9" s="419"/>
+      <c r="AF9" s="429"/>
+      <c r="AG9" s="429"/>
+      <c r="AH9" s="430"/>
       <c r="AJ9" s="347"/>
       <c r="AK9" s="348"/>
       <c r="AL9" s="74" t="s">
@@ -13988,12 +14043,12 @@
       </c>
       <c r="V10" s="349"/>
       <c r="AA10" s="313"/>
-      <c r="AE10" s="417" t="s">
+      <c r="AE10" s="428" t="s">
         <v>1118</v>
       </c>
-      <c r="AF10" s="418"/>
-      <c r="AG10" s="418"/>
-      <c r="AH10" s="419"/>
+      <c r="AF10" s="429"/>
+      <c r="AG10" s="429"/>
+      <c r="AH10" s="430"/>
       <c r="AJ10" s="347"/>
       <c r="AK10" s="74" t="s">
         <v>578</v>
@@ -14056,12 +14111,12 @@
       <c r="AD11" s="344" t="s">
         <v>1117</v>
       </c>
-      <c r="AE11" s="449" t="s">
+      <c r="AE11" s="452" t="s">
         <v>1119</v>
       </c>
-      <c r="AF11" s="415"/>
-      <c r="AG11" s="415"/>
-      <c r="AH11" s="416"/>
+      <c r="AF11" s="426"/>
+      <c r="AG11" s="426"/>
+      <c r="AH11" s="427"/>
       <c r="AJ11" s="75" t="s">
         <v>579</v>
       </c>
@@ -17402,12 +17457,12 @@
       <c r="P3" s="176"/>
       <c r="Q3" s="176"/>
       <c r="R3" s="177"/>
-      <c r="S3" s="424" t="s">
+      <c r="S3" s="423" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="425"/>
-      <c r="U3" s="425"/>
-      <c r="V3" s="428"/>
+      <c r="T3" s="424"/>
+      <c r="U3" s="424"/>
+      <c r="V3" s="425"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="231" t="s">
@@ -17476,12 +17531,12 @@
       <c r="P5" s="176"/>
       <c r="Q5" s="176"/>
       <c r="R5" s="177"/>
-      <c r="S5" s="417" t="s">
+      <c r="S5" s="428" t="s">
         <v>234</v>
       </c>
-      <c r="T5" s="418"/>
-      <c r="U5" s="418"/>
-      <c r="V5" s="419"/>
+      <c r="T5" s="429"/>
+      <c r="U5" s="429"/>
+      <c r="V5" s="430"/>
     </row>
     <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="231" t="s">
@@ -17512,12 +17567,12 @@
       <c r="P6" s="176"/>
       <c r="Q6" s="176"/>
       <c r="R6" s="177"/>
-      <c r="S6" s="417" t="s">
+      <c r="S6" s="428" t="s">
         <v>235</v>
       </c>
-      <c r="T6" s="418"/>
-      <c r="U6" s="418"/>
-      <c r="V6" s="419"/>
+      <c r="T6" s="429"/>
+      <c r="U6" s="429"/>
+      <c r="V6" s="430"/>
     </row>
     <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="231" t="s">
@@ -17585,12 +17640,12 @@
         <v>236</v>
       </c>
       <c r="R8" s="177"/>
-      <c r="S8" s="450" t="s">
+      <c r="S8" s="453" t="s">
         <v>829</v>
       </c>
-      <c r="T8" s="451"/>
-      <c r="U8" s="451"/>
-      <c r="V8" s="451"/>
+      <c r="T8" s="454"/>
+      <c r="U8" s="454"/>
+      <c r="V8" s="454"/>
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="231" t="s">
@@ -19898,59 +19953,56 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0308FE05-318F-4754-9DD5-50D0105D6ADD}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="409"/>
-    <col min="2" max="2" width="16" style="411" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.06640625" style="409"/>
-    <col min="6" max="6" width="12.06640625" style="409" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.9296875" style="409" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.9296875" style="410" customWidth="1"/>
+    <col min="1" max="4" width="9.06640625" style="409"/>
+    <col min="5" max="5" width="10.9296875" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" style="410" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.9296875" style="413" customWidth="1"/>
     <col min="9" max="11" width="9.06640625" style="409"/>
     <col min="12" max="12" width="9.06640625" style="410"/>
-    <col min="13" max="13" width="10.9296875" style="409" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.53125" style="410" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.06640625" style="409"/>
-    <col min="17" max="17" width="10.53125" style="409" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.06640625" style="409"/>
-    <col min="19" max="19" width="7.86328125" style="409" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.73046875" style="409" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.06640625" style="409"/>
+    <col min="13" max="13" width="12.53125" style="68" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.73046875" style="409" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="9.06640625" style="409"/>
+    <col min="21" max="21" width="10.53125" style="409" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.06640625" style="409"/>
+    <col min="23" max="23" width="7.86328125" style="409" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.06640625" style="409"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="410" t="s">
         <v>964</v>
       </c>
-      <c r="B1" s="411" t="s">
-        <v>1208</v>
+      <c r="B1" s="409" t="s">
+        <v>1157</v>
       </c>
       <c r="C1" s="409" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D1" s="409" t="s">
-        <v>1158</v>
-      </c>
-      <c r="E1" s="409" t="s">
         <v>1159</v>
       </c>
-      <c r="F1" s="409" t="s">
+      <c r="E1" s="455" t="s">
         <v>1172</v>
       </c>
-      <c r="G1" s="409" t="s">
-        <v>1160</v>
-      </c>
-      <c r="H1" s="410" t="s">
+      <c r="F1" s="410" t="s">
         <v>558</v>
+      </c>
+      <c r="G1" s="413" t="s">
+        <v>557</v>
+      </c>
+      <c r="H1" s="413" t="s">
+        <v>1219</v>
       </c>
       <c r="I1" s="409" t="s">
         <v>103</v>
@@ -19964,421 +20016,769 @@
       <c r="L1" s="410" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="409" t="s">
+      <c r="M1" s="455" t="s">
+        <v>1173</v>
+      </c>
+      <c r="N1" s="409" t="s">
+        <v>1160</v>
+      </c>
+      <c r="O1" s="410" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="410" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="410" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="410" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="410" t="s">
+        <v>1178</v>
+      </c>
+      <c r="T1" s="409" t="s">
+        <v>1174</v>
+      </c>
+      <c r="U1" s="410" t="s">
         <v>1175</v>
       </c>
-      <c r="N1" s="409" t="s">
+      <c r="V1" s="410" t="s">
         <v>1176</v>
       </c>
-      <c r="O1" s="410" t="s">
-        <v>1181</v>
-      </c>
-      <c r="P1" s="409" t="s">
+      <c r="W1" s="410" t="s">
         <v>1177</v>
       </c>
-      <c r="Q1" s="410" t="s">
-        <v>1178</v>
-      </c>
-      <c r="R1" s="410" t="s">
-        <v>1179</v>
-      </c>
-      <c r="S1" s="410" t="s">
-        <v>1180</v>
-      </c>
-      <c r="T1" s="409" t="s">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="B2" s="409" t="s">
         <v>1161</v>
       </c>
-      <c r="U1" s="410" t="s">
-        <v>103</v>
-      </c>
-      <c r="V1" s="410" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="410" t="s">
-        <v>2</v>
-      </c>
-      <c r="X1" s="410" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C2" s="409" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="D2" s="409" t="s">
         <v>1162</v>
       </c>
-      <c r="E2" s="409" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A3" s="409">
-        <v>0</v>
+      <c r="I2" s="409" t="s">
+        <v>1195</v>
+      </c>
+      <c r="O2" s="409" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A3" s="409" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B3" s="409" t="s">
+        <v>1162</v>
       </c>
       <c r="C3" s="409" t="s">
         <v>1163</v>
       </c>
-      <c r="D3" s="409" t="s">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="368" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="368"/>
-      <c r="D4" s="409" t="s">
+      <c r="C4" s="409" t="s">
+        <v>1163</v>
+      </c>
+      <c r="H4" s="413" t="s">
         <v>1164</v>
       </c>
-      <c r="G4" s="409">
-        <v>3</v>
-      </c>
-      <c r="H4" s="410" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="368" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="368"/>
-      <c r="D5" s="409" t="s">
-        <v>1164</v>
-      </c>
-      <c r="G5" s="409" t="s">
+      <c r="C5" s="409" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F5" s="410" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+      <c r="H5" s="413" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="368" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="368"/>
-      <c r="D6" s="409" t="s">
+      <c r="C6" s="409" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F6" s="410" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I6" s="409" t="s">
         <v>1164</v>
       </c>
-      <c r="F6" s="409" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="368" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="368"/>
-      <c r="D7" s="410" t="s">
-        <v>1174</v>
+      <c r="C7" s="410" t="s">
+        <v>1171</v>
       </c>
       <c r="I7" s="409" t="s">
+        <v>1183</v>
+      </c>
+      <c r="J7" s="409" t="s">
         <v>1165</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="368" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="368"/>
-      <c r="D8" s="410" t="s">
-        <v>1174</v>
-      </c>
-      <c r="I8" s="409" t="s">
-        <v>1198</v>
+      <c r="C8" s="410" t="s">
+        <v>1171</v>
       </c>
       <c r="J8" s="409" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K8" s="409" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="368" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="368"/>
-      <c r="D9" s="410" t="s">
+      <c r="C9" s="410" t="s">
+        <v>1171</v>
+      </c>
+      <c r="K9" s="409" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.4">
+      <c r="A10" s="368" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="410" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>1200</v>
+      </c>
+      <c r="L10" s="410" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.4">
+      <c r="A11" s="368"/>
+      <c r="C11" s="409" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.4">
+      <c r="A12" s="368"/>
+      <c r="C12" s="409" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.4">
+      <c r="A13" s="368"/>
+      <c r="C13" s="409" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="414" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="456"/>
+      <c r="C14" s="414" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E14" s="199"/>
+      <c r="M14" s="199"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="C15" s="409" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M15" s="68" t="s">
+        <v>1200</v>
+      </c>
+      <c r="T15" s="415" t="s">
         <v>1174</v>
       </c>
-      <c r="J9" s="409" t="s">
-        <v>1199</v>
-      </c>
-      <c r="K9" s="409" t="s">
-        <v>1167</v>
-      </c>
-      <c r="M9" s="409">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A10" s="368"/>
-      <c r="B10" s="368"/>
-      <c r="D10" s="410" t="s">
+      <c r="U15" s="415" t="s">
+        <v>1191</v>
+      </c>
+      <c r="V15" s="415" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A16" s="410" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C16" s="409" t="s">
         <v>1169</v>
       </c>
-      <c r="K10" s="409" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A11" s="368"/>
-      <c r="B11" s="368"/>
-      <c r="D11" s="409" t="s">
-        <v>1168</v>
-      </c>
-      <c r="L11" s="410" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A12" s="368"/>
-      <c r="B12" s="368"/>
-      <c r="D12" s="409" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A13" s="368"/>
-      <c r="B13" s="368"/>
-      <c r="D13" s="409" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="368"/>
-      <c r="B14" s="368"/>
-      <c r="D14" s="409" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="D15" s="409" t="s">
-        <v>1169</v>
-      </c>
-      <c r="N15" s="410">
-        <v>1</v>
-      </c>
-      <c r="P15" s="452" t="s">
-        <v>1177</v>
-      </c>
-      <c r="Q15" s="452" t="s">
-        <v>1206</v>
-      </c>
-      <c r="R15" s="452" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A16" s="410">
-        <v>0</v>
-      </c>
-      <c r="D16" s="409" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" s="368" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="368"/>
-      <c r="D17" s="409" t="s">
-        <v>1170</v>
-      </c>
-      <c r="G17" s="409">
-        <v>3</v>
-      </c>
-      <c r="T17" s="409">
+      <c r="C17" s="409" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G17" s="413" t="s">
+        <v>1199</v>
+      </c>
+      <c r="N17" s="409">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="368" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="368"/>
-      <c r="D18" s="409" t="s">
-        <v>1170</v>
+      <c r="C18" s="409" t="s">
+        <v>1169</v>
       </c>
       <c r="I18" s="409" t="s">
-        <v>1202</v>
-      </c>
-      <c r="T18" s="409">
+        <v>1187</v>
+      </c>
+      <c r="N18" s="409">
         <v>3</v>
       </c>
-      <c r="U18" s="409" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+      <c r="O18" s="409" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="368" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="368"/>
-      <c r="D19" s="409" t="s">
-        <v>1170</v>
+      <c r="C19" s="409" t="s">
+        <v>1169</v>
       </c>
       <c r="J19" s="409" t="s">
-        <v>1203</v>
-      </c>
-      <c r="T19" s="409">
+        <v>1188</v>
+      </c>
+      <c r="N19" s="409">
         <v>4</v>
       </c>
-      <c r="U19" s="409">
+      <c r="O19" s="409">
         <v>1</v>
       </c>
-      <c r="V19" s="409" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+      <c r="P19" s="409" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="368" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="368"/>
-      <c r="D20" s="410" t="s">
-        <v>1196</v>
+      <c r="C20" s="410" t="s">
+        <v>1182</v>
       </c>
       <c r="K20" s="409" t="s">
-        <v>1184</v>
-      </c>
-      <c r="U20" s="409">
+        <v>1181</v>
+      </c>
+      <c r="O20" s="409">
         <v>0</v>
       </c>
-      <c r="V20" s="409">
+      <c r="P20" s="409">
         <v>0</v>
       </c>
-      <c r="W20" s="409">
+      <c r="Q20" s="409">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="368" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="368"/>
-      <c r="D21" s="410" t="s">
-        <v>1196</v>
+      <c r="C21" s="410" t="s">
+        <v>1182</v>
       </c>
       <c r="L21" s="410">
         <v>0</v>
       </c>
-      <c r="V21" s="409">
+      <c r="P21" s="409">
         <v>1</v>
       </c>
-      <c r="W21" s="411" t="s">
-        <v>1182</v>
-      </c>
-      <c r="X21" s="409">
+      <c r="Q21" s="411" t="s">
+        <v>1179</v>
+      </c>
+      <c r="R21" s="409">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="368" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="368"/>
-      <c r="D22" s="410" t="s">
-        <v>1196</v>
-      </c>
-      <c r="W22" s="411" t="s">
-        <v>1183</v>
-      </c>
-      <c r="X22" s="409">
+      <c r="C22" s="410" t="s">
+        <v>1182</v>
+      </c>
+      <c r="Q22" s="411" t="s">
+        <v>1180</v>
+      </c>
+      <c r="R22" s="409">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A23" s="368"/>
-      <c r="B23" s="368"/>
-      <c r="D23" s="410" t="s">
-        <v>1196</v>
-      </c>
-      <c r="X23" s="409">
+    <row r="23" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A23" s="368" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="410" t="s">
+        <v>1182</v>
+      </c>
+      <c r="R23" s="409">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="368"/>
-      <c r="B24" s="368"/>
-      <c r="D24" s="409" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+      <c r="C24" s="409" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="368"/>
-      <c r="B25" s="368"/>
-      <c r="D25" s="409" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A26" s="368"/>
-      <c r="B26" s="368"/>
-    </row>
-    <row r="27" spans="1:24" ht="15" x14ac:dyDescent="0.4">
+      <c r="C25" s="409" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="414" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="456"/>
+      <c r="E26" s="199"/>
+      <c r="M26" s="199"/>
+    </row>
+    <row r="27" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A27" s="368"/>
-      <c r="B27" s="368"/>
-    </row>
-    <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A28" s="368"/>
-      <c r="B28" s="368"/>
-    </row>
-    <row r="29" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A29" s="368"/>
-      <c r="B29" s="368"/>
-    </row>
-    <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.4">
-      <c r="A30" s="368"/>
-      <c r="B30" s="368"/>
-    </row>
-    <row r="35" spans="14:18" x14ac:dyDescent="0.4">
-      <c r="N35" s="410">
-        <v>1</v>
-      </c>
-      <c r="O35" s="410" t="s">
-        <v>1185</v>
-      </c>
-      <c r="P35" s="410" t="s">
-        <v>1186</v>
-      </c>
-      <c r="Q35" s="410" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="36" spans="14:18" x14ac:dyDescent="0.4">
-      <c r="O36" s="409" t="s">
-        <v>1188</v>
-      </c>
-      <c r="P36" s="409" t="s">
+      <c r="M27" s="68" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A28" s="413" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B28" s="413"/>
+      <c r="C28" s="413" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A29" s="368" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="413"/>
+      <c r="C29" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N29" s="413">
+        <v>17</v>
+      </c>
+      <c r="O29" s="413"/>
+      <c r="P29" s="413"/>
+      <c r="Q29" s="413"/>
+      <c r="R29" s="413"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A30" s="368" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="413"/>
+      <c r="C30" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N30" s="413">
+        <v>18</v>
+      </c>
+      <c r="O30" s="413" t="s">
+        <v>1202</v>
+      </c>
+      <c r="P30" s="413"/>
+      <c r="Q30" s="413"/>
+      <c r="R30" s="413"/>
+    </row>
+    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A31" s="368" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="413"/>
+      <c r="C31" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N31" s="413">
+        <v>19</v>
+      </c>
+      <c r="O31" s="413" t="s">
+        <v>1203</v>
+      </c>
+      <c r="P31" s="413" t="s">
+        <v>1205</v>
+      </c>
+      <c r="Q31" s="413"/>
+      <c r="R31" s="413"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A32" s="368" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="413"/>
+      <c r="C32" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N32" s="413"/>
+      <c r="O32" s="413" t="s">
+        <v>1204</v>
+      </c>
+      <c r="P32" s="413" t="s">
+        <v>1206</v>
+      </c>
+      <c r="Q32" s="413">
+        <v>0</v>
+      </c>
+      <c r="R32" s="413"/>
+    </row>
+    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A33" s="368" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="413"/>
+      <c r="C33" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N33" s="413"/>
+      <c r="O33" s="413"/>
+      <c r="P33" s="413" t="s">
+        <v>1207</v>
+      </c>
+      <c r="Q33" s="413">
+        <v>0</v>
+      </c>
+      <c r="R33" s="413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A34" s="368" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="413"/>
+      <c r="C34" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N34" s="413"/>
+      <c r="O34" s="413"/>
+      <c r="P34" s="413"/>
+      <c r="Q34" s="413">
+        <v>0</v>
+      </c>
+      <c r="R34" s="413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A35" s="368" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="413"/>
+      <c r="C35" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="N35" s="413"/>
+      <c r="O35" s="413"/>
+      <c r="P35" s="413"/>
+      <c r="Q35" s="413"/>
+      <c r="R35" s="413">
+        <v>0</v>
+      </c>
+      <c r="T35" s="410"/>
+      <c r="U35" s="410"/>
+      <c r="V35" s="410"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="V36" s="412"/>
+    </row>
+    <row r="38" spans="1:22" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="456"/>
+      <c r="B38" s="414"/>
+      <c r="C38" s="414"/>
+      <c r="D38" s="414"/>
+      <c r="E38" s="199"/>
+      <c r="F38" s="414"/>
+      <c r="G38" s="414"/>
+      <c r="H38" s="414"/>
+      <c r="I38" s="414"/>
+      <c r="J38" s="414"/>
+      <c r="K38" s="414"/>
+      <c r="L38" s="414"/>
+      <c r="M38" s="199"/>
+      <c r="N38" s="414"/>
+      <c r="O38" s="414"/>
+      <c r="P38" s="414"/>
+      <c r="Q38" s="414"/>
+      <c r="R38" s="414"/>
+    </row>
+    <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A39" s="368"/>
+      <c r="B39" s="413"/>
+      <c r="C39" s="413"/>
+      <c r="D39" s="413"/>
+      <c r="F39" s="413"/>
+      <c r="I39" s="413"/>
+      <c r="J39" s="413"/>
+      <c r="K39" s="413"/>
+      <c r="L39" s="413"/>
+      <c r="M39" s="68" t="s">
+        <v>1208</v>
+      </c>
+      <c r="N39" s="413"/>
+      <c r="O39" s="413"/>
+      <c r="P39" s="413"/>
+      <c r="Q39" s="413"/>
+      <c r="R39" s="413"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A40" s="413" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B40" s="413"/>
+      <c r="C40" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D40" s="413"/>
+      <c r="F40" s="413"/>
+      <c r="I40" s="413"/>
+      <c r="J40" s="413"/>
+      <c r="K40" s="413"/>
+      <c r="L40" s="413"/>
+      <c r="N40" s="413"/>
+      <c r="O40" s="413"/>
+      <c r="P40" s="413"/>
+      <c r="Q40" s="413"/>
+      <c r="R40" s="413"/>
+    </row>
+    <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A41" s="368" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="413"/>
+      <c r="C41" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D41" s="413"/>
+      <c r="F41" s="413"/>
+      <c r="I41" s="413"/>
+      <c r="J41" s="413"/>
+      <c r="K41" s="413"/>
+      <c r="L41" s="413"/>
+      <c r="N41" s="413">
+        <v>26</v>
+      </c>
+      <c r="O41" s="413"/>
+      <c r="P41" s="413"/>
+      <c r="Q41" s="413"/>
+      <c r="R41" s="413"/>
+    </row>
+    <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A42" s="368" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="413"/>
+      <c r="C42" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D42" s="413"/>
+      <c r="F42" s="413"/>
+      <c r="I42" s="413"/>
+      <c r="J42" s="413"/>
+      <c r="K42" s="413"/>
+      <c r="L42" s="413"/>
+      <c r="N42" s="413">
+        <v>27</v>
+      </c>
+      <c r="O42" s="413" t="s">
+        <v>1209</v>
+      </c>
+      <c r="P42" s="413"/>
+      <c r="Q42" s="413"/>
+      <c r="R42" s="413"/>
+    </row>
+    <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A43" s="368" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="413"/>
+      <c r="C43" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D43" s="413"/>
+      <c r="F43" s="413"/>
+      <c r="I43" s="413"/>
+      <c r="J43" s="413"/>
+      <c r="K43" s="413"/>
+      <c r="L43" s="413"/>
+      <c r="N43" s="413">
+        <v>29</v>
+      </c>
+      <c r="O43" s="409" t="s">
+        <v>1212</v>
+      </c>
+      <c r="P43" s="413" t="s">
+        <v>1213</v>
+      </c>
+      <c r="Q43" s="413"/>
+      <c r="R43" s="413"/>
+    </row>
+    <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A44" s="368" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="413"/>
+      <c r="C44" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D44" s="413"/>
+      <c r="F44" s="413"/>
+      <c r="I44" s="413"/>
+      <c r="J44" s="413"/>
+      <c r="K44" s="413"/>
+      <c r="L44" s="413"/>
+      <c r="N44" s="413">
+        <v>30</v>
+      </c>
+      <c r="O44" s="413" t="s">
+        <v>1210</v>
+      </c>
+      <c r="P44" s="413" t="s">
+        <v>1214</v>
+      </c>
+      <c r="Q44" s="413">
+        <v>0</v>
+      </c>
+      <c r="R44" s="413"/>
+    </row>
+    <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A45" s="368" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="413"/>
+      <c r="C45" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D45" s="413"/>
+      <c r="F45" s="413"/>
+      <c r="I45" s="413"/>
+      <c r="J45" s="413"/>
+      <c r="K45" s="413"/>
+      <c r="L45" s="413"/>
+      <c r="N45" s="413">
+        <v>38</v>
+      </c>
+      <c r="O45" s="413" t="s">
+        <v>1211</v>
+      </c>
+      <c r="P45" s="413" t="s">
+        <v>1215</v>
+      </c>
+      <c r="Q45" s="413">
+        <v>0</v>
+      </c>
+      <c r="R45" s="413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A46" s="368" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="413"/>
+      <c r="C46" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D46" s="413"/>
+      <c r="F46" s="413"/>
+      <c r="I46" s="413"/>
+      <c r="J46" s="413"/>
+      <c r="K46" s="413"/>
+      <c r="L46" s="413"/>
+      <c r="N46" s="413">
+        <v>39</v>
+      </c>
+      <c r="O46" s="413">
+        <v>0</v>
+      </c>
+      <c r="P46" s="413" t="s">
+        <v>1216</v>
+      </c>
+      <c r="Q46" s="413">
+        <v>0</v>
+      </c>
+      <c r="R46" s="413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A47" s="368" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="413"/>
+      <c r="C47" s="413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D47" s="413"/>
+      <c r="F47" s="413"/>
+      <c r="I47" s="413"/>
+      <c r="J47" s="413"/>
+      <c r="K47" s="413"/>
+      <c r="L47" s="413"/>
+      <c r="N47" s="413"/>
+      <c r="O47" s="413">
+        <v>0</v>
+      </c>
+      <c r="P47" s="413">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="413">
+        <v>0</v>
+      </c>
+      <c r="R47" s="413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.4">
+      <c r="A48" s="368" t="s">
+        <v>52</v>
+      </c>
+      <c r="P48" s="413">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="413">
+        <v>0</v>
+      </c>
+      <c r="R48" s="409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A49" s="368" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q49" s="413">
+        <v>0</v>
+      </c>
+      <c r="R49" s="409" t="s">
         <v>1189</v>
       </c>
-      <c r="Q36" s="412" t="s">
-        <v>1191</v>
-      </c>
-      <c r="R36" s="409" t="s">
+    </row>
+    <row r="50" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+      <c r="A50" s="368"/>
+      <c r="R50" s="409" t="s">
         <v>1190</v>
-      </c>
-    </row>
-    <row r="40" spans="14:18" x14ac:dyDescent="0.4">
-      <c r="N40" s="410">
-        <v>1</v>
-      </c>
-      <c r="O40" s="409" t="s">
-        <v>1204</v>
-      </c>
-      <c r="P40" s="409" t="s">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="41" spans="14:18" x14ac:dyDescent="0.4">
-      <c r="O41" s="409" t="s">
-        <v>1192</v>
-      </c>
-      <c r="P41" s="409" t="s">
-        <v>1193</v>
-      </c>
-      <c r="Q41" s="409" t="s">
-        <v>1194</v>
-      </c>
-      <c r="R41" s="409" t="s">
-        <v>1195</v>
       </c>
     </row>
   </sheetData>
@@ -20422,7 +20822,7 @@
       <c r="D1" s="421"/>
       <c r="E1" s="421"/>
       <c r="F1" s="422"/>
-      <c r="G1" s="423" t="s">
+      <c r="G1" s="431" t="s">
         <v>105</v>
       </c>
       <c r="H1" s="421"/>
@@ -20514,33 +20914,33 @@
       <c r="B3" s="18">
         <v>0</v>
       </c>
-      <c r="C3" s="424" t="s">
+      <c r="C3" s="423" t="s">
         <v>217</v>
       </c>
-      <c r="D3" s="425"/>
-      <c r="E3" s="425"/>
-      <c r="F3" s="428"/>
-      <c r="G3" s="424"/>
-      <c r="H3" s="425"/>
-      <c r="I3" s="425"/>
-      <c r="J3" s="428"/>
+      <c r="D3" s="424"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="425"/>
+      <c r="G3" s="423"/>
+      <c r="H3" s="424"/>
+      <c r="I3" s="424"/>
+      <c r="J3" s="425"/>
       <c r="K3" s="175"/>
       <c r="O3" s="175"/>
       <c r="P3" s="176"/>
       <c r="Q3" s="176"/>
       <c r="R3" s="177"/>
-      <c r="S3" s="424" t="s">
+      <c r="S3" s="423" t="s">
         <v>340</v>
       </c>
-      <c r="T3" s="425"/>
-      <c r="U3" s="425"/>
-      <c r="V3" s="428"/>
-      <c r="Z3" s="424" t="s">
+      <c r="T3" s="424"/>
+      <c r="U3" s="424"/>
+      <c r="V3" s="425"/>
+      <c r="Z3" s="423" t="s">
         <v>217</v>
       </c>
-      <c r="AA3" s="425"/>
-      <c r="AB3" s="425"/>
-      <c r="AC3" s="428"/>
+      <c r="AA3" s="424"/>
+      <c r="AB3" s="424"/>
+      <c r="AC3" s="425"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B4" s="34" t="s">
@@ -20597,12 +20997,12 @@
       <c r="P5" s="176"/>
       <c r="Q5" s="176"/>
       <c r="R5" s="177"/>
-      <c r="S5" s="417" t="s">
+      <c r="S5" s="428" t="s">
         <v>440</v>
       </c>
-      <c r="T5" s="418"/>
-      <c r="U5" s="418"/>
-      <c r="V5" s="419"/>
+      <c r="T5" s="429"/>
+      <c r="U5" s="429"/>
+      <c r="V5" s="430"/>
       <c r="W5" s="64" t="s">
         <v>442</v>
       </c>
@@ -20632,12 +21032,12 @@
       <c r="P6" s="176"/>
       <c r="Q6" s="176"/>
       <c r="R6" s="177"/>
-      <c r="S6" s="417" t="s">
+      <c r="S6" s="428" t="s">
         <v>357</v>
       </c>
-      <c r="T6" s="418"/>
-      <c r="U6" s="418"/>
-      <c r="V6" s="419"/>
+      <c r="T6" s="429"/>
+      <c r="U6" s="429"/>
+      <c r="V6" s="430"/>
       <c r="Z6" s="175"/>
       <c r="AA6" s="176"/>
       <c r="AB6" s="176"/>
@@ -21996,17 +22396,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="S5:V5"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="Z3:AC3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22047,7 +22447,7 @@
       <c r="C1" s="421"/>
       <c r="D1" s="421"/>
       <c r="E1" s="422"/>
-      <c r="F1" s="423" t="s">
+      <c r="F1" s="431" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="421"/>
@@ -22065,11 +22465,11 @@
       <c r="O1" s="421"/>
       <c r="P1" s="421"/>
       <c r="Q1" s="422"/>
-      <c r="R1" s="424" t="s">
+      <c r="R1" s="423" t="s">
         <v>211</v>
       </c>
-      <c r="S1" s="425"/>
-      <c r="T1" s="425"/>
+      <c r="S1" s="424"/>
+      <c r="T1" s="424"/>
       <c r="U1" s="37"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -22190,12 +22590,12 @@
       <c r="O4" s="23"/>
       <c r="P4" s="23"/>
       <c r="Q4" s="29"/>
-      <c r="R4" s="414" t="s">
+      <c r="R4" s="417" t="s">
         <v>234</v>
       </c>
-      <c r="S4" s="415"/>
-      <c r="T4" s="415"/>
-      <c r="U4" s="416"/>
+      <c r="S4" s="426"/>
+      <c r="T4" s="426"/>
+      <c r="U4" s="427"/>
     </row>
     <row r="5" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="174" t="s">
@@ -22218,12 +22618,12 @@
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
       <c r="Q5" s="29"/>
-      <c r="R5" s="417" t="s">
+      <c r="R5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="S5" s="418"/>
-      <c r="T5" s="418"/>
-      <c r="U5" s="419"/>
+      <c r="S5" s="429"/>
+      <c r="T5" s="429"/>
+      <c r="U5" s="430"/>
     </row>
     <row r="6" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="174" t="s">
@@ -23893,11 +24293,11 @@
       <c r="K93" s="172"/>
       <c r="L93" s="182"/>
       <c r="M93" s="182"/>
-      <c r="R93" s="424" t="s">
+      <c r="R93" s="423" t="s">
         <v>211</v>
       </c>
-      <c r="S93" s="425"/>
-      <c r="T93" s="425"/>
+      <c r="S93" s="424"/>
+      <c r="T93" s="424"/>
       <c r="U93" s="37"/>
     </row>
     <row r="94" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -23986,12 +24386,12 @@
       <c r="K96" s="61"/>
       <c r="L96" s="61"/>
       <c r="M96" s="62"/>
-      <c r="R96" s="414" t="s">
+      <c r="R96" s="417" t="s">
         <v>50</v>
       </c>
-      <c r="S96" s="426"/>
-      <c r="T96" s="426"/>
-      <c r="U96" s="427"/>
+      <c r="S96" s="418"/>
+      <c r="T96" s="418"/>
+      <c r="U96" s="419"/>
     </row>
     <row r="97" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="174" t="s">
@@ -24013,12 +24413,12 @@
       <c r="K97" s="61"/>
       <c r="L97" s="61"/>
       <c r="M97" s="62"/>
-      <c r="R97" s="424" t="s">
+      <c r="R97" s="423" t="s">
         <v>754</v>
       </c>
-      <c r="S97" s="425"/>
-      <c r="T97" s="425"/>
-      <c r="U97" s="428"/>
+      <c r="S97" s="424"/>
+      <c r="T97" s="424"/>
+      <c r="U97" s="425"/>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A98" s="174" t="s">
@@ -24070,11 +24470,11 @@
       <c r="K100" s="61"/>
       <c r="L100" s="61"/>
       <c r="M100" s="62"/>
-      <c r="R100" s="424" t="s">
+      <c r="R100" s="423" t="s">
         <v>755</v>
       </c>
-      <c r="S100" s="425"/>
-      <c r="T100" s="425"/>
+      <c r="S100" s="424"/>
+      <c r="T100" s="424"/>
       <c r="U100" s="37"/>
     </row>
     <row r="101" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -24170,12 +24570,12 @@
       <c r="M103" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="R103" s="414" t="s">
+      <c r="R103" s="417" t="s">
         <v>234</v>
       </c>
-      <c r="S103" s="426"/>
-      <c r="T103" s="426"/>
-      <c r="U103" s="427"/>
+      <c r="S103" s="418"/>
+      <c r="T103" s="418"/>
+      <c r="U103" s="419"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A104" s="174" t="s">
@@ -24192,12 +24592,12 @@
       <c r="L104" s="29" t="s">
         <v>407</v>
       </c>
-      <c r="R104" s="424" t="s">
+      <c r="R104" s="423" t="s">
         <v>754</v>
       </c>
-      <c r="S104" s="425"/>
-      <c r="T104" s="425"/>
-      <c r="U104" s="428"/>
+      <c r="S104" s="424"/>
+      <c r="T104" s="424"/>
+      <c r="U104" s="425"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A105" s="174" t="s">
@@ -24547,12 +24947,12 @@
       <c r="L124" s="29" t="s">
         <v>659</v>
       </c>
-      <c r="R124" s="424" t="s">
+      <c r="R124" s="423" t="s">
         <v>766</v>
       </c>
-      <c r="S124" s="425"/>
-      <c r="T124" s="425"/>
-      <c r="U124" s="428"/>
+      <c r="S124" s="424"/>
+      <c r="T124" s="424"/>
+      <c r="U124" s="425"/>
     </row>
     <row r="125" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="174" t="s">
@@ -24628,12 +25028,12 @@
       <c r="G127" s="55" t="s">
         <v>491</v>
       </c>
-      <c r="R127" s="414" t="s">
+      <c r="R127" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="S127" s="426"/>
-      <c r="T127" s="426"/>
-      <c r="U127" s="427"/>
+      <c r="S127" s="418"/>
+      <c r="T127" s="418"/>
+      <c r="U127" s="419"/>
     </row>
     <row r="128" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="174" t="s">
@@ -24699,12 +25099,12 @@
       <c r="F135" s="60" t="s">
         <v>735</v>
       </c>
-      <c r="R135" s="424" t="s">
+      <c r="R135" s="423" t="s">
         <v>786</v>
       </c>
-      <c r="S135" s="425"/>
-      <c r="T135" s="425"/>
-      <c r="U135" s="428"/>
+      <c r="S135" s="424"/>
+      <c r="T135" s="424"/>
+      <c r="U135" s="425"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A136" s="174" t="s">
@@ -24756,12 +25156,12 @@
       <c r="A138" s="174" t="s">
         <v>743</v>
       </c>
-      <c r="R138" s="414" t="s">
+      <c r="R138" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="S138" s="426"/>
-      <c r="T138" s="426"/>
-      <c r="U138" s="427"/>
+      <c r="S138" s="418"/>
+      <c r="T138" s="418"/>
+      <c r="U138" s="419"/>
     </row>
     <row r="139" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="174" t="s">
@@ -24821,12 +25221,12 @@
       <c r="F145" s="56" t="s">
         <v>728</v>
       </c>
-      <c r="R145" s="424" t="s">
+      <c r="R145" s="423" t="s">
         <v>796</v>
       </c>
-      <c r="S145" s="425"/>
-      <c r="T145" s="425"/>
-      <c r="U145" s="428"/>
+      <c r="S145" s="424"/>
+      <c r="T145" s="424"/>
+      <c r="U145" s="425"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A146" s="174" t="s">
@@ -24878,12 +25278,12 @@
       <c r="A148" s="174" t="s">
         <v>768</v>
       </c>
-      <c r="R148" s="414" t="s">
+      <c r="R148" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="S148" s="426"/>
-      <c r="T148" s="426"/>
-      <c r="U148" s="427"/>
+      <c r="S148" s="418"/>
+      <c r="T148" s="418"/>
+      <c r="U148" s="419"/>
     </row>
     <row r="149" spans="1:21" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="174" t="s">
@@ -25007,21 +25407,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R138:U138"/>
-    <mergeCell ref="R139:U139"/>
-    <mergeCell ref="R148:U148"/>
-    <mergeCell ref="R149:U149"/>
-    <mergeCell ref="R135:U135"/>
-    <mergeCell ref="R145:U145"/>
-    <mergeCell ref="R128:U128"/>
-    <mergeCell ref="R93:T93"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="R97:U97"/>
-    <mergeCell ref="R100:T100"/>
-    <mergeCell ref="R103:U103"/>
-    <mergeCell ref="R104:U104"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="R127:U127"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="B1:E1"/>
@@ -25032,6 +25417,21 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="R128:U128"/>
+    <mergeCell ref="R93:T93"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="R97:U97"/>
+    <mergeCell ref="R100:T100"/>
+    <mergeCell ref="R103:U103"/>
+    <mergeCell ref="R104:U104"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="R127:U127"/>
+    <mergeCell ref="R138:U138"/>
+    <mergeCell ref="R139:U139"/>
+    <mergeCell ref="R148:U148"/>
+    <mergeCell ref="R149:U149"/>
+    <mergeCell ref="R135:U135"/>
+    <mergeCell ref="R145:U145"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25068,7 +25468,7 @@
       <c r="C1" s="421"/>
       <c r="D1" s="421"/>
       <c r="E1" s="422"/>
-      <c r="F1" s="423" t="s">
+      <c r="F1" s="431" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="421"/>
@@ -25172,12 +25572,12 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="36"/>
-      <c r="R3" s="424" t="s">
+      <c r="R3" s="423" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="425"/>
-      <c r="T3" s="425"/>
-      <c r="U3" s="428"/>
+      <c r="S3" s="424"/>
+      <c r="T3" s="424"/>
+      <c r="U3" s="425"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="34" t="s">
@@ -25230,12 +25630,12 @@
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
       <c r="Q5" s="29"/>
-      <c r="R5" s="417" t="s">
+      <c r="R5" s="428" t="s">
         <v>50</v>
       </c>
-      <c r="S5" s="418"/>
-      <c r="T5" s="418"/>
-      <c r="U5" s="419"/>
+      <c r="S5" s="429"/>
+      <c r="T5" s="429"/>
+      <c r="U5" s="430"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="34" t="s">
@@ -25257,12 +25657,12 @@
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
       <c r="Q6" s="29"/>
-      <c r="R6" s="417" t="s">
+      <c r="R6" s="428" t="s">
         <v>214</v>
       </c>
-      <c r="S6" s="418"/>
-      <c r="T6" s="418"/>
-      <c r="U6" s="419"/>
+      <c r="S6" s="429"/>
+      <c r="T6" s="429"/>
+      <c r="U6" s="430"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="34" t="s">
@@ -26501,18 +26901,18 @@
       <c r="AB1" s="234"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="B2" s="413" t="s">
+      <c r="B2" s="416" t="s">
         <v>583</v>
       </c>
-      <c r="C2" s="413"/>
-      <c r="D2" s="413"/>
-      <c r="E2" s="413"/>
-      <c r="F2" s="413"/>
-      <c r="G2" s="413"/>
-      <c r="H2" s="413"/>
-      <c r="I2" s="413"/>
-      <c r="J2" s="413"/>
-      <c r="K2" s="413"/>
+      <c r="C2" s="416"/>
+      <c r="D2" s="416"/>
+      <c r="E2" s="416"/>
+      <c r="F2" s="416"/>
+      <c r="G2" s="416"/>
+      <c r="H2" s="416"/>
+      <c r="I2" s="416"/>
+      <c r="J2" s="416"/>
+      <c r="K2" s="416"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B3" s="18" t="s">
@@ -26895,15 +27295,15 @@
       <c r="O18" s="18">
         <v>1</v>
       </c>
-      <c r="V18" s="413" t="s">
+      <c r="V18" s="416" t="s">
         <v>933</v>
       </c>
-      <c r="W18" s="413"/>
-      <c r="X18" s="413"/>
-      <c r="Y18" s="413"/>
-      <c r="Z18" s="413"/>
-      <c r="AA18" s="413"/>
-      <c r="AB18" s="413"/>
+      <c r="W18" s="416"/>
+      <c r="X18" s="416"/>
+      <c r="Y18" s="416"/>
+      <c r="Z18" s="416"/>
+      <c r="AA18" s="416"/>
+      <c r="AB18" s="416"/>
       <c r="AC18" s="156"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.4">
@@ -28912,18 +29312,18 @@
       <c r="A89" s="243" t="s">
         <v>893</v>
       </c>
-      <c r="B89" s="424" t="s">
+      <c r="B89" s="423" t="s">
         <v>894</v>
       </c>
-      <c r="C89" s="425"/>
-      <c r="D89" s="425"/>
-      <c r="E89" s="428"/>
-      <c r="G89" s="429" t="s">
+      <c r="C89" s="424"/>
+      <c r="D89" s="424"/>
+      <c r="E89" s="425"/>
+      <c r="G89" s="432" t="s">
         <v>895</v>
       </c>
-      <c r="H89" s="430"/>
-      <c r="I89" s="430"/>
-      <c r="J89" s="431"/>
+      <c r="H89" s="433"/>
+      <c r="I89" s="433"/>
+      <c r="J89" s="434"/>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B90" s="28" t="s">
@@ -31577,7 +31977,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D57" sqref="D57:D59"/>
+      <selection pane="topRight" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -31623,11 +32023,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D1" s="424" t="s">
+      <c r="D1" s="423" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="425"/>
-      <c r="F1" s="425"/>
+      <c r="E1" s="424"/>
+      <c r="F1" s="424"/>
       <c r="G1" s="37"/>
       <c r="H1" s="45"/>
       <c r="I1" s="65"/>
@@ -31669,12 +32069,12 @@
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.4">
-      <c r="D3" s="417" t="s">
+      <c r="D3" s="428" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="418"/>
-      <c r="F3" s="418"/>
-      <c r="G3" s="419"/>
+      <c r="E3" s="429"/>
+      <c r="F3" s="429"/>
+      <c r="G3" s="430"/>
       <c r="H3" s="81"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
@@ -31795,11 +32195,11 @@
       <c r="J8" s="67"/>
       <c r="K8" s="67"/>
       <c r="L8" s="67"/>
-      <c r="M8" s="432" t="s">
+      <c r="M8" s="436" t="s">
         <v>457</v>
       </c>
-      <c r="N8" s="432"/>
-      <c r="O8" s="432"/>
+      <c r="N8" s="436"/>
+      <c r="O8" s="436"/>
       <c r="T8" s="112"/>
       <c r="U8" s="114"/>
       <c r="V8" s="112"/>
@@ -31816,12 +32216,12 @@
       <c r="AL8" s="113"/>
       <c r="AM8" s="113"/>
       <c r="AN8" s="113"/>
-      <c r="AQ8" s="417" t="s">
+      <c r="AQ8" s="428" t="s">
         <v>16</v>
       </c>
-      <c r="AR8" s="418"/>
-      <c r="AS8" s="418"/>
-      <c r="AT8" s="419"/>
+      <c r="AR8" s="429"/>
+      <c r="AS8" s="429"/>
+      <c r="AT8" s="430"/>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D9" s="238"/>
@@ -31833,11 +32233,11 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
-      <c r="M9" s="434" t="s">
+      <c r="M9" s="438" t="s">
         <v>458</v>
       </c>
-      <c r="N9" s="434"/>
-      <c r="O9" s="433"/>
+      <c r="N9" s="438"/>
+      <c r="O9" s="437"/>
       <c r="T9" s="112"/>
       <c r="U9" s="114"/>
       <c r="V9" s="112"/>
@@ -31898,12 +32298,12 @@
       <c r="AL10" s="113"/>
       <c r="AM10" s="113"/>
       <c r="AN10" s="113"/>
-      <c r="AQ10" s="417" t="s">
+      <c r="AQ10" s="428" t="s">
         <v>50</v>
       </c>
-      <c r="AR10" s="418"/>
-      <c r="AS10" s="418"/>
-      <c r="AT10" s="419"/>
+      <c r="AR10" s="429"/>
+      <c r="AS10" s="429"/>
+      <c r="AT10" s="430"/>
     </row>
     <row r="11" spans="1:49" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="238"/>
@@ -31935,12 +32335,12 @@
       <c r="AL11" s="113"/>
       <c r="AM11" s="113"/>
       <c r="AN11" s="113"/>
-      <c r="AQ11" s="417" t="s">
+      <c r="AQ11" s="428" t="s">
         <v>530</v>
       </c>
-      <c r="AR11" s="418"/>
-      <c r="AS11" s="418"/>
-      <c r="AT11" s="419"/>
+      <c r="AR11" s="429"/>
+      <c r="AS11" s="429"/>
+      <c r="AT11" s="430"/>
       <c r="AU11" s="23" t="s">
         <v>215</v>
       </c>
@@ -31966,11 +32366,11 @@
       <c r="J12" s="67"/>
       <c r="K12" s="67"/>
       <c r="L12" s="67"/>
-      <c r="M12" s="436" t="s">
+      <c r="M12" s="439" t="s">
         <v>456</v>
       </c>
-      <c r="N12" s="436"/>
-      <c r="O12" s="436"/>
+      <c r="N12" s="439"/>
+      <c r="O12" s="439"/>
       <c r="AF12" s="85"/>
       <c r="AG12" s="86"/>
       <c r="AH12" s="86"/>
@@ -31980,12 +32380,12 @@
       <c r="AL12" s="113"/>
       <c r="AM12" s="113"/>
       <c r="AN12" s="113"/>
-      <c r="AQ12" s="417" t="s">
+      <c r="AQ12" s="428" t="s">
         <v>455</v>
       </c>
-      <c r="AR12" s="418"/>
-      <c r="AS12" s="418"/>
-      <c r="AT12" s="419"/>
+      <c r="AR12" s="429"/>
+      <c r="AS12" s="429"/>
+      <c r="AT12" s="430"/>
       <c r="AV12" s="18" t="s">
         <v>526</v>
       </c>
@@ -32069,18 +32469,18 @@
       <c r="AH13" s="45"/>
       <c r="AI13" s="38"/>
       <c r="AJ13" s="112"/>
-      <c r="AK13" s="417" t="s">
+      <c r="AK13" s="428" t="s">
         <v>459</v>
       </c>
-      <c r="AL13" s="418"/>
-      <c r="AM13" s="418"/>
-      <c r="AN13" s="418"/>
-      <c r="AQ13" s="417" t="s">
+      <c r="AL13" s="429"/>
+      <c r="AM13" s="429"/>
+      <c r="AN13" s="429"/>
+      <c r="AQ13" s="428" t="s">
         <v>523</v>
       </c>
-      <c r="AR13" s="413"/>
-      <c r="AS13" s="413"/>
-      <c r="AT13" s="413"/>
+      <c r="AR13" s="416"/>
+      <c r="AS13" s="416"/>
+      <c r="AT13" s="416"/>
       <c r="AV13" s="18" t="s">
         <v>527</v>
       </c>
@@ -32767,8 +33167,8 @@
       </c>
       <c r="AO30" s="117"/>
       <c r="AP30" s="119"/>
-      <c r="AR30" s="433"/>
-      <c r="AS30" s="433"/>
+      <c r="AR30" s="437"/>
+      <c r="AS30" s="437"/>
     </row>
     <row r="31" spans="1:52" s="23" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="153" t="s">
@@ -34869,13 +35269,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="AR46:AS46"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="AR40:AS40"/>
-    <mergeCell ref="AQ11:AT11"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="D6:G6"/>
@@ -34892,6 +35285,13 @@
     <mergeCell ref="AK13:AN13"/>
     <mergeCell ref="AQ10:AT10"/>
     <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="AR46:AS46"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="AR40:AS40"/>
+    <mergeCell ref="AQ11:AT11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34949,17 +35349,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.4">
-      <c r="B1" s="424" t="s">
+      <c r="B1" s="423" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="425"/>
-      <c r="D1" s="425"/>
+      <c r="C1" s="424"/>
+      <c r="D1" s="424"/>
       <c r="E1" s="37"/>
-      <c r="F1" s="424" t="s">
+      <c r="F1" s="423" t="s">
         <v>831</v>
       </c>
-      <c r="G1" s="425"/>
-      <c r="H1" s="425"/>
+      <c r="G1" s="424"/>
+      <c r="H1" s="424"/>
       <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.4">
@@ -35002,32 +35402,32 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="414" t="s">
+      <c r="B4" s="417" t="s">
         <v>830</v>
       </c>
-      <c r="C4" s="415"/>
-      <c r="D4" s="415"/>
-      <c r="E4" s="416"/>
-      <c r="F4" s="414" t="s">
+      <c r="C4" s="426"/>
+      <c r="D4" s="426"/>
+      <c r="E4" s="427"/>
+      <c r="F4" s="417" t="s">
         <v>234</v>
       </c>
-      <c r="G4" s="415"/>
-      <c r="H4" s="415"/>
-      <c r="I4" s="416"/>
+      <c r="G4" s="426"/>
+      <c r="H4" s="426"/>
+      <c r="I4" s="427"/>
     </row>
     <row r="5" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="417" t="s">
+      <c r="B5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="C5" s="418"/>
-      <c r="D5" s="418"/>
-      <c r="E5" s="419"/>
-      <c r="F5" s="417" t="s">
+      <c r="C5" s="429"/>
+      <c r="D5" s="429"/>
+      <c r="E5" s="430"/>
+      <c r="F5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="G5" s="418"/>
-      <c r="H5" s="418"/>
-      <c r="I5" s="419"/>
+      <c r="G5" s="429"/>
+      <c r="H5" s="429"/>
+      <c r="I5" s="430"/>
     </row>
     <row r="6" spans="1:46" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="160" t="s">
@@ -35039,7 +35439,7 @@
       <c r="C6" s="421"/>
       <c r="D6" s="421"/>
       <c r="E6" s="422"/>
-      <c r="F6" s="423" t="s">
+      <c r="F6" s="431" t="s">
         <v>105</v>
       </c>
       <c r="G6" s="421"/>
@@ -38794,11 +39194,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B4:E4"/>
@@ -38807,6 +39202,11 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38869,31 +39269,31 @@
       <c r="B1" s="212"/>
       <c r="C1" s="212"/>
       <c r="D1" s="299"/>
-      <c r="E1" s="424" t="s">
+      <c r="E1" s="423" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="425"/>
-      <c r="G1" s="425"/>
+      <c r="F1" s="424"/>
+      <c r="G1" s="424"/>
       <c r="H1" s="37"/>
       <c r="I1" s="92"/>
-      <c r="J1" s="424" t="s">
+      <c r="J1" s="423" t="s">
         <v>831</v>
       </c>
-      <c r="K1" s="425"/>
-      <c r="L1" s="425"/>
+      <c r="K1" s="424"/>
+      <c r="L1" s="424"/>
       <c r="M1" s="47"/>
       <c r="N1" s="271"/>
-      <c r="O1" s="424" t="s">
+      <c r="O1" s="423" t="s">
         <v>881</v>
       </c>
-      <c r="P1" s="425"/>
-      <c r="Q1" s="425"/>
+      <c r="P1" s="424"/>
+      <c r="Q1" s="424"/>
       <c r="R1" s="37"/>
-      <c r="S1" s="424" t="s">
+      <c r="S1" s="423" t="s">
         <v>884</v>
       </c>
-      <c r="T1" s="425"/>
-      <c r="U1" s="425"/>
+      <c r="T1" s="424"/>
+      <c r="U1" s="424"/>
       <c r="V1" s="47"/>
       <c r="W1" s="269"/>
       <c r="X1" s="232"/>
@@ -38902,11 +39302,11 @@
       <c r="AA1" s="263"/>
       <c r="AB1" s="263"/>
       <c r="AC1" s="263"/>
-      <c r="AD1" s="424" t="s">
+      <c r="AD1" s="423" t="s">
         <v>885</v>
       </c>
-      <c r="AE1" s="425"/>
-      <c r="AF1" s="425"/>
+      <c r="AE1" s="424"/>
+      <c r="AF1" s="424"/>
       <c r="AG1" s="37"/>
       <c r="AH1" s="321"/>
       <c r="AI1" s="42"/>
@@ -39010,72 +39410,72 @@
       </c>
     </row>
     <row r="4" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E4" s="414" t="s">
+      <c r="E4" s="417" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="415"/>
-      <c r="G4" s="415"/>
-      <c r="H4" s="416"/>
+      <c r="F4" s="426"/>
+      <c r="G4" s="426"/>
+      <c r="H4" s="427"/>
       <c r="I4" s="67"/>
-      <c r="J4" s="414" t="s">
+      <c r="J4" s="417" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="415"/>
-      <c r="L4" s="415"/>
-      <c r="M4" s="416"/>
+      <c r="K4" s="426"/>
+      <c r="L4" s="426"/>
+      <c r="M4" s="427"/>
       <c r="N4" s="199"/>
-      <c r="O4" s="414" t="s">
+      <c r="O4" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="P4" s="415"/>
-      <c r="Q4" s="415"/>
-      <c r="R4" s="416"/>
-      <c r="S4" s="414" t="s">
+      <c r="P4" s="426"/>
+      <c r="Q4" s="426"/>
+      <c r="R4" s="427"/>
+      <c r="S4" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="T4" s="415"/>
-      <c r="U4" s="415"/>
-      <c r="V4" s="416"/>
-      <c r="AD4" s="414" t="s">
+      <c r="T4" s="426"/>
+      <c r="U4" s="426"/>
+      <c r="V4" s="427"/>
+      <c r="AD4" s="417" t="s">
         <v>758</v>
       </c>
-      <c r="AE4" s="415"/>
-      <c r="AF4" s="415"/>
-      <c r="AG4" s="416"/>
+      <c r="AE4" s="426"/>
+      <c r="AF4" s="426"/>
+      <c r="AG4" s="427"/>
     </row>
     <row r="5" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E5" s="417" t="s">
+      <c r="E5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="F5" s="418"/>
-      <c r="G5" s="418"/>
-      <c r="H5" s="419"/>
+      <c r="F5" s="429"/>
+      <c r="G5" s="429"/>
+      <c r="H5" s="430"/>
       <c r="I5" s="264"/>
-      <c r="J5" s="417" t="s">
+      <c r="J5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="K5" s="418"/>
-      <c r="L5" s="418"/>
-      <c r="M5" s="419"/>
+      <c r="K5" s="429"/>
+      <c r="L5" s="429"/>
+      <c r="M5" s="430"/>
       <c r="N5" s="68"/>
-      <c r="O5" s="417" t="s">
+      <c r="O5" s="428" t="s">
         <v>754</v>
       </c>
-      <c r="P5" s="418"/>
-      <c r="Q5" s="418"/>
-      <c r="R5" s="419"/>
-      <c r="S5" s="417" t="s">
+      <c r="P5" s="429"/>
+      <c r="Q5" s="429"/>
+      <c r="R5" s="430"/>
+      <c r="S5" s="428" t="s">
         <v>797</v>
       </c>
-      <c r="T5" s="418"/>
-      <c r="U5" s="418"/>
-      <c r="V5" s="419"/>
-      <c r="AD5" s="417" t="s">
+      <c r="T5" s="429"/>
+      <c r="U5" s="429"/>
+      <c r="V5" s="430"/>
+      <c r="AD5" s="428" t="s">
         <v>797</v>
       </c>
-      <c r="AE5" s="418"/>
-      <c r="AF5" s="418"/>
-      <c r="AG5" s="419"/>
+      <c r="AE5" s="429"/>
+      <c r="AF5" s="429"/>
+      <c r="AG5" s="430"/>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="160" t="s">
@@ -39096,7 +39496,7 @@
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
       <c r="N6" s="274"/>
-      <c r="O6" s="423" t="s">
+      <c r="O6" s="431" t="s">
         <v>105</v>
       </c>
       <c r="P6" s="421"/>
@@ -39170,12 +39570,12 @@
       <c r="T7" s="421"/>
       <c r="U7" s="421"/>
       <c r="V7" s="422"/>
-      <c r="W7" s="439" t="s">
+      <c r="W7" s="442" t="s">
         <v>926</v>
       </c>
-      <c r="X7" s="440"/>
-      <c r="Y7" s="440"/>
-      <c r="Z7" s="441"/>
+      <c r="X7" s="443"/>
+      <c r="Y7" s="443"/>
+      <c r="Z7" s="444"/>
       <c r="AA7" s="106"/>
       <c r="AB7" s="106"/>
       <c r="AC7" s="106"/>
@@ -39545,12 +39945,12 @@
       <c r="I14" s="61" t="s">
         <v>935</v>
       </c>
-      <c r="J14" s="437" t="s">
+      <c r="J14" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K14" s="438"/>
-      <c r="L14" s="438"/>
-      <c r="M14" s="438"/>
+      <c r="K14" s="441"/>
+      <c r="L14" s="441"/>
+      <c r="M14" s="441"/>
       <c r="N14" s="122"/>
       <c r="O14" s="58" t="s">
         <v>1143</v>
@@ -39560,12 +39960,12 @@
       </c>
       <c r="Q14" s="23"/>
       <c r="R14" s="18"/>
-      <c r="S14" s="437" t="s">
+      <c r="S14" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="T14" s="438"/>
-      <c r="U14" s="438"/>
-      <c r="V14" s="438"/>
+      <c r="T14" s="441"/>
+      <c r="U14" s="441"/>
+      <c r="V14" s="441"/>
       <c r="AD14" s="133"/>
       <c r="AE14" s="61"/>
       <c r="AF14" s="9"/>
@@ -39892,12 +40292,12 @@
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="61"/>
-      <c r="J22" s="437" t="s">
+      <c r="J22" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K22" s="438"/>
-      <c r="L22" s="438"/>
-      <c r="M22" s="438"/>
+      <c r="K22" s="441"/>
+      <c r="L22" s="441"/>
+      <c r="M22" s="441"/>
       <c r="N22" s="122"/>
       <c r="P22" s="58" t="s">
         <v>195</v>
@@ -39908,12 +40308,12 @@
       <c r="R22" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="S22" s="437" t="s">
+      <c r="S22" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="T22" s="438"/>
-      <c r="U22" s="438"/>
-      <c r="V22" s="438"/>
+      <c r="T22" s="441"/>
+      <c r="U22" s="441"/>
+      <c r="V22" s="441"/>
       <c r="Y22" s="29"/>
       <c r="Z22" s="29" t="s">
         <v>407</v>
@@ -40219,12 +40619,12 @@
         <v>490</v>
       </c>
       <c r="I30" s="61"/>
-      <c r="J30" s="437" t="s">
+      <c r="J30" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K30" s="438"/>
-      <c r="L30" s="438"/>
-      <c r="M30" s="438"/>
+      <c r="K30" s="441"/>
+      <c r="L30" s="441"/>
+      <c r="M30" s="441"/>
       <c r="N30" s="277"/>
       <c r="P30" s="58" t="s">
         <v>209</v>
@@ -40235,12 +40635,12 @@
       <c r="R30" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="S30" s="437" t="s">
+      <c r="S30" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="T30" s="438"/>
-      <c r="U30" s="438"/>
-      <c r="V30" s="438"/>
+      <c r="T30" s="441"/>
+      <c r="U30" s="441"/>
+      <c r="V30" s="441"/>
       <c r="Y30" s="29"/>
       <c r="Z30" s="29" t="s">
         <v>646</v>
@@ -40528,12 +40928,12 @@
         <v>490</v>
       </c>
       <c r="I38" s="61"/>
-      <c r="J38" s="437" t="s">
+      <c r="J38" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K38" s="438"/>
-      <c r="L38" s="438"/>
-      <c r="M38" s="438"/>
+      <c r="K38" s="441"/>
+      <c r="L38" s="441"/>
+      <c r="M38" s="441"/>
       <c r="N38" s="277"/>
       <c r="O38" s="9"/>
       <c r="P38" s="58" t="s">
@@ -40541,12 +40941,12 @@
       </c>
       <c r="Q38" s="61"/>
       <c r="R38" s="61"/>
-      <c r="S38" s="437" t="s">
+      <c r="S38" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="T38" s="438"/>
-      <c r="U38" s="438"/>
-      <c r="V38" s="438"/>
+      <c r="T38" s="441"/>
+      <c r="U38" s="441"/>
+      <c r="V38" s="441"/>
       <c r="Y38" s="29"/>
       <c r="Z38" s="29" t="s">
         <v>650</v>
@@ -40798,12 +41198,12 @@
       </c>
       <c r="H46" s="62"/>
       <c r="I46" s="61"/>
-      <c r="J46" s="437" t="s">
+      <c r="J46" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K46" s="438"/>
-      <c r="L46" s="438"/>
-      <c r="M46" s="438"/>
+      <c r="K46" s="441"/>
+      <c r="L46" s="441"/>
+      <c r="M46" s="441"/>
       <c r="O46" s="61"/>
       <c r="P46" s="53" t="s">
         <v>490</v>
@@ -41000,12 +41400,12 @@
       <c r="B58" s="215" t="s">
         <v>834</v>
       </c>
-      <c r="J58" s="437" t="s">
+      <c r="J58" s="440" t="s">
         <v>880</v>
       </c>
-      <c r="K58" s="438"/>
-      <c r="L58" s="438"/>
-      <c r="M58" s="438"/>
+      <c r="K58" s="441"/>
+      <c r="L58" s="441"/>
+      <c r="M58" s="441"/>
       <c r="AF58" s="56" t="s">
         <v>790</v>
       </c>
@@ -41409,30 +41809,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="AQ7:AT7"/>
-    <mergeCell ref="AM6:AP6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="AD7:AG7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="S7:V7"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD1:AF1"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AD5:AG5"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W7:Z7"/>
     <mergeCell ref="J58:M58"/>
     <mergeCell ref="J46:M46"/>
     <mergeCell ref="S1:U1"/>
@@ -41445,6 +41821,30 @@
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="J30:M30"/>
     <mergeCell ref="J38:M38"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="W7:Z7"/>
+    <mergeCell ref="AQ7:AT7"/>
+    <mergeCell ref="AM6:AP6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="AD7:AG7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41457,7 +41857,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D32" sqref="D32"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -41484,30 +41884,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E1" s="442" t="s">
+      <c r="E1" s="445" t="s">
         <v>1083</v>
       </c>
-      <c r="F1" s="443"/>
-      <c r="G1" s="443"/>
-      <c r="H1" s="444"/>
-      <c r="I1" s="442" t="s">
+      <c r="F1" s="446"/>
+      <c r="G1" s="446"/>
+      <c r="H1" s="447"/>
+      <c r="I1" s="445" t="s">
         <v>1084</v>
       </c>
-      <c r="J1" s="443"/>
-      <c r="K1" s="443"/>
-      <c r="L1" s="444"/>
-      <c r="N1" s="442" t="s">
+      <c r="J1" s="446"/>
+      <c r="K1" s="446"/>
+      <c r="L1" s="447"/>
+      <c r="N1" s="445" t="s">
         <v>1085</v>
       </c>
-      <c r="O1" s="443"/>
-      <c r="P1" s="443"/>
-      <c r="Q1" s="444"/>
-      <c r="U1" s="442" t="s">
+      <c r="O1" s="446"/>
+      <c r="P1" s="446"/>
+      <c r="Q1" s="447"/>
+      <c r="U1" s="445" t="s">
         <v>1087</v>
       </c>
-      <c r="V1" s="443"/>
-      <c r="W1" s="443"/>
-      <c r="X1" s="444"/>
+      <c r="V1" s="446"/>
+      <c r="W1" s="446"/>
+      <c r="X1" s="447"/>
     </row>
     <row r="2" spans="1:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="344" t="s">
@@ -41596,10 +41996,10 @@
       <c r="F3" s="47"/>
       <c r="G3" s="47"/>
       <c r="H3" s="37"/>
-      <c r="I3" s="424"/>
-      <c r="J3" s="425"/>
-      <c r="K3" s="425"/>
-      <c r="L3" s="428"/>
+      <c r="I3" s="423"/>
+      <c r="J3" s="424"/>
+      <c r="K3" s="424"/>
+      <c r="L3" s="425"/>
       <c r="M3" s="354"/>
       <c r="N3" s="347"/>
       <c r="R3" s="154" t="s">

</xml_diff>